<commit_message>
Changed the master for motre links and less constants
</commit_message>
<xml_diff>
--- a/data/MetaMaster.xlsx
+++ b/data/MetaMaster.xlsx
@@ -21,7 +21,7 @@
     <definedName name="Column">Lists!$P$2:$P$258</definedName>
     <definedName name="DerivationFactor">Lists!$K$2:$K$6</definedName>
     <definedName name="Designation">Lists!$B$2:$B$6</definedName>
-    <definedName name="Factor">Lists!$J$2:$J$47</definedName>
+    <definedName name="Factor">Lists!$J$2:$J$52</definedName>
     <definedName name="FeildsThatNeedUnit" localSheetId="2">[1]Lists!$P$2:$P$4</definedName>
     <definedName name="FeildsThatNeedUnit">Lists!$O$2:$O$4</definedName>
     <definedName name="Location">Lists!$C$2:$C$14</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="445">
   <si>
     <t>Easting</t>
   </si>
@@ -500,12 +500,6 @@
     <t>Location for Site</t>
   </si>
   <si>
-    <t xml:space="preserve">The column that contains the ID of the Location for this Site. Enter "row" if the Location has no ID column. Only applicable for columns with a "Site" category. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The column that contains the ID of the Survey for this Item. Enter "row" if the Survey has no ID column. Only applicable for columns with a "Site" category. </t>
-  </si>
-  <si>
     <t>Factor for Observation's Value</t>
   </si>
   <si>
@@ -533,9 +527,6 @@
     <t>Sorry only an amdinistrator can add a new Category</t>
   </si>
   <si>
-    <t>WANRING</t>
-  </si>
-  <si>
     <t>Unexpected Feild Value</t>
   </si>
   <si>
@@ -551,15 +542,9 @@
     <t>Not a direct value</t>
   </si>
   <si>
-    <t>You entered a vlaue which is not a local value. Andvance use only.</t>
-  </si>
-  <si>
     <t>Unexpected Factor</t>
   </si>
   <si>
-    <t>Entered value not found in list of expected Factors. Only use values not in the list if you are absolutely sure none of the values in the list are applicable.</t>
-  </si>
-  <si>
     <t>Unexpected Unit.</t>
   </si>
   <si>
@@ -1277,9 +1262,6 @@
     <t>INDIRECT(IF(OR(A$2="Value"),"Column","NotApplicable"))</t>
   </si>
   <si>
-    <t>INDIRECT(IF(OR(A$2="Site"),"Column","NotApplicable"))</t>
-  </si>
-  <si>
     <t>INDIRECT(IF(A$2="Value","Factor","NotApplicable"))</t>
   </si>
   <si>
@@ -1310,9 +1292,6 @@
     <t>SimilarTo</t>
   </si>
   <si>
-    <t>INDIRECT(IF(OR(A$2="Observation"),"Column","NotApplicable"))</t>
-  </si>
-  <si>
     <t>Header</t>
   </si>
   <si>
@@ -1347,13 +1326,64 @@
   </si>
   <si>
     <t>Lifeform</t>
+  </si>
+  <si>
+    <t>INDIRECT(IF(OR(A$2="Value",A$2="Id"),"Column","NotApplicable"))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The column that contains the ID of the Location for this Site. Enter "row" if the Location has no ID column. Start Constants with =. Only applicable for columns with a "Site" category. </t>
+  </si>
+  <si>
+    <t>INDIRECT(IF(A$1="Site","Column","NotApplicable"))</t>
+  </si>
+  <si>
+    <t>INDIRECT(IF(A$2="Value","Column","NotApplicable"))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The column that contains the ID of the Survey for this Item. Enter "row" if the Survey has no ID column. Start constants with an =. Only applicable for columns with a "Value" field. </t>
+  </si>
+  <si>
+    <t>You entered a vlaue which is not a lookup value. Constants must start with an = symbol. Any other value will cause an error.</t>
+  </si>
+  <si>
+    <t>Entered value not found in list of expected Factors. Any other value will need to be added to the global accepted list.</t>
+  </si>
+  <si>
+    <t>WARNING</t>
+  </si>
+  <si>
+    <t>PHYTOPL</t>
+  </si>
+  <si>
+    <t>FISH</t>
+  </si>
+  <si>
+    <t>SANDSTONE</t>
+  </si>
+  <si>
+    <t>CARBONIF</t>
+  </si>
+  <si>
+    <t>SILURIAN</t>
+  </si>
+  <si>
+    <t>CONISTON_L</t>
+  </si>
+  <si>
+    <t>GRANITE</t>
+  </si>
+  <si>
+    <t>BORROWDALE</t>
+  </si>
+  <si>
+    <t>SKIDDAW_S</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="9"/>
       <name val="Geneva"/>
@@ -1366,6 +1396,14 @@
     <font>
       <sz val="8"/>
       <name val="Geneva"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Geneva"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1385,10 +1423,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1396,9 +1436,13 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1811,13 +1855,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z124"/>
+  <dimension ref="A1:Z128"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="18" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="22" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12"/>
@@ -1830,7 +1874,7 @@
     <col min="6" max="7" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1847,16 +1891,16 @@
         <v>143</v>
       </c>
       <c r="F1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H1" t="s">
         <v>160</v>
       </c>
-      <c r="G1" t="s">
-        <v>161</v>
-      </c>
-      <c r="H1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26">
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1864,7 +1908,7 @@
         <v>35</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
@@ -1873,21 +1917,21 @@
         <v>144</v>
       </c>
       <c r="F2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>77</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="D3" t="s">
         <v>145</v>
@@ -1896,61 +1940,61 @@
         <v>146</v>
       </c>
       <c r="F3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="E4" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="D5" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="E5" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="F5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G5" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D7" t="s">
         <v>147</v>
@@ -1959,16 +2003,16 @@
         <v>148</v>
       </c>
       <c r="F7" t="s">
-        <v>163</v>
+        <v>435</v>
       </c>
       <c r="G7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>139</v>
       </c>
@@ -1979,223 +2023,269 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>411</v>
+        <v>430</v>
       </c>
       <c r="D9" t="s">
         <v>151</v>
       </c>
       <c r="E9" t="s">
-        <v>152</v>
+        <v>429</v>
       </c>
       <c r="F9" t="s">
-        <v>163</v>
+        <v>435</v>
       </c>
       <c r="G9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H9" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>135</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
       <c r="D10" t="s">
         <v>135</v>
       </c>
       <c r="E10" t="s">
-        <v>153</v>
+        <v>432</v>
       </c>
       <c r="F10" t="s">
-        <v>163</v>
+        <v>435</v>
       </c>
       <c r="G10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H10" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26">
-      <c r="A11" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="F11" t="s">
+        <v>435</v>
+      </c>
+      <c r="G11" t="s">
+        <v>165</v>
+      </c>
+      <c r="H11" t="s">
+        <v>433</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>412</v>
+        <v>431</v>
       </c>
       <c r="D12" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E12" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
       <c r="F12" t="s">
-        <v>163</v>
+        <v>435</v>
       </c>
       <c r="G12" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H12" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>413</v>
+        <v>428</v>
       </c>
       <c r="D13" t="s">
-        <v>155</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="F13" t="s">
-        <v>163</v>
+        <v>435</v>
       </c>
       <c r="G13" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="H13" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>130</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>414</v>
+        <v>428</v>
       </c>
       <c r="D14" t="s">
         <v>157</v>
       </c>
       <c r="E14" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="F14" t="s">
-        <v>163</v>
+        <v>435</v>
       </c>
       <c r="G14" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="H14" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26">
-      <c r="A15" t="s">
-        <v>78</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>427</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="3"/>
-      <c r="W15" s="3"/>
-      <c r="X15" s="3"/>
-      <c r="Y15" s="3"/>
-      <c r="Z15" s="3"/>
-    </row>
-    <row r="16" spans="1:26">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>14</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>406</v>
       </c>
       <c r="D16" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E16" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>423</v>
+      </c>
+      <c r="F16" t="s">
+        <v>435</v>
+      </c>
+      <c r="G16" t="s">
+        <v>166</v>
+      </c>
+      <c r="H16" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>407</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>153</v>
       </c>
       <c r="E17" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>422</v>
+      </c>
+      <c r="F17" t="s">
+        <v>435</v>
+      </c>
+      <c r="G17" t="s">
+        <v>167</v>
+      </c>
+      <c r="H17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26">
       <c r="A18" t="s">
-        <v>130</v>
+        <v>12</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>408</v>
       </c>
       <c r="D18" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E18" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21">
+        <v>421</v>
+      </c>
+      <c r="F18" t="s">
+        <v>435</v>
+      </c>
+      <c r="G18" t="s">
+        <v>169</v>
+      </c>
+      <c r="H18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26">
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+    </row>
+    <row r="24" spans="1:26">
+      <c r="A24" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26">
+      <c r="A25">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22">
+    <row r="26" spans="1:26">
+      <c r="A26">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23">
+    <row r="27" spans="1:26">
+      <c r="A27">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
-      <c r="C28" s="4"/>
-    </row>
-    <row r="124" spans="14:14">
-      <c r="N124" s="1"/>
+    <row r="32" spans="1:26">
+      <c r="C32" s="4"/>
+    </row>
+    <row r="128" spans="14:14">
+      <c r="N128" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations xWindow="285" yWindow="282" count="16">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Unit." error="The Unit provided was not in the list. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." promptTitle="Unit for Observation's Value" prompt="Please describe the Unit the values are in. Whenever possible pick a value from the list." sqref="B13">
+  <dataValidations xWindow="284" yWindow="481" count="16">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Unit." error="The Unit provided was not in the list. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." promptTitle="Unit for Observation's Value" prompt="Please describe the Unit the values are in. Whenever possible pick a value from the list." sqref="B17">
       <formula1>INDIRECT(IF(ISNA(VLOOKUP(B2,FeildsThatNeedUnit,1,FALSE)),"NotApplicable","UNIT"))</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Category" prompt="Please category this data will belong to. " sqref="B1">
@@ -2207,19 +2297,19 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="id/Value Column" prompt="The column that contains the ID/value of the Category this columns applies to. Enter &quot;row&quot; if the Category has no Id column. Not required for &quot;Id&quot; or Observation's &quot;value&quot; fields." sqref="B4">
       <formula1>INDIRECT(IF(OR(B3="Id",B3="Value"),"NotApplicable"+"Column","Column"))</formula1>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="No Values Allow" error="Sorry this cell must be left blank" sqref="B6:C6 B11:C11">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="No Values Allow" error="Sorry this cell must be left blank" sqref="B6:C6 B15:C15">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Factor" error="Entered value not found in list of expected Factors. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." promptTitle="Factor for Observation's Value" prompt="Select the Factor or thing that the values in this column describe. _x000a_Selection from the offered list is HIGHLY recommended. " sqref="B12">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Factor" error="Entered value not found in list of expected Factors. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." promptTitle="Factor for Observation's Value" prompt="Select the Factor or thing that the values in this column describe. _x000a_Selection from the offered list is HIGHLY recommended. " sqref="B16">
       <formula1>INDIRECT(IF(B2="Value","Factor","NotApplicable"))</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Derviation Factor" error="The Dervation Factor select was not found in the list. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." sqref="B14">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Derviation Factor" error="The Dervation Factor select was not found in the list. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." sqref="B18">
       <formula1>INDIRECT(IF(B2="Value","DerivationFactor","NotApplicable"))</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data / Start Data" prompt="The data (and time) this observation was taken. Or if a time range the start data/ Time." sqref="B15"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="End Data" prompt="The end date/time of the date/time this observation was taken. If left blank above date will be assumed to be a single point." sqref="B16:B17"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Contirbutor" prompt="Person or Organisation that provided/ recorded/ measured the data." sqref="B18"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data / Start Data" prompt="The data (and time) this observation was taken. Or if a time range the start data/ Time." sqref="B11"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="End Data" prompt="The end date/time of the date/time this observation was taken. If left blank above date will be assumed to be a single point." sqref="B12:B13"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Contirbutor" prompt="Person or Organisation that provided/ recorded/ measured the data." sqref="B14"/>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected or Indirect Link" error="The linlk entered is not in the format of a link to data on the same page. Ignore this is you intended an external link." promptTitle="Survey" prompt="The column that contains the ID of the Survey for this Item. Enter &quot;row&quot; if the Survey has no ID column. Only applicable for columns with a &quot;Site&quot; category. " sqref="B10">
       <formula1>INDIRECT(IF(OR(B2="Site"),"Column","NotApplicable"))</formula1>
     </dataValidation>
@@ -2247,8 +2337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P258"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="J57" sqref="J2:J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -2338,7 +2428,7 @@
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>129</v>
@@ -2361,7 +2451,7 @@
     </row>
     <row r="3" spans="1:16" ht="15">
       <c r="A3" s="2" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>25</v>
@@ -2386,7 +2476,7 @@
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>125</v>
@@ -2403,7 +2493,7 @@
     </row>
     <row r="4" spans="1:16" ht="15">
       <c r="A4" s="2" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
@@ -2543,8 +2633,8 @@
         <v>136</v>
       </c>
       <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
-        <v>85</v>
+      <c r="J7" s="6" t="s">
+        <v>443</v>
       </c>
       <c r="K7" s="2"/>
       <c r="N7" t="s">
@@ -2578,7 +2668,7 @@
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K8" s="2"/>
       <c r="N8" s="2" t="s">
@@ -2612,7 +2702,7 @@
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K9" s="2"/>
       <c r="N9" t="s">
@@ -2636,7 +2726,7 @@
         <v>38</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>15</v>
@@ -2646,7 +2736,7 @@
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K10" s="2"/>
       <c r="P10" t="s">
@@ -2661,14 +2751,14 @@
         <v>39</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K11" s="2"/>
       <c r="P11" t="s">
@@ -2680,10 +2770,10 @@
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
@@ -2715,8 +2805,8 @@
       <c r="C14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>92</v>
+      <c r="J14" t="s">
+        <v>439</v>
       </c>
       <c r="K14" s="2"/>
       <c r="P14" t="s">
@@ -2725,7 +2815,7 @@
     </row>
     <row r="15" spans="1:16" ht="15">
       <c r="J15" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K15" s="2"/>
       <c r="P15" t="s">
@@ -2734,7 +2824,7 @@
     </row>
     <row r="16" spans="1:16" ht="15">
       <c r="J16" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K16" s="2"/>
       <c r="P16" t="s">
@@ -2743,7 +2833,7 @@
     </row>
     <row r="17" spans="1:16" ht="15">
       <c r="J17" s="2" t="s">
-        <v>4</v>
+        <v>94</v>
       </c>
       <c r="K17" s="2"/>
       <c r="P17" t="s">
@@ -2752,7 +2842,7 @@
     </row>
     <row r="18" spans="1:16" ht="15">
       <c r="J18" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="K18" s="2"/>
       <c r="P18" t="s">
@@ -2763,8 +2853,8 @@
       <c r="D19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="2" t="s">
-        <v>96</v>
+      <c r="J19" s="5" t="s">
+        <v>441</v>
       </c>
       <c r="K19" s="2"/>
       <c r="P19" t="s">
@@ -2777,7 +2867,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
-        <v>97</v>
+        <v>4</v>
       </c>
       <c r="K20" s="2"/>
       <c r="P20" t="s">
@@ -2790,7 +2880,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="K21" s="2"/>
       <c r="P21" t="s">
@@ -2806,7 +2896,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K22" s="2"/>
       <c r="P22" t="s">
@@ -2819,7 +2909,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2" t="s">
-        <v>99</v>
+        <v>437</v>
       </c>
       <c r="K23" s="2"/>
       <c r="P23" t="s">
@@ -2831,7 +2921,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="K24" s="2"/>
       <c r="P24" t="s">
@@ -2843,8 +2933,8 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="2" t="s">
-        <v>101</v>
+      <c r="J25" s="5" t="s">
+        <v>442</v>
       </c>
       <c r="K25" s="2"/>
       <c r="P25" t="s">
@@ -2860,7 +2950,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2" t="s">
-        <v>102</v>
+        <v>2</v>
       </c>
       <c r="K26" s="2"/>
       <c r="P26" t="s">
@@ -2870,7 +2960,7 @@
     <row r="27" spans="1:16" ht="15">
       <c r="E27" s="2"/>
       <c r="J27" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="K27" s="2"/>
       <c r="P27" t="s">
@@ -2880,7 +2970,7 @@
     <row r="28" spans="1:16" ht="15">
       <c r="E28" s="2"/>
       <c r="J28" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="K28" s="2"/>
       <c r="P28" t="s">
@@ -2892,1241 +2982,1274 @@
       <c r="B29" s="2"/>
       <c r="E29" s="2"/>
       <c r="J29" s="2" t="s">
-        <v>3</v>
+        <v>105</v>
       </c>
       <c r="K29" s="2"/>
       <c r="P29" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15">
       <c r="E30" s="2"/>
       <c r="J30" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K30" s="2"/>
       <c r="P30" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15">
       <c r="E31" s="2"/>
       <c r="J31" s="2" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="K31" s="2"/>
       <c r="P31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15">
       <c r="E32" s="2"/>
       <c r="J32" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="K32" s="2"/>
       <c r="P32" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="5:16" ht="15">
       <c r="E33" s="2"/>
       <c r="J33" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="K33" s="2"/>
       <c r="P33" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="34" spans="5:16" ht="15">
       <c r="E34" s="2"/>
       <c r="J34" s="2" t="s">
-        <v>108</v>
+        <v>3</v>
       </c>
       <c r="K34" s="2"/>
       <c r="P34" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="5:16" ht="15">
       <c r="E35" s="2"/>
       <c r="J35" s="2" t="s">
-        <v>109</v>
+        <v>45</v>
       </c>
       <c r="K35" s="2"/>
       <c r="P35" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="36" spans="5:16" ht="15">
       <c r="E36" s="2"/>
-      <c r="J36" s="2" t="s">
-        <v>110</v>
+      <c r="J36" t="s">
+        <v>436</v>
       </c>
       <c r="K36" s="2"/>
       <c r="P36" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="5:16" ht="15">
       <c r="E37" s="2"/>
       <c r="J37" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="K37" s="2"/>
       <c r="P37" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="5:16" ht="15">
       <c r="E38" s="2"/>
       <c r="J38" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="K38" s="2"/>
       <c r="P38" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="5:16" ht="15">
       <c r="E39" s="2"/>
       <c r="J39" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="K39" s="2"/>
       <c r="P39" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="5:16" ht="15">
       <c r="J40" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="K40" s="2"/>
       <c r="P40" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="5:16" ht="15">
       <c r="J41" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K41" s="2"/>
       <c r="P41" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="5:16" ht="15">
       <c r="J42" s="2" t="s">
-        <v>116</v>
+        <v>438</v>
       </c>
       <c r="K42" s="2"/>
       <c r="P42" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="43" spans="5:16" ht="15">
       <c r="J43" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="K43" s="2"/>
       <c r="P43" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44" spans="5:16" ht="15">
       <c r="J44" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="K44" s="2"/>
       <c r="P44" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="45" spans="5:16" ht="15">
-      <c r="J45" s="2" t="s">
-        <v>120</v>
+      <c r="J45" t="s">
+        <v>440</v>
       </c>
       <c r="K45" s="2"/>
       <c r="P45" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" spans="5:16" ht="15">
-      <c r="J46" s="2" t="s">
-        <v>119</v>
+      <c r="J46" s="6" t="s">
+        <v>444</v>
       </c>
       <c r="K46" s="2"/>
       <c r="P46" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="47" spans="5:16" ht="15">
       <c r="J47" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="K47" s="2"/>
       <c r="P47" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="48" spans="5:16" ht="15">
+      <c r="J48" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="P48" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="49" spans="10:16">
+      <c r="J49" t="s">
+        <v>22</v>
+      </c>
+      <c r="P49" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="50" spans="10:16" ht="15">
+      <c r="J50" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="P50" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="51" spans="10:16" ht="15">
+      <c r="J51" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="P51" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="52" spans="10:16" ht="15">
+      <c r="J52" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="P52" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="48" spans="5:16">
-      <c r="P48" t="s">
+    <row r="53" spans="10:16" ht="15">
+      <c r="J53" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="P53" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="49" spans="16:16">
-      <c r="P49" t="s">
+    <row r="54" spans="10:16" ht="15">
+      <c r="J54" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="P54" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="50" spans="16:16">
-      <c r="P50" t="s">
+    <row r="55" spans="10:16" ht="15">
+      <c r="J55" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="P55" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="51" spans="16:16">
-      <c r="P51" t="s">
+    <row r="56" spans="10:16" ht="15">
+      <c r="J56" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="P56" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="52" spans="16:16">
-      <c r="P52" t="s">
+    <row r="57" spans="10:16" ht="15">
+      <c r="J57" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="P57" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="53" spans="16:16">
-      <c r="P53" t="s">
+    <row r="58" spans="10:16">
+      <c r="P58" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="54" spans="16:16">
-      <c r="P54" t="s">
+    <row r="59" spans="10:16">
+      <c r="P59" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="55" spans="16:16">
-      <c r="P55" t="s">
+    <row r="60" spans="10:16">
+      <c r="P60" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="56" spans="16:16">
-      <c r="P56" t="s">
+    <row r="61" spans="10:16">
+      <c r="P61" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="57" spans="16:16">
-      <c r="P57" t="s">
+    <row r="62" spans="10:16">
+      <c r="P62" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="58" spans="16:16">
-      <c r="P58" t="s">
+    <row r="63" spans="10:16">
+      <c r="P63" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="59" spans="16:16">
-      <c r="P59" t="s">
+    <row r="64" spans="10:16">
+      <c r="P64" t="s">
         <v>206</v>
-      </c>
-    </row>
-    <row r="60" spans="16:16">
-      <c r="P60" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="61" spans="16:16">
-      <c r="P61" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="62" spans="16:16">
-      <c r="P62" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="63" spans="16:16">
-      <c r="P63" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="64" spans="16:16">
-      <c r="P64" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="65" spans="16:16">
       <c r="P65" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="66" spans="16:16">
       <c r="P66" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="67" spans="16:16">
       <c r="P67" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="68" spans="16:16">
       <c r="P68" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="69" spans="16:16">
       <c r="P69" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="70" spans="16:16">
       <c r="P70" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="71" spans="16:16">
       <c r="P71" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="72" spans="16:16">
       <c r="P72" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="73" spans="16:16">
       <c r="P73" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="74" spans="16:16">
       <c r="P74" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="75" spans="16:16">
       <c r="P75" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="76" spans="16:16">
       <c r="P76" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="77" spans="16:16">
       <c r="P77" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="78" spans="16:16">
       <c r="P78" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="79" spans="16:16">
       <c r="P79" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="80" spans="16:16">
       <c r="P80" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="81" spans="16:16">
       <c r="P81" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="82" spans="16:16">
       <c r="P82" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="83" spans="16:16">
       <c r="P83" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="84" spans="16:16">
       <c r="P84" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="85" spans="16:16">
       <c r="P85" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="86" spans="16:16">
       <c r="P86" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="87" spans="16:16">
       <c r="P87" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="88" spans="16:16">
       <c r="P88" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="89" spans="16:16">
       <c r="P89" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="90" spans="16:16">
       <c r="P90" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="91" spans="16:16">
       <c r="P91" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="92" spans="16:16">
       <c r="P92" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="93" spans="16:16">
       <c r="P93" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="94" spans="16:16">
       <c r="P94" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="95" spans="16:16">
       <c r="P95" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="96" spans="16:16">
       <c r="P96" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="97" spans="16:16">
       <c r="P97" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="98" spans="16:16">
       <c r="P98" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="99" spans="16:16">
       <c r="P99" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="100" spans="16:16">
       <c r="P100" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="101" spans="16:16">
       <c r="P101" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="102" spans="16:16">
       <c r="P102" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="103" spans="16:16">
       <c r="P103" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="104" spans="16:16">
       <c r="P104" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="105" spans="16:16">
       <c r="P105" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="106" spans="16:16">
       <c r="P106" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="107" spans="16:16">
       <c r="P107" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="108" spans="16:16">
       <c r="P108" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="109" spans="16:16">
       <c r="P109" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="110" spans="16:16">
       <c r="P110" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="111" spans="16:16">
       <c r="P111" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="112" spans="16:16">
       <c r="P112" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="113" spans="16:16">
       <c r="P113" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="114" spans="16:16">
       <c r="P114" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="115" spans="16:16">
       <c r="P115" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="116" spans="16:16">
       <c r="P116" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="117" spans="16:16">
       <c r="P117" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="118" spans="16:16">
       <c r="P118" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="119" spans="16:16">
       <c r="P119" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="120" spans="16:16">
       <c r="P120" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="121" spans="16:16">
       <c r="P121" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="122" spans="16:16">
       <c r="P122" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="123" spans="16:16">
       <c r="P123" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="124" spans="16:16">
       <c r="P124" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="125" spans="16:16">
       <c r="P125" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="126" spans="16:16">
       <c r="P126" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="127" spans="16:16">
       <c r="P127" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="128" spans="16:16">
       <c r="P128" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="129" spans="16:16">
       <c r="P129" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="130" spans="16:16">
       <c r="P130" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="131" spans="16:16">
       <c r="P131" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="132" spans="16:16">
       <c r="P132" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="133" spans="16:16">
       <c r="P133" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="134" spans="16:16">
       <c r="P134" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="135" spans="16:16">
       <c r="P135" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="136" spans="16:16">
       <c r="P136" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="137" spans="16:16">
       <c r="P137" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="138" spans="16:16">
       <c r="P138" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="139" spans="16:16">
       <c r="P139" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="140" spans="16:16">
       <c r="P140" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="141" spans="16:16">
       <c r="P141" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="142" spans="16:16">
       <c r="P142" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="143" spans="16:16">
       <c r="P143" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="144" spans="16:16">
       <c r="P144" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="145" spans="16:16">
       <c r="P145" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="146" spans="16:16">
       <c r="P146" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="147" spans="16:16">
       <c r="P147" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="148" spans="16:16">
       <c r="P148" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="149" spans="16:16">
       <c r="P149" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="150" spans="16:16">
       <c r="P150" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="151" spans="16:16">
       <c r="P151" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="152" spans="16:16">
       <c r="P152" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
     </row>
     <row r="153" spans="16:16">
       <c r="P153" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="154" spans="16:16">
       <c r="P154" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="155" spans="16:16">
       <c r="P155" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="156" spans="16:16">
       <c r="P156" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="157" spans="16:16">
       <c r="P157" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="158" spans="16:16">
       <c r="P158" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="159" spans="16:16">
       <c r="P159" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="160" spans="16:16">
       <c r="P160" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="161" spans="16:16">
       <c r="P161" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="162" spans="16:16">
       <c r="P162" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="163" spans="16:16">
       <c r="P163" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="164" spans="16:16">
       <c r="P164" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="165" spans="16:16">
       <c r="P165" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="166" spans="16:16">
       <c r="P166" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="167" spans="16:16">
       <c r="P167" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="168" spans="16:16">
       <c r="P168" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="169" spans="16:16">
       <c r="P169" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="170" spans="16:16">
       <c r="P170" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="171" spans="16:16">
       <c r="P171" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="172" spans="16:16">
       <c r="P172" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="173" spans="16:16">
       <c r="P173" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="174" spans="16:16">
       <c r="P174" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="175" spans="16:16">
       <c r="P175" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="176" spans="16:16">
       <c r="P176" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="177" spans="16:16">
       <c r="P177" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="178" spans="16:16">
       <c r="P178" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="179" spans="16:16">
       <c r="P179" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="180" spans="16:16">
       <c r="P180" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="181" spans="16:16">
       <c r="P181" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="182" spans="16:16">
       <c r="P182" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="183" spans="16:16">
       <c r="P183" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="184" spans="16:16">
       <c r="P184" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="185" spans="16:16">
       <c r="P185" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="186" spans="16:16">
       <c r="P186" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="187" spans="16:16">
       <c r="P187" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="188" spans="16:16">
       <c r="P188" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="189" spans="16:16">
       <c r="P189" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="190" spans="16:16">
       <c r="P190" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="191" spans="16:16">
       <c r="P191" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="192" spans="16:16">
       <c r="P192" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="193" spans="16:16">
       <c r="P193" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="194" spans="16:16">
       <c r="P194" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="195" spans="16:16">
       <c r="P195" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="196" spans="16:16">
       <c r="P196" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="197" spans="16:16">
       <c r="P197" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="198" spans="16:16">
       <c r="P198" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="199" spans="16:16">
       <c r="P199" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="200" spans="16:16">
       <c r="P200" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="201" spans="16:16">
       <c r="P201" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="202" spans="16:16">
       <c r="P202" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="203" spans="16:16">
       <c r="P203" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="204" spans="16:16">
       <c r="P204" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="205" spans="16:16">
       <c r="P205" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="206" spans="16:16">
       <c r="P206" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
     <row r="207" spans="16:16">
       <c r="P207" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
     </row>
     <row r="208" spans="16:16">
       <c r="P208" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="209" spans="16:16">
       <c r="P209" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="210" spans="16:16">
       <c r="P210" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="211" spans="16:16">
       <c r="P211" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="212" spans="16:16">
       <c r="P212" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="213" spans="16:16">
       <c r="P213" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="214" spans="16:16">
       <c r="P214" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="215" spans="16:16">
       <c r="P215" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="216" spans="16:16">
       <c r="P216" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="217" spans="16:16">
       <c r="P217" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="218" spans="16:16">
       <c r="P218" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="219" spans="16:16">
       <c r="P219" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="220" spans="16:16">
       <c r="P220" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="221" spans="16:16">
       <c r="P221" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="222" spans="16:16">
       <c r="P222" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="223" spans="16:16">
       <c r="P223" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="224" spans="16:16">
       <c r="P224" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="225" spans="16:16">
       <c r="P225" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="226" spans="16:16">
       <c r="P226" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
     </row>
     <row r="227" spans="16:16">
       <c r="P227" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="228" spans="16:16">
       <c r="P228" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="229" spans="16:16">
       <c r="P229" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="230" spans="16:16">
       <c r="P230" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="231" spans="16:16">
       <c r="P231" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
     <row r="232" spans="16:16">
       <c r="P232" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
     <row r="233" spans="16:16">
       <c r="P233" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
     </row>
     <row r="234" spans="16:16">
       <c r="P234" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="235" spans="16:16">
       <c r="P235" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
     </row>
     <row r="236" spans="16:16">
       <c r="P236" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="237" spans="16:16">
       <c r="P237" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="238" spans="16:16">
       <c r="P238" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="239" spans="16:16">
       <c r="P239" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
     </row>
     <row r="240" spans="16:16">
       <c r="P240" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="241" spans="16:16">
       <c r="P241" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="242" spans="16:16">
       <c r="P242" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="243" spans="16:16">
       <c r="P243" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="244" spans="16:16">
       <c r="P244" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="245" spans="16:16">
       <c r="P245" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
     </row>
     <row r="246" spans="16:16">
       <c r="P246" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="247" spans="16:16">
       <c r="P247" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="248" spans="16:16">
       <c r="P248" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
     </row>
     <row r="249" spans="16:16">
       <c r="P249" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="250" spans="16:16">
       <c r="P250" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="251" spans="16:16">
       <c r="P251" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="252" spans="16:16">
       <c r="P252" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="253" spans="16:16">
       <c r="P253" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="254" spans="16:16">
       <c r="P254" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="255" spans="16:16">
       <c r="P255" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
     </row>
     <row r="256" spans="16:16">
       <c r="P256" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="257" spans="16:16">
       <c r="P257" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
     </row>
     <row r="258" spans="16:16">
       <c r="P258" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="J2:J57">
+    <sortCondition ref="J2:J57"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
All datavalidation forumals are now absolute due to difference between how excell 2007 and Excel 2010 handle relative ones.
</commit_message>
<xml_diff>
--- a/data/MetaMaster.xlsx
+++ b/data/MetaMaster.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="24030" windowHeight="5790" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="24030" windowHeight="5790"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,12 +37,12 @@
     <definedName name="UNDEFINED">Lists!$L$2</definedName>
     <definedName name="Unit">Lists!$N$2:$N$9</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="446">
   <si>
     <t>Easting</t>
   </si>
@@ -1247,30 +1247,12 @@
     <t>IV</t>
   </si>
   <si>
-    <t>INDIRECT(SUBSTITUTE(A$1," ","_"))</t>
-  </si>
-  <si>
-    <t>INDIRECT(IF(OR(A$2="Id",A$2="Value"),"NotApplicable","Column"))</t>
-  </si>
-  <si>
     <t>External_ID</t>
   </si>
   <si>
     <t>External_Link</t>
   </si>
   <si>
-    <t>INDIRECT(IF(OR(A$2="Value"),"Column","NotApplicable"))</t>
-  </si>
-  <si>
-    <t>INDIRECT(IF(A$2="Value","Factor","NotApplicable"))</t>
-  </si>
-  <si>
-    <t>INDIRECT(IF(ISNA(VLOOKUP(A$2,FeildsThatNeedUnit,1,FALSE)),"NotApplicable","UNIT"))</t>
-  </si>
-  <si>
-    <t>INDIRECT(IF(A$2="Value","DerivationFactor","NotApplicable"))</t>
-  </si>
-  <si>
     <t>External Sheet</t>
   </si>
   <si>
@@ -1328,18 +1310,9 @@
     <t>Lifeform</t>
   </si>
   <si>
-    <t>INDIRECT(IF(OR(A$2="Value",A$2="Id"),"Column","NotApplicable"))</t>
-  </si>
-  <si>
     <t xml:space="preserve">The column that contains the ID of the Location for this Site. Enter "row" if the Location has no ID column. Start Constants with =. Only applicable for columns with a "Site" category. </t>
   </si>
   <si>
-    <t>INDIRECT(IF(A$1="Site","Column","NotApplicable"))</t>
-  </si>
-  <si>
-    <t>INDIRECT(IF(A$2="Value","Column","NotApplicable"))</t>
-  </si>
-  <si>
     <t xml:space="preserve">The column that contains the ID of the Survey for this Item. Enter "row" if the Survey has no ID column. Start constants with an =. Only applicable for columns with a "Value" field. </t>
   </si>
   <si>
@@ -1377,12 +1350,42 @@
   </si>
   <si>
     <t>SKIDDAW_S</t>
+  </si>
+  <si>
+    <t>INDIRECT(IF(OR($B$2="Id",$B$2="Value"),"NotApplicable","Column"))</t>
+  </si>
+  <si>
+    <t>INDIRECT(SUBSTITUTE($B$1," ","_"))</t>
+  </si>
+  <si>
+    <t>INDIRECT(IF(OR($B$2="Value"),"Column","NotApplicable"))</t>
+  </si>
+  <si>
+    <t>INDIRECT(IF($B$1="Site","Column","NotApplicable"))</t>
+  </si>
+  <si>
+    <t>INDIRECT(IF($B$2="Value","Column","NotApplicable"))</t>
+  </si>
+  <si>
+    <t>INDIRECT(IF(OR($B$2="Value",A$2="Id"),"Column","NotApplicable"))</t>
+  </si>
+  <si>
+    <t>INDIRECT(IF(OR($B$2="Value",$B$2="Id"),"Column","NotApplicable"))</t>
+  </si>
+  <si>
+    <t>INDIRECT(IF($B$2="Value","Factor","NotApplicable"))</t>
+  </si>
+  <si>
+    <t>INDIRECT(IF(ISNA(VLOOKUP($B$2,FeildsThatNeedUnit,1,FALSE)),"NotApplicable","UNIT"))</t>
+  </si>
+  <si>
+    <t>INDIRECT(IF($B$2="Value","DerivationFactor","NotApplicable"))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="5">
     <font>
       <sz val="9"/>
@@ -1425,8 +1428,8 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1436,26 +1439,21 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Survey"/>
@@ -1492,7 +1490,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Locations"/>
@@ -1643,7 +1641,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1678,7 +1675,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1854,14 +1850,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z128"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="22" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="22" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12"/>
@@ -1908,7 +1904,7 @@
         <v>35</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>401</v>
+        <v>437</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
@@ -1931,7 +1927,7 @@
         <v>77</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>402</v>
+        <v>436</v>
       </c>
       <c r="D3" t="s">
         <v>145</v>
@@ -1951,37 +1947,37 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="E4" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="D5" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="E5" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="F5" t="s">
         <v>158</v>
       </c>
       <c r="G5" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1994,7 +1990,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>405</v>
+        <v>438</v>
       </c>
       <c r="D7" t="s">
         <v>147</v>
@@ -2003,13 +1999,13 @@
         <v>148</v>
       </c>
       <c r="F7" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="G7" t="s">
         <v>165</v>
       </c>
       <c r="H7" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -2028,22 +2024,22 @@
         <v>19</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="D9" t="s">
         <v>151</v>
       </c>
       <c r="E9" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="F9" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="G9" t="s">
         <v>165</v>
       </c>
       <c r="H9" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -2051,22 +2047,22 @@
         <v>135</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="D10" t="s">
         <v>135</v>
       </c>
       <c r="E10" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="F10" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="G10" t="s">
         <v>165</v>
       </c>
       <c r="H10" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -2075,22 +2071,22 @@
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="4" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>154</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="F11" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="G11" t="s">
         <v>165</v>
       </c>
       <c r="H11" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -2103,22 +2099,22 @@
         <v>79</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="D12" t="s">
         <v>156</v>
       </c>
       <c r="E12" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="F12" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="G12" t="s">
         <v>165</v>
       </c>
       <c r="H12" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -2126,22 +2122,22 @@
         <v>26</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>428</v>
+        <v>441</v>
       </c>
       <c r="D13" t="s">
         <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="F13" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="G13" t="s">
         <v>165</v>
       </c>
       <c r="H13" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -2149,22 +2145,22 @@
         <v>130</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>428</v>
+        <v>442</v>
       </c>
       <c r="D14" t="s">
         <v>157</v>
       </c>
       <c r="E14" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="F14" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="G14" t="s">
         <v>165</v>
       </c>
       <c r="H14" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -2177,22 +2173,22 @@
         <v>14</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>406</v>
+        <v>443</v>
       </c>
       <c r="D16" t="s">
         <v>152</v>
       </c>
       <c r="E16" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="F16" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="G16" t="s">
         <v>166</v>
       </c>
       <c r="H16" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
     </row>
     <row r="17" spans="1:26">
@@ -2200,16 +2196,16 @@
         <v>34</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>407</v>
+        <v>444</v>
       </c>
       <c r="D17" t="s">
         <v>153</v>
       </c>
       <c r="E17" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="F17" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="G17" t="s">
         <v>167</v>
@@ -2223,16 +2219,16 @@
         <v>12</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>408</v>
+        <v>445</v>
       </c>
       <c r="D18" t="s">
         <v>155</v>
       </c>
       <c r="E18" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="F18" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="G18" t="s">
         <v>169</v>
@@ -2258,7 +2254,7 @@
     </row>
     <row r="24" spans="1:26">
       <c r="A24" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
     </row>
     <row r="25" spans="1:26">
@@ -2284,15 +2280,15 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations xWindow="284" yWindow="481" count="16">
+  <dataValidations xWindow="284" yWindow="481" count="17">
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Unit." error="The Unit provided was not in the list. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." promptTitle="Unit for Observation's Value" prompt="Please describe the Unit the values are in. Whenever possible pick a value from the list." sqref="B17">
-      <formula1>INDIRECT(IF(ISNA(VLOOKUP(B2,FeildsThatNeedUnit,1,FALSE)),"NotApplicable","UNIT"))</formula1>
+      <formula1>"INDIRECT(IF(ISNA(VLOOKUP($B$2,FeildsThatNeedUnit,1,FALSE)),""NotApplicable"",""UNIT""))"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Category" prompt="Please category this data will belong to. " sqref="B1">
       <formula1>Category</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Feild Value" error="Sorry Feild value input does not match the expected feilds for the category you picked.  Only add and unexpected feild if you are sure no Category and Feild combination matches ths column. You may have to explain this!" promptTitle="Field" prompt="Please Select the feild that data in this column belongs to. Options available depend on the Category selected above." sqref="B2">
-      <formula1>INDIRECT(SUBSTITUTE(B1," ","_"))</formula1>
+      <formula1>INDIRECT(SUBSTITUTE(B$1," ","_"))</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="id/Value Column" prompt="The column that contains the ID/value of the Category this columns applies to. Enter &quot;row&quot; if the Category has no Id column. Not required for &quot;Id&quot; or Observation's &quot;value&quot; fields." sqref="B4">
       <formula1>INDIRECT(IF(OR(B3="Id",B3="Value"),"NotApplicable"+"Column","Column"))</formula1>
@@ -2302,29 +2298,36 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Factor" error="Entered value not found in list of expected Factors. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." promptTitle="Factor for Observation's Value" prompt="Select the Factor or thing that the values in this column describe. _x000a_Selection from the offered list is HIGHLY recommended. " sqref="B16">
-      <formula1>INDIRECT(IF(B2="Value","Factor","NotApplicable"))</formula1>
+      <formula1>INDIRECT(IF($B$2="Value","Factor","NotApplicable"))</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Derviation Factor" error="The Dervation Factor select was not found in the list. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." sqref="B18">
-      <formula1>INDIRECT(IF(B2="Value","DerivationFactor","NotApplicable"))</formula1>
+      <formula1>INDIRECT(IF($B$2="Value","DerivationFactor","NotApplicable"))</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data / Start Data" prompt="The data (and time) this observation was taken. Or if a time range the start data/ Time." sqref="B11"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="End Data" prompt="The end date/time of the date/time this observation was taken. If left blank above date will be assumed to be a single point." sqref="B12:B13"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Contirbutor" prompt="Person or Organisation that provided/ recorded/ measured the data." sqref="B14"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data / Start Data" prompt="The data (and time) this observation was taken. Or if a time range the start data/ Time." sqref="B11">
+      <formula1>INDIRECT(IF($B$2="Value","Column","NotApplicable"))</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="End Data" prompt="The end date/time of the date/time this observation was taken. If left blank above date will be assumed to be a single point." sqref="B13"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Contirbutor" prompt="Person or Organisation that provided/ recorded/ measured the data." sqref="B14">
+      <formula1>INDIRECT(IF(OR($B$2="Value",$B$2="Id"),"Column","NotApplicable"))</formula1>
+    </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected or Indirect Link" error="The linlk entered is not in the format of a link to data on the same page. Ignore this is you intended an external link." promptTitle="Survey" prompt="The column that contains the ID of the Survey for this Item. Enter &quot;row&quot; if the Survey has no ID column. Only applicable for columns with a &quot;Site&quot; category. " sqref="B10">
-      <formula1>INDIRECT(IF(OR(B2="Site"),"Column","NotApplicable"))</formula1>
+      <formula1>INDIRECT(IF($B$2="Value","Column","NotApplicable"))</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="&quot;Unexpected column reference&quot;" error="The link does not refer to a link on the same page. Please ignore this if you intended an external link." promptTitle="Site for Observation/Value" prompt="The column that contains the ID of the Site this Observation applies to. Enter &quot;row&quot; if the Site has no ID column. Only applicable for columns with Observation's &quot;value&quot; field." sqref="B7">
-      <formula1>INDIRECT(IF(OR(B2="Value"),"Column","NotApplicable"))</formula1>
+      <formula1>INDIRECT(IF(OR($B$2="Value"),"Column","NotApplicable"))</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="&quot;Unexpected column reference&quot;" promptTitle="Type of Link to the Site" prompt="Advance feature: The default (if left blank) is to associate the site as vocab:site. If a different vocab: is to be used enter it here." sqref="B8:C8"/>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Location for Site" prompt="The column that contains the ID of the Location for this Site. Enter &quot;row&quot; if the Location has no ID column. Only applicable for columns with a &quot;Site&quot; category. " sqref="B9">
-      <formula1>INDIRECT(IF(OR(B1="Site"),"Column","NotApplicable"))</formula1>
+      <formula1>INDIRECT(IF($B$1="Site","Column","NotApplicable"))</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Ignore Zeros" prompt="If set to true any zeros in this column will be treated as nulls." sqref="B5">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="id/Value Column" prompt="The column that contains the ID/value of the Category this columns applies to. Enter &quot;row&quot; if the Category has no Id column. Not required for &quot;Id&quot; or Observation's &quot;value&quot; fields." sqref="B3">
-      <formula1>INDIRECT(IF(OR(B2="Id",B2="Value"),"NotApplicable","Column"))</formula1>
+      <formula1>INDIRECT(IF(OR($B$2="Id",$B$2="Value"),"NotApplicable","Column"))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="End Data" prompt="The end date/time of the date/time this observation was taken. If left blank above date will be assumed to be a single point." sqref="B12">
+      <formula1>INDIRECT(IF($B$2="Value","Column","NotApplicable"))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2334,11 +2337,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="J57" sqref="J2:J57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -2451,7 +2454,7 @@
     </row>
     <row r="3" spans="1:16" ht="15">
       <c r="A3" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>25</v>
@@ -2493,7 +2496,7 @@
     </row>
     <row r="4" spans="1:16" ht="15">
       <c r="A4" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
@@ -2634,7 +2637,7 @@
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="6" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="K7" s="2"/>
       <c r="N7" t="s">
@@ -2726,7 +2729,7 @@
         <v>38</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>15</v>
@@ -2751,7 +2754,7 @@
         <v>39</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>18</v>
@@ -2770,10 +2773,10 @@
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
@@ -2806,7 +2809,7 @@
         <v>33</v>
       </c>
       <c r="J14" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="K14" s="2"/>
       <c r="P14" t="s">
@@ -2854,7 +2857,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="5" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="K19" s="2"/>
       <c r="P19" t="s">
@@ -2909,7 +2912,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="K23" s="2"/>
       <c r="P23" t="s">
@@ -2934,7 +2937,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="5" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="K25" s="2"/>
       <c r="P25" t="s">
@@ -3052,7 +3055,7 @@
     <row r="36" spans="5:16" ht="15">
       <c r="E36" s="2"/>
       <c r="J36" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="K36" s="2"/>
       <c r="P36" t="s">
@@ -3109,7 +3112,7 @@
     </row>
     <row r="42" spans="5:16" ht="15">
       <c r="J42" s="2" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="K42" s="2"/>
       <c r="P42" t="s">
@@ -3136,7 +3139,7 @@
     </row>
     <row r="45" spans="5:16" ht="15">
       <c r="J45" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="K45" s="2"/>
       <c r="P45" t="s">
@@ -3145,7 +3148,7 @@
     </row>
     <row r="46" spans="5:16" ht="15">
       <c r="J46" s="6" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="K46" s="2"/>
       <c r="P46" t="s">
@@ -4247,9 +4250,6 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="J2:J57">
-    <sortCondition ref="J2:J57"/>
-  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4257,7 +4257,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4280,6 +4280,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added no length data validation where needed.Buig fix on errors.
</commit_message>
<xml_diff>
--- a/data/MetaMaster.xlsx
+++ b/data/MetaMaster.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="24030" windowHeight="5790"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="24030" windowHeight="5790" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="446">
   <si>
     <t>Easting</t>
   </si>
@@ -461,9 +461,6 @@
     <t>Initial</t>
   </si>
   <si>
-    <t>*Site Link Type*</t>
-  </si>
-  <si>
     <t>File</t>
   </si>
   <si>
@@ -491,12 +488,6 @@
     <t>The column that contains the ID of the Site this Observation applies to. Enter "row" if the Site has no ID column. Only applicable for columns with Observation's "value" field.</t>
   </si>
   <si>
-    <t>Type of Link to the Site</t>
-  </si>
-  <si>
-    <t>Advance feature: The default (if left blank) is to associate the site as vocab:site. If a different vocab: is to be used enter it here.</t>
-  </si>
-  <si>
     <t>Location for Site</t>
   </si>
   <si>
@@ -1271,9 +1262,6 @@
     <t>Only legal values are "TRUE", "FALSE". Where a null/Blank is treated as "FALSE".</t>
   </si>
   <si>
-    <t>SimilarTo</t>
-  </si>
-  <si>
     <t>Header</t>
   </si>
   <si>
@@ -1380,6 +1368,18 @@
   </si>
   <si>
     <t>INDIRECT(IF($B$2="Value","DerivationFactor","NotApplicable"))</t>
+  </si>
+  <si>
+    <t>BLANK</t>
+  </si>
+  <si>
+    <t>No Values Allow</t>
+  </si>
+  <si>
+    <t>Sorry this cell must be left blank</t>
+  </si>
+  <si>
+    <t>isSimilarTo</t>
   </si>
 </sst>
 </file>
@@ -1851,13 +1851,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z128"/>
+  <dimension ref="A1:Z127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="22" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="21" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12"/>
@@ -1884,16 +1884,16 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1904,22 +1904,22 @@
         <v>35</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G2" t="s">
         <v>158</v>
       </c>
-      <c r="G2" t="s">
-        <v>161</v>
-      </c>
       <c r="H2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1927,365 +1927,375 @@
         <v>77</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E3" t="s">
         <v>145</v>
       </c>
-      <c r="E3" t="s">
-        <v>146</v>
-      </c>
       <c r="F3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="E4" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D5" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="E5" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="F5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G5" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="C6" t="s">
+        <v>442</v>
+      </c>
+      <c r="F6" t="s">
+        <v>155</v>
+      </c>
+      <c r="G6" t="s">
+        <v>443</v>
+      </c>
+      <c r="H6" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="D7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" t="s">
         <v>147</v>
       </c>
-      <c r="E7" t="s">
-        <v>148</v>
-      </c>
       <c r="F7" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H7" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>139</v>
+        <v>19</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>435</v>
       </c>
       <c r="D8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E8" t="s">
-        <v>150</v>
+        <v>418</v>
+      </c>
+      <c r="F8" t="s">
+        <v>422</v>
+      </c>
+      <c r="G8" t="s">
+        <v>162</v>
+      </c>
+      <c r="H8" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>135</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D9" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="E9" t="s">
+        <v>419</v>
+      </c>
+      <c r="F9" t="s">
         <v>422</v>
       </c>
-      <c r="F9" t="s">
-        <v>426</v>
-      </c>
       <c r="G9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H9" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>135</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B10" s="3"/>
       <c r="C10" s="4" t="s">
-        <v>440</v>
-      </c>
-      <c r="D10" t="s">
-        <v>135</v>
-      </c>
-      <c r="E10" t="s">
-        <v>423</v>
+        <v>436</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="F10" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H10" t="s">
-        <v>424</v>
-      </c>
+        <v>420</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" s="3"/>
+        <v>79</v>
+      </c>
       <c r="C11" s="4" t="s">
-        <v>440</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>414</v>
+        <v>436</v>
+      </c>
+      <c r="D11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E11" t="s">
+        <v>409</v>
       </c>
       <c r="F11" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G11" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H11" t="s">
-        <v>424</v>
-      </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
+        <v>420</v>
+      </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D12" t="s">
-        <v>156</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="F12" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G12" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H12" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>130</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>154</v>
       </c>
       <c r="E13" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="F13" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G13" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H13" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" t="s">
-        <v>130</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="A14" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" t="s">
         <v>442</v>
       </c>
-      <c r="D14" t="s">
-        <v>157</v>
-      </c>
-      <c r="E14" t="s">
-        <v>412</v>
-      </c>
       <c r="F14" t="s">
-        <v>426</v>
+        <v>155</v>
       </c>
       <c r="G14" t="s">
-        <v>165</v>
+        <v>443</v>
       </c>
       <c r="H14" t="s">
-        <v>424</v>
+        <v>444</v>
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="4" t="s">
-        <v>131</v>
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="D15" t="s">
+        <v>149</v>
+      </c>
+      <c r="E15" t="s">
+        <v>413</v>
+      </c>
+      <c r="F15" t="s">
+        <v>422</v>
+      </c>
+      <c r="G15" t="s">
+        <v>163</v>
+      </c>
+      <c r="H15" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D16" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E16" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="F16" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H16" t="s">
-        <v>425</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:26">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E17" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="F17" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G17" t="s">
+        <v>166</v>
+      </c>
+      <c r="H17" t="s">
         <v>167</v>
       </c>
-      <c r="H17" t="s">
-        <v>168</v>
-      </c>
     </row>
     <row r="18" spans="1:26">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="D18" t="s">
-        <v>155</v>
-      </c>
-      <c r="E18" t="s">
-        <v>415</v>
-      </c>
-      <c r="F18" t="s">
-        <v>426</v>
-      </c>
-      <c r="G18" t="s">
-        <v>169</v>
-      </c>
-      <c r="H18" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26">
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
-      <c r="Y19" s="3"/>
-      <c r="Z19" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
+    </row>
+    <row r="23" spans="1:26">
+      <c r="A23" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="24" spans="1:26">
-      <c r="A24" t="s">
-        <v>410</v>
+      <c r="A24">
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:26">
       <c r="A25">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:26">
       <c r="A26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26">
-      <c r="A27">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:26">
-      <c r="C32" s="4"/>
-    </row>
-    <row r="128" spans="14:14">
-      <c r="N128" s="1"/>
+    <row r="31" spans="1:26">
+      <c r="C31" s="4"/>
+    </row>
+    <row r="127" spans="14:14">
+      <c r="N127" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations xWindow="284" yWindow="481" count="17">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Unit." error="The Unit provided was not in the list. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." promptTitle="Unit for Observation's Value" prompt="Please describe the Unit the values are in. Whenever possible pick a value from the list." sqref="B17">
+  <dataValidations xWindow="284" yWindow="481" count="16">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Unit." error="The Unit provided was not in the list. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." promptTitle="Unit for Observation's Value" prompt="Please describe the Unit the values are in. Whenever possible pick a value from the list." sqref="B16">
       <formula1>"INDIRECT(IF(ISNA(VLOOKUP($B$2,FeildsThatNeedUnit,1,FALSE)),""NotApplicable"",""UNIT""))"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Category" prompt="Please category this data will belong to. " sqref="B1">
-      <formula1>Category</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Feild Value" error="Sorry Feild value input does not match the expected feilds for the category you picked.  Only add and unexpected feild if you are sure no Category and Feild combination matches ths column. You may have to explain this!" promptTitle="Field" prompt="Please Select the feild that data in this column belongs to. Options available depend on the Category selected above." sqref="B2">
       <formula1>INDIRECT(SUBSTITUTE(B$1," ","_"))</formula1>
@@ -2293,41 +2303,43 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="id/Value Column" prompt="The column that contains the ID/value of the Category this columns applies to. Enter &quot;row&quot; if the Category has no Id column. Not required for &quot;Id&quot; or Observation's &quot;value&quot; fields." sqref="B4">
       <formula1>INDIRECT(IF(OR(B3="Id",B3="Value"),"NotApplicable"+"Column","Column"))</formula1>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="No Values Allow" error="Sorry this cell must be left blank" sqref="B6:C6 B15:C15">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="No Values Allow" error="Sorry this cell must be left blank" sqref="B6 B14">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Factor" error="Entered value not found in list of expected Factors. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." promptTitle="Factor for Observation's Value" prompt="Select the Factor or thing that the values in this column describe. _x000a_Selection from the offered list is HIGHLY recommended. " sqref="B16">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Factor" error="Entered value not found in list of expected Factors. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." promptTitle="Factor for Observation's Value" prompt="Select the Factor or thing that the values in this column describe. _x000a_Selection from the offered list is HIGHLY recommended. " sqref="B15">
       <formula1>INDIRECT(IF($B$2="Value","Factor","NotApplicable"))</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Derviation Factor" error="The Dervation Factor select was not found in the list. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." sqref="B18">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Derviation Factor" error="The Dervation Factor select was not found in the list. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." sqref="B17">
       <formula1>INDIRECT(IF($B$2="Value","DerivationFactor","NotApplicable"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data / Start Data" prompt="The data (and time) this observation was taken. Or if a time range the start data/ Time." sqref="B11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data / Start Data" prompt="The data (and time) this observation was taken. Or if a time range the start data/ Time." sqref="B10">
       <formula1>INDIRECT(IF($B$2="Value","Column","NotApplicable"))</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="End Data" prompt="The end date/time of the date/time this observation was taken. If left blank above date will be assumed to be a single point." sqref="B13"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Contirbutor" prompt="Person or Organisation that provided/ recorded/ measured the data." sqref="B14">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="End Data" prompt="The end date/time of the date/time this observation was taken. If left blank above date will be assumed to be a single point." sqref="B12"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Contirbutor" prompt="Person or Organisation that provided/ recorded/ measured the data." sqref="B13">
       <formula1>INDIRECT(IF(OR($B$2="Value",$B$2="Id"),"Column","NotApplicable"))</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected or Indirect Link" error="The linlk entered is not in the format of a link to data on the same page. Ignore this is you intended an external link." promptTitle="Survey" prompt="The column that contains the ID of the Survey for this Item. Enter &quot;row&quot; if the Survey has no ID column. Only applicable for columns with a &quot;Site&quot; category. " sqref="B10">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected or Indirect Link" error="The linlk entered is not in the format of a link to data on the same page. Ignore this is you intended an external link." promptTitle="Survey" prompt="The column that contains the ID of the Survey for this Item. Enter &quot;row&quot; if the Survey has no ID column. Only applicable for columns with a &quot;Site&quot; category. " sqref="B9">
       <formula1>INDIRECT(IF($B$2="Value","Column","NotApplicable"))</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Location for Site" prompt="The column that contains the ID of the Location for this Site. Enter &quot;row&quot; if the Location has no ID column. Only applicable for columns with a &quot;Site&quot; category. " sqref="B8">
+      <formula1>INDIRECT(IF($B$1="Site","Column","NotApplicable"))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="End Data" prompt="The end date/time of the date/time this observation was taken. If left blank above date will be assumed to be a single point." sqref="B11">
+      <formula1>INDIRECT(IF($B$2="Value","Column","NotApplicable"))</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Category" prompt="Please category this data will belong to. " sqref="B1">
+      <formula1>Category</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="&quot;Unexpected column reference&quot;" error="The link does not refer to a link on the same page. Please ignore this if you intended an external link." promptTitle="Site for Observation/Value" prompt="The column that contains the ID of the Site this Observation applies to. Enter &quot;row&quot; if the Site has no ID column. Only applicable for columns with Observation's &quot;value&quot; field." sqref="B7">
       <formula1>INDIRECT(IF(OR($B$2="Value"),"Column","NotApplicable"))</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="&quot;Unexpected column reference&quot;" promptTitle="Type of Link to the Site" prompt="Advance feature: The default (if left blank) is to associate the site as vocab:site. If a different vocab: is to be used enter it here." sqref="B8:C8"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Location for Site" prompt="The column that contains the ID of the Location for this Site. Enter &quot;row&quot; if the Location has no ID column. Only applicable for columns with a &quot;Site&quot; category. " sqref="B9">
-      <formula1>INDIRECT(IF($B$1="Site","Column","NotApplicable"))</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Ignore Zeros" prompt="If set to true any zeros in this column will be treated as nulls." sqref="B5">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="id/Value Column" prompt="The column that contains the ID/value of the Category this columns applies to. Enter &quot;row&quot; if the Category has no Id column. Not required for &quot;Id&quot; or Observation's &quot;value&quot; fields." sqref="B3">
       <formula1>INDIRECT(IF(OR($B$2="Id",$B$2="Value"),"NotApplicable","Column"))</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="End Data" prompt="The end date/time of the date/time this observation was taken. If left blank above date will be assumed to be a single point." sqref="B12">
-      <formula1>INDIRECT(IF($B$2="Value","Column","NotApplicable"))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2340,8 +2352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P258"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -2454,7 +2466,7 @@
     </row>
     <row r="3" spans="1:16" ht="15">
       <c r="A3" s="2" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>25</v>
@@ -2496,7 +2508,7 @@
     </row>
     <row r="4" spans="1:16" ht="15">
       <c r="A4" s="2" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
@@ -2637,7 +2649,7 @@
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="6" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="K7" s="2"/>
       <c r="N7" t="s">
@@ -2729,7 +2741,7 @@
         <v>38</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>15</v>
@@ -2754,7 +2766,7 @@
         <v>39</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>18</v>
@@ -2773,10 +2785,10 @@
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>409</v>
+        <v>445</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
@@ -2809,7 +2821,7 @@
         <v>33</v>
       </c>
       <c r="J14" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="K14" s="2"/>
       <c r="P14" t="s">
@@ -2857,7 +2869,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="5" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="K19" s="2"/>
       <c r="P19" t="s">
@@ -2912,7 +2924,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="K23" s="2"/>
       <c r="P23" t="s">
@@ -2937,7 +2949,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="5" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="K25" s="2"/>
       <c r="P25" t="s">
@@ -2989,7 +3001,7 @@
       </c>
       <c r="K29" s="2"/>
       <c r="P29" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15">
@@ -2999,7 +3011,7 @@
       </c>
       <c r="K30" s="2"/>
       <c r="P30" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15">
@@ -3009,7 +3021,7 @@
       </c>
       <c r="K31" s="2"/>
       <c r="P31" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15">
@@ -3019,7 +3031,7 @@
       </c>
       <c r="K32" s="2"/>
       <c r="P32" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="5:16" ht="15">
@@ -3029,7 +3041,7 @@
       </c>
       <c r="K33" s="2"/>
       <c r="P33" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="5:16" ht="15">
@@ -3039,7 +3051,7 @@
       </c>
       <c r="K34" s="2"/>
       <c r="P34" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="5:16" ht="15">
@@ -3049,17 +3061,17 @@
       </c>
       <c r="K35" s="2"/>
       <c r="P35" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="5:16" ht="15">
       <c r="E36" s="2"/>
       <c r="J36" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="K36" s="2"/>
       <c r="P36" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" spans="5:16" ht="15">
@@ -3069,7 +3081,7 @@
       </c>
       <c r="K37" s="2"/>
       <c r="P37" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="5:16" ht="15">
@@ -3079,7 +3091,7 @@
       </c>
       <c r="K38" s="2"/>
       <c r="P38" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="39" spans="5:16" ht="15">
@@ -3089,7 +3101,7 @@
       </c>
       <c r="K39" s="2"/>
       <c r="P39" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" spans="5:16" ht="15">
@@ -3098,7 +3110,7 @@
       </c>
       <c r="K40" s="2"/>
       <c r="P40" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="41" spans="5:16" ht="15">
@@ -3107,16 +3119,16 @@
       </c>
       <c r="K41" s="2"/>
       <c r="P41" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="5:16" ht="15">
       <c r="J42" s="2" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="K42" s="2"/>
       <c r="P42" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" spans="5:16" ht="15">
@@ -3125,7 +3137,7 @@
       </c>
       <c r="K43" s="2"/>
       <c r="P43" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" spans="5:16" ht="15">
@@ -3134,25 +3146,25 @@
       </c>
       <c r="K44" s="2"/>
       <c r="P44" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="45" spans="5:16" ht="15">
       <c r="J45" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="K45" s="2"/>
       <c r="P45" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="46" spans="5:16" ht="15">
       <c r="J46" s="6" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="K46" s="2"/>
       <c r="P46" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="5:16" ht="15">
@@ -3161,7 +3173,7 @@
       </c>
       <c r="K47" s="2"/>
       <c r="P47" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" spans="5:16" ht="15">
@@ -3169,7 +3181,7 @@
         <v>114</v>
       </c>
       <c r="P48" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="49" spans="10:16">
@@ -3177,7 +3189,7 @@
         <v>22</v>
       </c>
       <c r="P49" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50" spans="10:16" ht="15">
@@ -3185,7 +3197,7 @@
         <v>111</v>
       </c>
       <c r="P50" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="51" spans="10:16" ht="15">
@@ -3193,7 +3205,7 @@
         <v>115</v>
       </c>
       <c r="P51" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="52" spans="10:16" ht="15">
@@ -3201,7 +3213,7 @@
         <v>116</v>
       </c>
       <c r="P52" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="53" spans="10:16" ht="15">
@@ -3209,7 +3221,7 @@
         <v>117</v>
       </c>
       <c r="P53" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="54" spans="10:16" ht="15">
@@ -3217,7 +3229,7 @@
         <v>118</v>
       </c>
       <c r="P54" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="55" spans="10:16" ht="15">
@@ -3225,7 +3237,7 @@
         <v>120</v>
       </c>
       <c r="P55" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="56" spans="10:16" ht="15">
@@ -3233,7 +3245,7 @@
         <v>119</v>
       </c>
       <c r="P56" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="57" spans="10:16" ht="15">
@@ -3241,1012 +3253,1012 @@
         <v>121</v>
       </c>
       <c r="P57" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="58" spans="10:16">
       <c r="P58" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="59" spans="10:16">
       <c r="P59" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="60" spans="10:16">
       <c r="P60" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="61" spans="10:16">
       <c r="P61" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="62" spans="10:16">
       <c r="P62" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="63" spans="10:16">
       <c r="P63" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="64" spans="10:16">
       <c r="P64" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="65" spans="16:16">
       <c r="P65" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="66" spans="16:16">
       <c r="P66" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="67" spans="16:16">
       <c r="P67" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="68" spans="16:16">
       <c r="P68" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="16:16">
       <c r="P69" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="70" spans="16:16">
       <c r="P70" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71" spans="16:16">
       <c r="P71" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="72" spans="16:16">
       <c r="P72" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="73" spans="16:16">
       <c r="P73" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="74" spans="16:16">
       <c r="P74" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="75" spans="16:16">
       <c r="P75" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="76" spans="16:16">
       <c r="P76" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="77" spans="16:16">
       <c r="P77" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="78" spans="16:16">
       <c r="P78" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="79" spans="16:16">
       <c r="P79" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="80" spans="16:16">
       <c r="P80" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="81" spans="16:16">
       <c r="P81" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="82" spans="16:16">
       <c r="P82" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="83" spans="16:16">
       <c r="P83" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="84" spans="16:16">
       <c r="P84" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="85" spans="16:16">
       <c r="P85" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="86" spans="16:16">
       <c r="P86" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="87" spans="16:16">
       <c r="P87" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="88" spans="16:16">
       <c r="P88" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="89" spans="16:16">
       <c r="P89" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="90" spans="16:16">
       <c r="P90" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="91" spans="16:16">
       <c r="P91" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="92" spans="16:16">
       <c r="P92" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="93" spans="16:16">
       <c r="P93" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="94" spans="16:16">
       <c r="P94" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="95" spans="16:16">
       <c r="P95" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="96" spans="16:16">
       <c r="P96" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="97" spans="16:16">
       <c r="P97" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="98" spans="16:16">
       <c r="P98" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="99" spans="16:16">
       <c r="P99" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="100" spans="16:16">
       <c r="P100" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="101" spans="16:16">
       <c r="P101" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="102" spans="16:16">
       <c r="P102" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="103" spans="16:16">
       <c r="P103" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="104" spans="16:16">
       <c r="P104" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="105" spans="16:16">
       <c r="P105" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="106" spans="16:16">
       <c r="P106" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="107" spans="16:16">
       <c r="P107" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="108" spans="16:16">
       <c r="P108" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="109" spans="16:16">
       <c r="P109" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="110" spans="16:16">
       <c r="P110" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="111" spans="16:16">
       <c r="P111" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="112" spans="16:16">
       <c r="P112" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="113" spans="16:16">
       <c r="P113" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="114" spans="16:16">
       <c r="P114" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="115" spans="16:16">
       <c r="P115" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="116" spans="16:16">
       <c r="P116" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="117" spans="16:16">
       <c r="P117" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="118" spans="16:16">
       <c r="P118" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="119" spans="16:16">
       <c r="P119" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="120" spans="16:16">
       <c r="P120" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="121" spans="16:16">
       <c r="P121" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="122" spans="16:16">
       <c r="P122" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="123" spans="16:16">
       <c r="P123" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="124" spans="16:16">
       <c r="P124" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="125" spans="16:16">
       <c r="P125" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="126" spans="16:16">
       <c r="P126" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="127" spans="16:16">
       <c r="P127" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="128" spans="16:16">
       <c r="P128" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="129" spans="16:16">
       <c r="P129" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="130" spans="16:16">
       <c r="P130" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="131" spans="16:16">
       <c r="P131" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="132" spans="16:16">
       <c r="P132" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="133" spans="16:16">
       <c r="P133" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="134" spans="16:16">
       <c r="P134" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="135" spans="16:16">
       <c r="P135" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="136" spans="16:16">
       <c r="P136" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="137" spans="16:16">
       <c r="P137" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="138" spans="16:16">
       <c r="P138" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="139" spans="16:16">
       <c r="P139" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="140" spans="16:16">
       <c r="P140" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="141" spans="16:16">
       <c r="P141" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="142" spans="16:16">
       <c r="P142" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="143" spans="16:16">
       <c r="P143" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="144" spans="16:16">
       <c r="P144" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="145" spans="16:16">
       <c r="P145" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="146" spans="16:16">
       <c r="P146" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="147" spans="16:16">
       <c r="P147" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="148" spans="16:16">
       <c r="P148" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="149" spans="16:16">
       <c r="P149" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="150" spans="16:16">
       <c r="P150" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="151" spans="16:16">
       <c r="P151" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="152" spans="16:16">
       <c r="P152" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="153" spans="16:16">
       <c r="P153" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="154" spans="16:16">
       <c r="P154" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="155" spans="16:16">
       <c r="P155" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="156" spans="16:16">
       <c r="P156" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="157" spans="16:16">
       <c r="P157" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="158" spans="16:16">
       <c r="P158" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="159" spans="16:16">
       <c r="P159" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="160" spans="16:16">
       <c r="P160" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="161" spans="16:16">
       <c r="P161" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="162" spans="16:16">
       <c r="P162" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="163" spans="16:16">
       <c r="P163" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="164" spans="16:16">
       <c r="P164" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="165" spans="16:16">
       <c r="P165" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="166" spans="16:16">
       <c r="P166" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="167" spans="16:16">
       <c r="P167" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="168" spans="16:16">
       <c r="P168" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="169" spans="16:16">
       <c r="P169" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="170" spans="16:16">
       <c r="P170" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="171" spans="16:16">
       <c r="P171" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="172" spans="16:16">
       <c r="P172" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="173" spans="16:16">
       <c r="P173" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="174" spans="16:16">
       <c r="P174" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="175" spans="16:16">
       <c r="P175" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="176" spans="16:16">
       <c r="P176" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="177" spans="16:16">
       <c r="P177" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="178" spans="16:16">
       <c r="P178" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="179" spans="16:16">
       <c r="P179" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="180" spans="16:16">
       <c r="P180" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="181" spans="16:16">
       <c r="P181" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="182" spans="16:16">
       <c r="P182" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="183" spans="16:16">
       <c r="P183" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="184" spans="16:16">
       <c r="P184" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="185" spans="16:16">
       <c r="P185" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="186" spans="16:16">
       <c r="P186" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="187" spans="16:16">
       <c r="P187" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="188" spans="16:16">
       <c r="P188" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="189" spans="16:16">
       <c r="P189" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="190" spans="16:16">
       <c r="P190" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="191" spans="16:16">
       <c r="P191" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="192" spans="16:16">
       <c r="P192" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="193" spans="16:16">
       <c r="P193" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="194" spans="16:16">
       <c r="P194" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="195" spans="16:16">
       <c r="P195" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="196" spans="16:16">
       <c r="P196" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="197" spans="16:16">
       <c r="P197" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="198" spans="16:16">
       <c r="P198" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="199" spans="16:16">
       <c r="P199" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="200" spans="16:16">
       <c r="P200" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="201" spans="16:16">
       <c r="P201" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="202" spans="16:16">
       <c r="P202" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="203" spans="16:16">
       <c r="P203" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="204" spans="16:16">
       <c r="P204" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="205" spans="16:16">
       <c r="P205" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="206" spans="16:16">
       <c r="P206" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="207" spans="16:16">
       <c r="P207" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="208" spans="16:16">
       <c r="P208" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="209" spans="16:16">
       <c r="P209" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="210" spans="16:16">
       <c r="P210" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="211" spans="16:16">
       <c r="P211" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="212" spans="16:16">
       <c r="P212" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="213" spans="16:16">
       <c r="P213" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="214" spans="16:16">
       <c r="P214" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="215" spans="16:16">
       <c r="P215" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="216" spans="16:16">
       <c r="P216" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="217" spans="16:16">
       <c r="P217" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="218" spans="16:16">
       <c r="P218" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="219" spans="16:16">
       <c r="P219" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="220" spans="16:16">
       <c r="P220" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="221" spans="16:16">
       <c r="P221" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="222" spans="16:16">
       <c r="P222" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="223" spans="16:16">
       <c r="P223" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="224" spans="16:16">
       <c r="P224" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="225" spans="16:16">
       <c r="P225" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="226" spans="16:16">
       <c r="P226" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="227" spans="16:16">
       <c r="P227" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="228" spans="16:16">
       <c r="P228" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="229" spans="16:16">
       <c r="P229" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="230" spans="16:16">
       <c r="P230" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="231" spans="16:16">
       <c r="P231" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="232" spans="16:16">
       <c r="P232" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="233" spans="16:16">
       <c r="P233" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="234" spans="16:16">
       <c r="P234" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="235" spans="16:16">
       <c r="P235" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="236" spans="16:16">
       <c r="P236" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="237" spans="16:16">
       <c r="P237" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="238" spans="16:16">
       <c r="P238" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="239" spans="16:16">
       <c r="P239" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="240" spans="16:16">
       <c r="P240" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="241" spans="16:16">
       <c r="P241" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="242" spans="16:16">
       <c r="P242" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="243" spans="16:16">
       <c r="P243" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="244" spans="16:16">
       <c r="P244" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="245" spans="16:16">
       <c r="P245" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="246" spans="16:16">
       <c r="P246" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="247" spans="16:16">
       <c r="P247" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="248" spans="16:16">
       <c r="P248" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="249" spans="16:16">
       <c r="P249" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="250" spans="16:16">
       <c r="P250" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="251" spans="16:16">
       <c r="P251" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="252" spans="16:16">
       <c r="P252" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="253" spans="16:16">
       <c r="P253" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="254" spans="16:16">
       <c r="P254" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="255" spans="16:16">
       <c r="P255" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="256" spans="16:16">
       <c r="P256" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="257" spans="16:16">
       <c r="P257" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="258" spans="16:16">
       <c r="P258" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
   </sheetData>
@@ -4268,15 +4280,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Links used a lot less often. Site and  Location to be auto added.
</commit_message>
<xml_diff>
--- a/data/MetaMaster.xlsx
+++ b/data/MetaMaster.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="423">
   <si>
     <t>Easting</t>
   </si>
@@ -278,12 +278,6 @@
     <t>Id/Value Column (or "Row")</t>
   </si>
   <si>
-    <t>Date/Start Date</t>
-  </si>
-  <si>
-    <t>End Date (if Applicable)</t>
-  </si>
-  <si>
     <t>ALLUVIAL</t>
   </si>
   <si>
@@ -434,15 +428,9 @@
     <t>Raw Data</t>
   </si>
   <si>
-    <t>Contirubutor</t>
-  </si>
-  <si>
     <t>-- Constants --</t>
   </si>
   <si>
-    <t>-- Links --</t>
-  </si>
-  <si>
     <t>row</t>
   </si>
   <si>
@@ -482,33 +470,15 @@
     <t>The column that contains the ID/value of the Category this columns applies to. Enter "row" if the Category has no Id column. Not required for "Id" or Observation's "value" fields.</t>
   </si>
   <si>
-    <t>Site for Observation/Value</t>
-  </si>
-  <si>
-    <t>The column that contains the ID of the Site this Observation applies to. Enter "row" if the Site has no ID column. Only applicable for columns with Observation's "value" field.</t>
-  </si>
-  <si>
-    <t>Location for Site</t>
-  </si>
-  <si>
     <t>Factor for Observation's Value</t>
   </si>
   <si>
     <t>Unit for Observation's Value</t>
   </si>
   <si>
-    <t>Data / Start Data</t>
-  </si>
-  <si>
     <t>Derivation Factor for Observation</t>
   </si>
   <si>
-    <t>End Data</t>
-  </si>
-  <si>
-    <t>Contirbutor</t>
-  </si>
-  <si>
     <t>STOP</t>
   </si>
   <si>
@@ -530,9 +500,6 @@
     <t>Please select a value from the list or contact an Admin to explain why a different value is required.</t>
   </si>
   <si>
-    <t>Not a direct value</t>
-  </si>
-  <si>
     <t>Unexpected Factor</t>
   </si>
   <si>
@@ -1265,18 +1232,6 @@
     <t>Header</t>
   </si>
   <si>
-    <t>Add a remark to this Subject. To use the value of another column enter !column</t>
-  </si>
-  <si>
-    <t>Person or Organisation that provided/ recorded/ measured the data.  To use the value of another column enter !column</t>
-  </si>
-  <si>
-    <t>The end date/time of the date/time this observation was taken. If left blank above date will be assumed to be a single point.  To use the value of another column enter !column</t>
-  </si>
-  <si>
-    <t>The data (and time) this observation was taken. Or if a time range the start data/ Time.  To use the value of another column enter !column</t>
-  </si>
-  <si>
     <t>Select "raw data" or the way that multiple data values where combined.  To use the value of another column enter !column</t>
   </si>
   <si>
@@ -1298,15 +1253,6 @@
     <t>Lifeform</t>
   </si>
   <si>
-    <t xml:space="preserve">The column that contains the ID of the Location for this Site. Enter "row" if the Location has no ID column. Start Constants with =. Only applicable for columns with a "Site" category. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The column that contains the ID of the Survey for this Item. Enter "row" if the Survey has no ID column. Start constants with an =. Only applicable for columns with a "Value" field. </t>
-  </si>
-  <si>
-    <t>You entered a vlaue which is not a lookup value. Constants must start with an = symbol. Any other value will cause an error.</t>
-  </si>
-  <si>
     <t>Entered value not found in list of expected Factors. Any other value will need to be added to the global accepted list.</t>
   </si>
   <si>
@@ -1344,21 +1290,6 @@
   </si>
   <si>
     <t>INDIRECT(SUBSTITUTE($B$1," ","_"))</t>
-  </si>
-  <si>
-    <t>INDIRECT(IF(OR($B$2="Value"),"Column","NotApplicable"))</t>
-  </si>
-  <si>
-    <t>INDIRECT(IF($B$1="Site","Column","NotApplicable"))</t>
-  </si>
-  <si>
-    <t>INDIRECT(IF($B$2="Value","Column","NotApplicable"))</t>
-  </si>
-  <si>
-    <t>INDIRECT(IF(OR($B$2="Value",A$2="Id"),"Column","NotApplicable"))</t>
-  </si>
-  <si>
-    <t>INDIRECT(IF(OR($B$2="Value",$B$2="Id"),"Column","NotApplicable"))</t>
   </si>
   <si>
     <t>INDIRECT(IF($B$2="Value","Factor","NotApplicable"))</t>
@@ -1851,13 +1782,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z127"/>
+  <dimension ref="A1:Z119"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="21" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="13" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12"/>
@@ -1870,7 +1801,7 @@
     <col min="6" max="7" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1884,19 +1815,19 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="G1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="H1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1904,397 +1835,213 @@
         <v>35</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>433</v>
+        <v>415</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F2" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="G2" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="H2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
       <c r="A3" t="s">
         <v>77</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
       <c r="D3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" t="s">
         <v>145</v>
       </c>
-      <c r="F3" t="s">
-        <v>155</v>
-      </c>
       <c r="G3" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="H3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="E4" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D5" t="s">
+        <v>392</v>
+      </c>
+      <c r="E5" t="s">
+        <v>393</v>
+      </c>
+      <c r="F5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G5" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" t="s">
+        <v>419</v>
+      </c>
+      <c r="F6" t="s">
+        <v>145</v>
+      </c>
+      <c r="G6" t="s">
+        <v>420</v>
+      </c>
+      <c r="H6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E7" t="s">
+        <v>398</v>
+      </c>
+      <c r="F7" t="s">
+        <v>404</v>
+      </c>
+      <c r="G7" t="s">
+        <v>152</v>
+      </c>
+      <c r="H7" t="s">
         <v>403</v>
       </c>
-      <c r="E5" t="s">
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E8" t="s">
+        <v>397</v>
+      </c>
+      <c r="F8" t="s">
         <v>404</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G8" t="s">
+        <v>153</v>
+      </c>
+      <c r="H8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="D9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E9" t="s">
+        <v>396</v>
+      </c>
+      <c r="F9" t="s">
+        <v>404</v>
+      </c>
+      <c r="G9" t="s">
         <v>155</v>
       </c>
-      <c r="G5" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C6" t="s">
-        <v>442</v>
-      </c>
-      <c r="F6" t="s">
-        <v>155</v>
-      </c>
-      <c r="G6" t="s">
-        <v>443</v>
-      </c>
-      <c r="H6" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="D7" t="s">
-        <v>146</v>
-      </c>
-      <c r="E7" t="s">
-        <v>147</v>
-      </c>
-      <c r="F7" t="s">
-        <v>422</v>
-      </c>
-      <c r="G7" t="s">
-        <v>162</v>
-      </c>
-      <c r="H7" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="D8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E8" t="s">
-        <v>418</v>
-      </c>
-      <c r="F8" t="s">
-        <v>422</v>
-      </c>
-      <c r="G8" t="s">
-        <v>162</v>
-      </c>
-      <c r="H8" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" t="s">
-        <v>135</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="D9" t="s">
-        <v>135</v>
-      </c>
-      <c r="E9" t="s">
-        <v>419</v>
-      </c>
-      <c r="F9" t="s">
-        <v>422</v>
-      </c>
-      <c r="G9" t="s">
-        <v>162</v>
-      </c>
       <c r="H9" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="F10" t="s">
-        <v>422</v>
-      </c>
-      <c r="G10" t="s">
-        <v>162</v>
-      </c>
-      <c r="H10" t="s">
-        <v>420</v>
-      </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="D11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E11" t="s">
-        <v>409</v>
-      </c>
-      <c r="F11" t="s">
-        <v>422</v>
-      </c>
-      <c r="G11" t="s">
-        <v>162</v>
-      </c>
-      <c r="H11" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="D12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" t="s">
-        <v>407</v>
-      </c>
-      <c r="F12" t="s">
-        <v>422</v>
-      </c>
-      <c r="G12" t="s">
-        <v>162</v>
-      </c>
-      <c r="H12" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" t="s">
-        <v>130</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>438</v>
-      </c>
-      <c r="D13" t="s">
-        <v>154</v>
-      </c>
-      <c r="E13" t="s">
-        <v>408</v>
-      </c>
-      <c r="F13" t="s">
-        <v>422</v>
-      </c>
-      <c r="G13" t="s">
-        <v>162</v>
-      </c>
-      <c r="H13" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C14" t="s">
-        <v>442</v>
-      </c>
-      <c r="F14" t="s">
-        <v>155</v>
-      </c>
-      <c r="G14" t="s">
-        <v>443</v>
-      </c>
-      <c r="H14" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+    </row>
+    <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>439</v>
-      </c>
-      <c r="D15" t="s">
-        <v>149</v>
-      </c>
-      <c r="E15" t="s">
-        <v>413</v>
-      </c>
-      <c r="F15" t="s">
-        <v>422</v>
-      </c>
-      <c r="G15" t="s">
-        <v>163</v>
-      </c>
-      <c r="H15" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>440</v>
-      </c>
-      <c r="D16" t="s">
-        <v>150</v>
-      </c>
-      <c r="E16" t="s">
-        <v>412</v>
-      </c>
-      <c r="F16" t="s">
-        <v>422</v>
-      </c>
-      <c r="G16" t="s">
-        <v>164</v>
-      </c>
-      <c r="H16" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>441</v>
-      </c>
-      <c r="D17" t="s">
-        <v>152</v>
-      </c>
-      <c r="E17" t="s">
-        <v>411</v>
-      </c>
-      <c r="F17" t="s">
-        <v>422</v>
-      </c>
-      <c r="G17" t="s">
-        <v>166</v>
-      </c>
-      <c r="H17" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26">
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
-      <c r="Z18" s="3"/>
-    </row>
-    <row r="23" spans="1:26">
-      <c r="A23" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26">
-      <c r="A24">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:26">
-      <c r="A25">
+    <row r="17" spans="1:3">
+      <c r="A17">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:26">
-      <c r="A26">
+    <row r="18" spans="1:3">
+      <c r="A18">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:26">
-      <c r="C31" s="4"/>
-    </row>
-    <row r="127" spans="14:14">
-      <c r="N127" s="1"/>
+    <row r="23" spans="1:3">
+      <c r="C23" s="4"/>
+    </row>
+    <row r="119" spans="14:14">
+      <c r="N119" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations xWindow="284" yWindow="481" count="16">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Unit." error="The Unit provided was not in the list. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." promptTitle="Unit for Observation's Value" prompt="Please describe the Unit the values are in. Whenever possible pick a value from the list." sqref="B16">
+  <dataValidations xWindow="284" yWindow="481" count="9">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Unit." error="The Unit provided was not in the list. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." promptTitle="Unit for Observation's Value" prompt="Please describe the Unit the values are in. Whenever possible pick a value from the list." sqref="B8">
       <formula1>"INDIRECT(IF(ISNA(VLOOKUP($B$2,FeildsThatNeedUnit,1,FALSE)),""NotApplicable"",""UNIT""))"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Feild Value" error="Sorry Feild value input does not match the expected feilds for the category you picked.  Only add and unexpected feild if you are sure no Category and Feild combination matches ths column. You may have to explain this!" promptTitle="Field" prompt="Please Select the feild that data in this column belongs to. Options available depend on the Category selected above." sqref="B2">
@@ -2303,37 +2050,18 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="id/Value Column" prompt="The column that contains the ID/value of the Category this columns applies to. Enter &quot;row&quot; if the Category has no Id column. Not required for &quot;Id&quot; or Observation's &quot;value&quot; fields." sqref="B4">
       <formula1>INDIRECT(IF(OR(B3="Id",B3="Value"),"NotApplicable"+"Column","Column"))</formula1>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="No Values Allow" error="Sorry this cell must be left blank" sqref="B6 B14">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="No Values Allow" error="Sorry this cell must be left blank" sqref="B6">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Factor" error="Entered value not found in list of expected Factors. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." promptTitle="Factor for Observation's Value" prompt="Select the Factor or thing that the values in this column describe. _x000a_Selection from the offered list is HIGHLY recommended. " sqref="B15">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Factor" error="Entered value not found in list of expected Factors. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." promptTitle="Factor for Observation's Value" prompt="Select the Factor or thing that the values in this column describe. _x000a_Selection from the offered list is HIGHLY recommended. " sqref="B7">
       <formula1>INDIRECT(IF($B$2="Value","Factor","NotApplicable"))</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Derviation Factor" error="The Dervation Factor select was not found in the list. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." sqref="B17">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Derviation Factor" error="The Dervation Factor select was not found in the list. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." sqref="B9">
       <formula1>INDIRECT(IF($B$2="Value","DerivationFactor","NotApplicable"))</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data / Start Data" prompt="The data (and time) this observation was taken. Or if a time range the start data/ Time." sqref="B10">
-      <formula1>INDIRECT(IF($B$2="Value","Column","NotApplicable"))</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="End Data" prompt="The end date/time of the date/time this observation was taken. If left blank above date will be assumed to be a single point." sqref="B12"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Contirbutor" prompt="Person or Organisation that provided/ recorded/ measured the data." sqref="B13">
-      <formula1>INDIRECT(IF(OR($B$2="Value",$B$2="Id"),"Column","NotApplicable"))</formula1>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected or Indirect Link" error="The linlk entered is not in the format of a link to data on the same page. Ignore this is you intended an external link." promptTitle="Survey" prompt="The column that contains the ID of the Survey for this Item. Enter &quot;row&quot; if the Survey has no ID column. Only applicable for columns with a &quot;Site&quot; category. " sqref="B9">
-      <formula1>INDIRECT(IF($B$2="Value","Column","NotApplicable"))</formula1>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Location for Site" prompt="The column that contains the ID of the Location for this Site. Enter &quot;row&quot; if the Location has no ID column. Only applicable for columns with a &quot;Site&quot; category. " sqref="B8">
-      <formula1>INDIRECT(IF($B$1="Site","Column","NotApplicable"))</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="End Data" prompt="The end date/time of the date/time this observation was taken. If left blank above date will be assumed to be a single point." sqref="B11">
-      <formula1>INDIRECT(IF($B$2="Value","Column","NotApplicable"))</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Category" prompt="Please category this data will belong to. " sqref="B1">
       <formula1>Category</formula1>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="&quot;Unexpected column reference&quot;" error="The link does not refer to a link on the same page. Please ignore this if you intended an external link." promptTitle="Site for Observation/Value" prompt="The column that contains the ID of the Site this Observation applies to. Enter &quot;row&quot; if the Site has no ID column. Only applicable for columns with Observation's &quot;value&quot; field." sqref="B7">
-      <formula1>INDIRECT(IF(OR($B$2="Value"),"Column","NotApplicable"))</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Ignore Zeros" prompt="If set to true any zeros in this column will be treated as nulls." sqref="B5">
       <formula1>"TRUE,FALSE"</formula1>
@@ -2353,7 +2081,7 @@
   <dimension ref="A1:P258"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -2373,7 +2101,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C1" t="s">
         <v>19</v>
@@ -2391,7 +2119,7 @@
         <v>22</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2" t="s">
@@ -2443,10 +2171,10 @@
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>30</v>
@@ -2455,18 +2183,18 @@
         <v>42</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>35</v>
       </c>
       <c r="P2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15">
       <c r="A3" s="2" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>25</v>
@@ -2491,10 +2219,10 @@
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N3" t="s">
         <v>46</v>
@@ -2508,7 +2236,7 @@
     </row>
     <row r="4" spans="1:16" ht="15">
       <c r="A4" s="2" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
@@ -2533,10 +2261,10 @@
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="N4" t="s">
         <v>47</v>
@@ -2574,13 +2302,13 @@
         <v>41</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="P5" t="s">
         <v>53</v>
@@ -2613,10 +2341,10 @@
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>44</v>
@@ -2638,18 +2366,18 @@
       <c r="E7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>19</v>
+      <c r="F7" t="s">
+        <v>130</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="6" t="s">
-        <v>430</v>
+        <v>412</v>
       </c>
       <c r="K7" s="2"/>
       <c r="N7" t="s">
@@ -2670,10 +2398,10 @@
         <v>7</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>10</v>
@@ -2683,11 +2411,11 @@
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K8" s="2"/>
       <c r="N8" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="P8" t="s">
         <v>56</v>
@@ -2706,8 +2434,8 @@
       <c r="E9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>135</v>
+      <c r="F9" t="s">
+        <v>133</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>9</v>
@@ -2717,7 +2445,7 @@
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K9" s="2"/>
       <c r="N9" t="s">
@@ -2740,18 +2468,18 @@
       <c r="E10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>414</v>
+      <c r="F10" t="s">
+        <v>131</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K10" s="2"/>
       <c r="P10" t="s">
@@ -2765,15 +2493,15 @@
       <c r="E11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>415</v>
+      <c r="F11" t="s">
+        <v>399</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K11" s="2"/>
       <c r="P11" t="s">
@@ -2784,15 +2512,15 @@
       <c r="C12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>445</v>
+      <c r="F12" t="s">
+        <v>400</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K12" s="2"/>
       <c r="P12" t="s">
@@ -2803,13 +2531,16 @@
       <c r="C13" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="F13" t="s">
+        <v>422</v>
+      </c>
       <c r="G13" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K13" s="2"/>
       <c r="P13" t="s">
@@ -2821,7 +2552,7 @@
         <v>33</v>
       </c>
       <c r="J14" t="s">
-        <v>426</v>
+        <v>408</v>
       </c>
       <c r="K14" s="2"/>
       <c r="P14" t="s">
@@ -2830,7 +2561,7 @@
     </row>
     <row r="15" spans="1:16" ht="15">
       <c r="J15" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K15" s="2"/>
       <c r="P15" t="s">
@@ -2839,7 +2570,7 @@
     </row>
     <row r="16" spans="1:16" ht="15">
       <c r="J16" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K16" s="2"/>
       <c r="P16" t="s">
@@ -2848,7 +2579,7 @@
     </row>
     <row r="17" spans="1:16" ht="15">
       <c r="J17" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K17" s="2"/>
       <c r="P17" t="s">
@@ -2857,7 +2588,7 @@
     </row>
     <row r="18" spans="1:16" ht="15">
       <c r="J18" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K18" s="2"/>
       <c r="P18" t="s">
@@ -2869,7 +2600,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="5" t="s">
-        <v>428</v>
+        <v>410</v>
       </c>
       <c r="K19" s="2"/>
       <c r="P19" t="s">
@@ -2895,7 +2626,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K21" s="2"/>
       <c r="P21" t="s">
@@ -2911,7 +2642,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K22" s="2"/>
       <c r="P22" t="s">
@@ -2924,7 +2655,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2" t="s">
-        <v>424</v>
+        <v>406</v>
       </c>
       <c r="K23" s="2"/>
       <c r="P23" t="s">
@@ -2936,7 +2667,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K24" s="2"/>
       <c r="P24" t="s">
@@ -2949,7 +2680,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="5" t="s">
-        <v>429</v>
+        <v>411</v>
       </c>
       <c r="K25" s="2"/>
       <c r="P25" t="s">
@@ -2975,7 +2706,7 @@
     <row r="27" spans="1:16" ht="15">
       <c r="E27" s="2"/>
       <c r="J27" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K27" s="2"/>
       <c r="P27" t="s">
@@ -2985,7 +2716,7 @@
     <row r="28" spans="1:16" ht="15">
       <c r="E28" s="2"/>
       <c r="J28" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K28" s="2"/>
       <c r="P28" t="s">
@@ -2997,51 +2728,51 @@
       <c r="B29" s="2"/>
       <c r="E29" s="2"/>
       <c r="J29" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K29" s="2"/>
       <c r="P29" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15">
       <c r="E30" s="2"/>
       <c r="J30" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K30" s="2"/>
       <c r="P30" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15">
       <c r="E31" s="2"/>
       <c r="J31" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K31" s="2"/>
       <c r="P31" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15">
       <c r="E32" s="2"/>
       <c r="J32" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K32" s="2"/>
       <c r="P32" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="5:16" ht="15">
       <c r="E33" s="2"/>
       <c r="J33" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K33" s="2"/>
       <c r="P33" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="5:16" ht="15">
@@ -3051,7 +2782,7 @@
       </c>
       <c r="K34" s="2"/>
       <c r="P34" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="5:16" ht="15">
@@ -3061,127 +2792,127 @@
       </c>
       <c r="K35" s="2"/>
       <c r="P35" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="5:16" ht="15">
       <c r="E36" s="2"/>
       <c r="J36" t="s">
-        <v>423</v>
+        <v>405</v>
       </c>
       <c r="K36" s="2"/>
       <c r="P36" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="5:16" ht="15">
       <c r="E37" s="2"/>
       <c r="J37" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K37" s="2"/>
       <c r="P37" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" spans="5:16" ht="15">
       <c r="E38" s="2"/>
       <c r="J38" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K38" s="2"/>
       <c r="P38" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="5:16" ht="15">
       <c r="E39" s="2"/>
       <c r="J39" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K39" s="2"/>
       <c r="P39" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="5:16" ht="15">
       <c r="J40" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K40" s="2"/>
       <c r="P40" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="5:16" ht="15">
       <c r="J41" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K41" s="2"/>
       <c r="P41" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42" spans="5:16" ht="15">
       <c r="J42" s="2" t="s">
-        <v>425</v>
+        <v>407</v>
       </c>
       <c r="K42" s="2"/>
       <c r="P42" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="5:16" ht="15">
       <c r="J43" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K43" s="2"/>
       <c r="P43" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" spans="5:16" ht="15">
       <c r="J44" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K44" s="2"/>
       <c r="P44" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="5:16" ht="15">
       <c r="J45" t="s">
-        <v>427</v>
+        <v>409</v>
       </c>
       <c r="K45" s="2"/>
       <c r="P45" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="5:16" ht="15">
       <c r="J46" s="6" t="s">
-        <v>431</v>
+        <v>413</v>
       </c>
       <c r="K46" s="2"/>
       <c r="P46" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
     <row r="47" spans="5:16" ht="15">
       <c r="J47" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K47" s="2"/>
       <c r="P47" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="5:16" ht="15">
       <c r="J48" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="P48" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="49" spans="10:16">
@@ -3189,1076 +2920,1076 @@
         <v>22</v>
       </c>
       <c r="P49" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="10:16" ht="15">
       <c r="J50" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P50" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
     <row r="51" spans="10:16" ht="15">
       <c r="J51" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P51" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52" spans="10:16" ht="15">
       <c r="J52" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="P52" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="10:16" ht="15">
       <c r="J53" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="P53" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="54" spans="10:16" ht="15">
       <c r="J54" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="P54" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="55" spans="10:16" ht="15">
       <c r="J55" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="P55" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="56" spans="10:16" ht="15">
       <c r="J56" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="P56" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="57" spans="10:16" ht="15">
       <c r="J57" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="P57" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="58" spans="10:16">
       <c r="P58" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="59" spans="10:16">
       <c r="P59" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="60" spans="10:16">
       <c r="P60" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="61" spans="10:16">
       <c r="P61" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
     </row>
     <row r="62" spans="10:16">
       <c r="P62" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="63" spans="10:16">
       <c r="P63" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="64" spans="10:16">
       <c r="P64" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
     </row>
     <row r="65" spans="16:16">
       <c r="P65" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
     </row>
     <row r="66" spans="16:16">
       <c r="P66" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="67" spans="16:16">
       <c r="P67" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="68" spans="16:16">
       <c r="P68" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
     </row>
     <row r="69" spans="16:16">
       <c r="P69" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="70" spans="16:16">
       <c r="P70" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="71" spans="16:16">
       <c r="P71" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
     </row>
     <row r="72" spans="16:16">
       <c r="P72" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="73" spans="16:16">
       <c r="P73" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
     </row>
     <row r="74" spans="16:16">
       <c r="P74" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
     </row>
     <row r="75" spans="16:16">
       <c r="P75" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
     </row>
     <row r="76" spans="16:16">
       <c r="P76" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
     </row>
     <row r="77" spans="16:16">
       <c r="P77" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
     </row>
     <row r="78" spans="16:16">
       <c r="P78" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
     </row>
     <row r="79" spans="16:16">
       <c r="P79" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="80" spans="16:16">
       <c r="P80" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
     <row r="81" spans="16:16">
       <c r="P81" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
     </row>
     <row r="82" spans="16:16">
       <c r="P82" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
     </row>
     <row r="83" spans="16:16">
       <c r="P83" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="84" spans="16:16">
       <c r="P84" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="85" spans="16:16">
       <c r="P85" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="86" spans="16:16">
       <c r="P86" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
     </row>
     <row r="87" spans="16:16">
       <c r="P87" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
     </row>
     <row r="88" spans="16:16">
       <c r="P88" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
     </row>
     <row r="89" spans="16:16">
       <c r="P89" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
     <row r="90" spans="16:16">
       <c r="P90" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
     </row>
     <row r="91" spans="16:16">
       <c r="P91" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
     </row>
     <row r="92" spans="16:16">
       <c r="P92" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
     </row>
     <row r="93" spans="16:16">
       <c r="P93" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
     </row>
     <row r="94" spans="16:16">
       <c r="P94" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
     </row>
     <row r="95" spans="16:16">
       <c r="P95" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
     </row>
     <row r="96" spans="16:16">
       <c r="P96" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
     </row>
     <row r="97" spans="16:16">
       <c r="P97" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
     </row>
     <row r="98" spans="16:16">
       <c r="P98" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
     </row>
     <row r="99" spans="16:16">
       <c r="P99" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
     </row>
     <row r="100" spans="16:16">
       <c r="P100" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
     </row>
     <row r="101" spans="16:16">
       <c r="P101" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
     </row>
     <row r="102" spans="16:16">
       <c r="P102" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
     </row>
     <row r="103" spans="16:16">
       <c r="P103" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
     </row>
     <row r="104" spans="16:16">
       <c r="P104" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
     </row>
     <row r="105" spans="16:16">
       <c r="P105" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
     </row>
     <row r="106" spans="16:16">
       <c r="P106" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
     </row>
     <row r="107" spans="16:16">
       <c r="P107" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
     </row>
     <row r="108" spans="16:16">
       <c r="P108" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
     </row>
     <row r="109" spans="16:16">
       <c r="P109" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
     </row>
     <row r="110" spans="16:16">
       <c r="P110" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
     </row>
     <row r="111" spans="16:16">
       <c r="P111" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
     </row>
     <row r="112" spans="16:16">
       <c r="P112" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
     </row>
     <row r="113" spans="16:16">
       <c r="P113" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
     </row>
     <row r="114" spans="16:16">
       <c r="P114" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
     </row>
     <row r="115" spans="16:16">
       <c r="P115" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
     </row>
     <row r="116" spans="16:16">
       <c r="P116" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
     </row>
     <row r="117" spans="16:16">
       <c r="P117" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="118" spans="16:16">
       <c r="P118" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
     </row>
     <row r="119" spans="16:16">
       <c r="P119" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
     </row>
     <row r="120" spans="16:16">
       <c r="P120" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
     </row>
     <row r="121" spans="16:16">
       <c r="P121" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
     </row>
     <row r="122" spans="16:16">
       <c r="P122" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
     </row>
     <row r="123" spans="16:16">
       <c r="P123" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
     </row>
     <row r="124" spans="16:16">
       <c r="P124" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
     </row>
     <row r="125" spans="16:16">
       <c r="P125" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
     </row>
     <row r="126" spans="16:16">
       <c r="P126" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
     </row>
     <row r="127" spans="16:16">
       <c r="P127" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
     </row>
     <row r="128" spans="16:16">
       <c r="P128" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="129" spans="16:16">
       <c r="P129" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="130" spans="16:16">
       <c r="P130" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
     </row>
     <row r="131" spans="16:16">
       <c r="P131" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
     </row>
     <row r="132" spans="16:16">
       <c r="P132" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
     </row>
     <row r="133" spans="16:16">
       <c r="P133" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
     </row>
     <row r="134" spans="16:16">
       <c r="P134" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
     </row>
     <row r="135" spans="16:16">
       <c r="P135" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
     </row>
     <row r="136" spans="16:16">
       <c r="P136" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
     </row>
     <row r="137" spans="16:16">
       <c r="P137" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
     </row>
     <row r="138" spans="16:16">
       <c r="P138" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="139" spans="16:16">
       <c r="P139" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
     </row>
     <row r="140" spans="16:16">
       <c r="P140" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
     </row>
     <row r="141" spans="16:16">
       <c r="P141" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
     </row>
     <row r="142" spans="16:16">
       <c r="P142" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
     </row>
     <row r="143" spans="16:16">
       <c r="P143" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
     </row>
     <row r="144" spans="16:16">
       <c r="P144" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
     </row>
     <row r="145" spans="16:16">
       <c r="P145" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
     </row>
     <row r="146" spans="16:16">
       <c r="P146" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
     </row>
     <row r="147" spans="16:16">
       <c r="P147" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
     </row>
     <row r="148" spans="16:16">
       <c r="P148" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
     </row>
     <row r="149" spans="16:16">
       <c r="P149" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
     </row>
     <row r="150" spans="16:16">
       <c r="P150" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
     </row>
     <row r="151" spans="16:16">
       <c r="P151" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
     </row>
     <row r="152" spans="16:16">
       <c r="P152" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
     </row>
     <row r="153" spans="16:16">
       <c r="P153" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
     </row>
     <row r="154" spans="16:16">
       <c r="P154" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
     </row>
     <row r="155" spans="16:16">
       <c r="P155" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
     </row>
     <row r="156" spans="16:16">
       <c r="P156" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
     </row>
     <row r="157" spans="16:16">
       <c r="P157" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
     </row>
     <row r="158" spans="16:16">
       <c r="P158" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
     </row>
     <row r="159" spans="16:16">
       <c r="P159" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
     </row>
     <row r="160" spans="16:16">
       <c r="P160" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
     </row>
     <row r="161" spans="16:16">
       <c r="P161" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
     </row>
     <row r="162" spans="16:16">
       <c r="P162" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
     </row>
     <row r="163" spans="16:16">
       <c r="P163" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
     </row>
     <row r="164" spans="16:16">
       <c r="P164" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
     </row>
     <row r="165" spans="16:16">
       <c r="P165" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
     </row>
     <row r="166" spans="16:16">
       <c r="P166" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
     </row>
     <row r="167" spans="16:16">
       <c r="P167" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
     </row>
     <row r="168" spans="16:16">
       <c r="P168" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
     </row>
     <row r="169" spans="16:16">
       <c r="P169" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="170" spans="16:16">
       <c r="P170" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
     </row>
     <row r="171" spans="16:16">
       <c r="P171" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
     </row>
     <row r="172" spans="16:16">
       <c r="P172" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
     </row>
     <row r="173" spans="16:16">
       <c r="P173" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
     </row>
     <row r="174" spans="16:16">
       <c r="P174" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="175" spans="16:16">
       <c r="P175" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
     </row>
     <row r="176" spans="16:16">
       <c r="P176" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
     </row>
     <row r="177" spans="16:16">
       <c r="P177" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
     </row>
     <row r="178" spans="16:16">
       <c r="P178" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
     <row r="179" spans="16:16">
       <c r="P179" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
     </row>
     <row r="180" spans="16:16">
       <c r="P180" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
     </row>
     <row r="181" spans="16:16">
       <c r="P181" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
     </row>
     <row r="182" spans="16:16">
       <c r="P182" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="183" spans="16:16">
       <c r="P183" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
     </row>
     <row r="184" spans="16:16">
       <c r="P184" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
     </row>
     <row r="185" spans="16:16">
       <c r="P185" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
     </row>
     <row r="186" spans="16:16">
       <c r="P186" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
     </row>
     <row r="187" spans="16:16">
       <c r="P187" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
     </row>
     <row r="188" spans="16:16">
       <c r="P188" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
     </row>
     <row r="189" spans="16:16">
       <c r="P189" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
     </row>
     <row r="190" spans="16:16">
       <c r="P190" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
     </row>
     <row r="191" spans="16:16">
       <c r="P191" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
     </row>
     <row r="192" spans="16:16">
       <c r="P192" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
     </row>
     <row r="193" spans="16:16">
       <c r="P193" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
     </row>
     <row r="194" spans="16:16">
       <c r="P194" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
     </row>
     <row r="195" spans="16:16">
       <c r="P195" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
     </row>
     <row r="196" spans="16:16">
       <c r="P196" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
     </row>
     <row r="197" spans="16:16">
       <c r="P197" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
     <row r="198" spans="16:16">
       <c r="P198" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
     </row>
     <row r="199" spans="16:16">
       <c r="P199" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
     </row>
     <row r="200" spans="16:16">
       <c r="P200" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
     </row>
     <row r="201" spans="16:16">
       <c r="P201" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
     </row>
     <row r="202" spans="16:16">
       <c r="P202" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
     </row>
     <row r="203" spans="16:16">
       <c r="P203" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
     </row>
     <row r="204" spans="16:16">
       <c r="P204" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
     </row>
     <row r="205" spans="16:16">
       <c r="P205" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="206" spans="16:16">
       <c r="P206" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
     </row>
     <row r="207" spans="16:16">
       <c r="P207" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
     </row>
     <row r="208" spans="16:16">
       <c r="P208" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
     </row>
     <row r="209" spans="16:16">
       <c r="P209" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
     </row>
     <row r="210" spans="16:16">
       <c r="P210" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
     </row>
     <row r="211" spans="16:16">
       <c r="P211" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
     </row>
     <row r="212" spans="16:16">
       <c r="P212" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
     </row>
     <row r="213" spans="16:16">
       <c r="P213" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
     </row>
     <row r="214" spans="16:16">
       <c r="P214" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
     </row>
     <row r="215" spans="16:16">
       <c r="P215" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
     </row>
     <row r="216" spans="16:16">
       <c r="P216" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
     </row>
     <row r="217" spans="16:16">
       <c r="P217" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
     </row>
     <row r="218" spans="16:16">
       <c r="P218" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
     </row>
     <row r="219" spans="16:16">
       <c r="P219" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
     </row>
     <row r="220" spans="16:16">
       <c r="P220" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
     </row>
     <row r="221" spans="16:16">
       <c r="P221" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
     </row>
     <row r="222" spans="16:16">
       <c r="P222" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
     </row>
     <row r="223" spans="16:16">
       <c r="P223" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
     </row>
     <row r="224" spans="16:16">
       <c r="P224" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
     </row>
     <row r="225" spans="16:16">
       <c r="P225" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
     </row>
     <row r="226" spans="16:16">
       <c r="P226" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
     </row>
     <row r="227" spans="16:16">
       <c r="P227" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
     </row>
     <row r="228" spans="16:16">
       <c r="P228" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
     </row>
     <row r="229" spans="16:16">
       <c r="P229" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
     </row>
     <row r="230" spans="16:16">
       <c r="P230" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
     </row>
     <row r="231" spans="16:16">
       <c r="P231" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
     </row>
     <row r="232" spans="16:16">
       <c r="P232" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
     </row>
     <row r="233" spans="16:16">
       <c r="P233" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
     </row>
     <row r="234" spans="16:16">
       <c r="P234" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
     </row>
     <row r="235" spans="16:16">
       <c r="P235" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
     </row>
     <row r="236" spans="16:16">
       <c r="P236" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
     </row>
     <row r="237" spans="16:16">
       <c r="P237" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
     </row>
     <row r="238" spans="16:16">
       <c r="P238" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
     </row>
     <row r="239" spans="16:16">
       <c r="P239" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
     </row>
     <row r="240" spans="16:16">
       <c r="P240" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
     </row>
     <row r="241" spans="16:16">
       <c r="P241" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
     </row>
     <row r="242" spans="16:16">
       <c r="P242" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
     </row>
     <row r="243" spans="16:16">
       <c r="P243" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
     </row>
     <row r="244" spans="16:16">
       <c r="P244" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
     </row>
     <row r="245" spans="16:16">
       <c r="P245" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
     </row>
     <row r="246" spans="16:16">
       <c r="P246" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
     </row>
     <row r="247" spans="16:16">
       <c r="P247" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
     </row>
     <row r="248" spans="16:16">
       <c r="P248" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
     </row>
     <row r="249" spans="16:16">
       <c r="P249" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
     </row>
     <row r="250" spans="16:16">
       <c r="P250" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
     </row>
     <row r="251" spans="16:16">
       <c r="P251" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
     </row>
     <row r="252" spans="16:16">
       <c r="P252" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
     </row>
     <row r="253" spans="16:16">
       <c r="P253" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
     </row>
     <row r="254" spans="16:16">
       <c r="P254" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
     </row>
     <row r="255" spans="16:16">
       <c r="P255" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
     </row>
     <row r="256" spans="16:16">
       <c r="P256" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
     </row>
     <row r="257" spans="16:16">
       <c r="P257" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
     </row>
     <row r="258" spans="16:16">
       <c r="P258" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -4280,15 +4011,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fixes on version without links.
</commit_message>
<xml_diff>
--- a/data/MetaMaster.xlsx
+++ b/data/MetaMaster.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="24030" windowHeight="5790" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="19155" windowHeight="5790" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
-    <definedName name="Assay">Lists!$A$2:$A$10</definedName>
+    <definedName name="Assay">Lists!$A$2:$A$8</definedName>
     <definedName name="Category">Lists!$A$1:$H$1</definedName>
     <definedName name="Column">Lists!$P$2:$P$258</definedName>
     <definedName name="DerivationFactor">Lists!$K$2:$K$6</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="421">
   <si>
     <t>Easting</t>
   </si>
@@ -431,9 +431,6 @@
     <t>-- Constants --</t>
   </si>
   <si>
-    <t>row</t>
-  </si>
-  <si>
     <t>Designation</t>
   </si>
   <si>
@@ -1205,12 +1202,6 @@
     <t>IV</t>
   </si>
   <si>
-    <t>External_ID</t>
-  </si>
-  <si>
-    <t>External_Link</t>
-  </si>
-  <si>
     <t>External Sheet</t>
   </si>
   <si>
@@ -1311,6 +1302,9 @@
   </si>
   <si>
     <t>isSimilarTo</t>
+  </si>
+  <si>
+    <t>all</t>
   </si>
 </sst>
 </file>
@@ -1785,10 +1779,10 @@
   <dimension ref="A1:Z119"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="13" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="13" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12"/>
@@ -1815,16 +1809,16 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" t="s">
         <v>145</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>146</v>
-      </c>
-      <c r="H1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:26">
@@ -1835,22 +1829,22 @@
         <v>35</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H2" t="s">
         <v>148</v>
-      </c>
-      <c r="H2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -1858,57 +1852,57 @@
         <v>77</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" t="s">
         <v>140</v>
       </c>
-      <c r="E3" t="s">
-        <v>141</v>
-      </c>
       <c r="F3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H3" t="s">
         <v>150</v>
-      </c>
-      <c r="H3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="E4" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D5" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="E5" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="F5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G5" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -1916,16 +1910,16 @@
         <v>128</v>
       </c>
       <c r="C6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="F6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G6" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="H6" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -1933,22 +1927,22 @@
         <v>14</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E7" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F7" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="G7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H7" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -1956,22 +1950,22 @@
         <v>34</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E8" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="F8" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="G8" t="s">
+        <v>152</v>
+      </c>
+      <c r="H8" t="s">
         <v>153</v>
-      </c>
-      <c r="H8" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -1979,22 +1973,22 @@
         <v>12</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E9" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="F9" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="G9" t="s">
+        <v>154</v>
+      </c>
+      <c r="H9" t="s">
         <v>155</v>
-      </c>
-      <c r="H9" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -2014,7 +2008,7 @@
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="16" spans="1:26">
@@ -2081,7 +2075,7 @@
   <dimension ref="A1:P258"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -2101,7 +2095,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C1" t="s">
         <v>19</v>
@@ -2119,7 +2113,7 @@
         <v>22</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2" t="s">
@@ -2189,12 +2183,12 @@
         <v>35</v>
       </c>
       <c r="P2" t="s">
-        <v>129</v>
+        <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15">
       <c r="A3" s="2" t="s">
-        <v>387</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>25</v>
@@ -2236,7 +2230,7 @@
     </row>
     <row r="4" spans="1:16" ht="15">
       <c r="A4" s="2" t="s">
-        <v>388</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
@@ -2277,8 +2271,8 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15">
-      <c r="A5" s="2" t="s">
-        <v>25</v>
+      <c r="A5" t="s">
+        <v>41</v>
       </c>
       <c r="B5" t="s">
         <v>41</v>
@@ -2316,7 +2310,7 @@
     </row>
     <row r="6" spans="1:16" ht="15">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>26</v>
@@ -2354,8 +2348,8 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="15">
-      <c r="A7" t="s">
-        <v>41</v>
+      <c r="A7" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>10</v>
@@ -2367,17 +2361,17 @@
         <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="6" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="K7" s="2"/>
       <c r="N7" t="s">
@@ -2389,7 +2383,7 @@
     </row>
     <row r="8" spans="1:16" ht="15">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>16</v>
@@ -2398,7 +2392,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F8" t="s">
         <v>19</v>
@@ -2422,9 +2416,6 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="15">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
@@ -2435,7 +2426,7 @@
         <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>9</v>
@@ -2456,9 +2447,6 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="15">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="C10" s="2" t="s">
         <v>28</v>
       </c>
@@ -2469,13 +2457,13 @@
         <v>38</v>
       </c>
       <c r="F10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
@@ -2490,11 +2478,14 @@
       <c r="C11" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="D11" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="E11" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F11" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>18</v>
@@ -2513,10 +2504,10 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
@@ -2532,7 +2523,7 @@
         <v>31</v>
       </c>
       <c r="F13" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>40</v>
@@ -2552,7 +2543,7 @@
         <v>33</v>
       </c>
       <c r="J14" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="K14" s="2"/>
       <c r="P14" t="s">
@@ -2600,7 +2591,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="5" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="K19" s="2"/>
       <c r="P19" t="s">
@@ -2655,7 +2646,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="K23" s="2"/>
       <c r="P23" t="s">
@@ -2680,7 +2671,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="5" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="K25" s="2"/>
       <c r="P25" t="s">
@@ -2732,7 +2723,7 @@
       </c>
       <c r="K29" s="2"/>
       <c r="P29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15">
@@ -2742,7 +2733,7 @@
       </c>
       <c r="K30" s="2"/>
       <c r="P30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15">
@@ -2752,7 +2743,7 @@
       </c>
       <c r="K31" s="2"/>
       <c r="P31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15">
@@ -2762,7 +2753,7 @@
       </c>
       <c r="K32" s="2"/>
       <c r="P32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="5:16" ht="15">
@@ -2772,7 +2763,7 @@
       </c>
       <c r="K33" s="2"/>
       <c r="P33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34" spans="5:16" ht="15">
@@ -2782,7 +2773,7 @@
       </c>
       <c r="K34" s="2"/>
       <c r="P34" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35" spans="5:16" ht="15">
@@ -2792,17 +2783,17 @@
       </c>
       <c r="K35" s="2"/>
       <c r="P35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="5:16" ht="15">
       <c r="E36" s="2"/>
       <c r="J36" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="K36" s="2"/>
       <c r="P36" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" spans="5:16" ht="15">
@@ -2812,7 +2803,7 @@
       </c>
       <c r="K37" s="2"/>
       <c r="P37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" spans="5:16" ht="15">
@@ -2822,7 +2813,7 @@
       </c>
       <c r="K38" s="2"/>
       <c r="P38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="5:16" ht="15">
@@ -2832,7 +2823,7 @@
       </c>
       <c r="K39" s="2"/>
       <c r="P39" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="5:16" ht="15">
@@ -2841,7 +2832,7 @@
       </c>
       <c r="K40" s="2"/>
       <c r="P40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="5:16" ht="15">
@@ -2850,16 +2841,16 @@
       </c>
       <c r="K41" s="2"/>
       <c r="P41" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="42" spans="5:16" ht="15">
       <c r="J42" s="2" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="K42" s="2"/>
       <c r="P42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="5:16" ht="15">
@@ -2868,7 +2859,7 @@
       </c>
       <c r="K43" s="2"/>
       <c r="P43" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="5:16" ht="15">
@@ -2877,25 +2868,25 @@
       </c>
       <c r="K44" s="2"/>
       <c r="P44" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="5:16" ht="15">
       <c r="J45" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="K45" s="2"/>
       <c r="P45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="46" spans="5:16" ht="15">
       <c r="J46" s="6" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="K46" s="2"/>
       <c r="P46" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" spans="5:16" ht="15">
@@ -2904,7 +2895,7 @@
       </c>
       <c r="K47" s="2"/>
       <c r="P47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="5:16" ht="15">
@@ -2912,7 +2903,7 @@
         <v>112</v>
       </c>
       <c r="P48" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="49" spans="10:16">
@@ -2920,7 +2911,7 @@
         <v>22</v>
       </c>
       <c r="P49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="50" spans="10:16" ht="15">
@@ -2928,7 +2919,7 @@
         <v>109</v>
       </c>
       <c r="P50" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="10:16" ht="15">
@@ -2936,7 +2927,7 @@
         <v>113</v>
       </c>
       <c r="P51" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="52" spans="10:16" ht="15">
@@ -2944,7 +2935,7 @@
         <v>114</v>
       </c>
       <c r="P52" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="53" spans="10:16" ht="15">
@@ -2952,7 +2943,7 @@
         <v>115</v>
       </c>
       <c r="P53" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="54" spans="10:16" ht="15">
@@ -2960,7 +2951,7 @@
         <v>116</v>
       </c>
       <c r="P54" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="55" spans="10:16" ht="15">
@@ -2968,7 +2959,7 @@
         <v>118</v>
       </c>
       <c r="P55" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="56" spans="10:16" ht="15">
@@ -2976,7 +2967,7 @@
         <v>117</v>
       </c>
       <c r="P56" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="57" spans="10:16" ht="15">
@@ -2984,1012 +2975,1012 @@
         <v>119</v>
       </c>
       <c r="P57" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="58" spans="10:16">
       <c r="P58" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="59" spans="10:16">
       <c r="P59" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="60" spans="10:16">
       <c r="P60" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="10:16">
       <c r="P61" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="62" spans="10:16">
       <c r="P62" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="63" spans="10:16">
       <c r="P63" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="64" spans="10:16">
       <c r="P64" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="65" spans="16:16">
       <c r="P65" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="66" spans="16:16">
       <c r="P66" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="67" spans="16:16">
       <c r="P67" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="68" spans="16:16">
       <c r="P68" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="69" spans="16:16">
       <c r="P69" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="70" spans="16:16">
       <c r="P70" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="71" spans="16:16">
       <c r="P71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="72" spans="16:16">
       <c r="P72" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="73" spans="16:16">
       <c r="P73" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="74" spans="16:16">
       <c r="P74" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="75" spans="16:16">
       <c r="P75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="76" spans="16:16">
       <c r="P76" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="77" spans="16:16">
       <c r="P77" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="78" spans="16:16">
       <c r="P78" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="79" spans="16:16">
       <c r="P79" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="80" spans="16:16">
       <c r="P80" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="81" spans="16:16">
       <c r="P81" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="82" spans="16:16">
       <c r="P82" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="83" spans="16:16">
       <c r="P83" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="84" spans="16:16">
       <c r="P84" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="85" spans="16:16">
       <c r="P85" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="86" spans="16:16">
       <c r="P86" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="87" spans="16:16">
       <c r="P87" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="88" spans="16:16">
       <c r="P88" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="89" spans="16:16">
       <c r="P89" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="90" spans="16:16">
       <c r="P90" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="91" spans="16:16">
       <c r="P91" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="92" spans="16:16">
       <c r="P92" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="93" spans="16:16">
       <c r="P93" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="94" spans="16:16">
       <c r="P94" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="95" spans="16:16">
       <c r="P95" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="96" spans="16:16">
       <c r="P96" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="97" spans="16:16">
       <c r="P97" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="98" spans="16:16">
       <c r="P98" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="99" spans="16:16">
       <c r="P99" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="100" spans="16:16">
       <c r="P100" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="101" spans="16:16">
       <c r="P101" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="102" spans="16:16">
       <c r="P102" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="103" spans="16:16">
       <c r="P103" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="104" spans="16:16">
       <c r="P104" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="105" spans="16:16">
       <c r="P105" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="106" spans="16:16">
       <c r="P106" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="107" spans="16:16">
       <c r="P107" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="108" spans="16:16">
       <c r="P108" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="109" spans="16:16">
       <c r="P109" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="110" spans="16:16">
       <c r="P110" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="111" spans="16:16">
       <c r="P111" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="112" spans="16:16">
       <c r="P112" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="113" spans="16:16">
       <c r="P113" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="114" spans="16:16">
       <c r="P114" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="115" spans="16:16">
       <c r="P115" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="116" spans="16:16">
       <c r="P116" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="117" spans="16:16">
       <c r="P117" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="118" spans="16:16">
       <c r="P118" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="119" spans="16:16">
       <c r="P119" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="120" spans="16:16">
       <c r="P120" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="121" spans="16:16">
       <c r="P121" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="122" spans="16:16">
       <c r="P122" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="123" spans="16:16">
       <c r="P123" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="124" spans="16:16">
       <c r="P124" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="125" spans="16:16">
       <c r="P125" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="126" spans="16:16">
       <c r="P126" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="127" spans="16:16">
       <c r="P127" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="128" spans="16:16">
       <c r="P128" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="129" spans="16:16">
       <c r="P129" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="130" spans="16:16">
       <c r="P130" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="131" spans="16:16">
       <c r="P131" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="132" spans="16:16">
       <c r="P132" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="133" spans="16:16">
       <c r="P133" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="134" spans="16:16">
       <c r="P134" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="135" spans="16:16">
       <c r="P135" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="136" spans="16:16">
       <c r="P136" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="137" spans="16:16">
       <c r="P137" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="138" spans="16:16">
       <c r="P138" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="139" spans="16:16">
       <c r="P139" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="140" spans="16:16">
       <c r="P140" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="141" spans="16:16">
       <c r="P141" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="142" spans="16:16">
       <c r="P142" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="143" spans="16:16">
       <c r="P143" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="144" spans="16:16">
       <c r="P144" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="145" spans="16:16">
       <c r="P145" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="146" spans="16:16">
       <c r="P146" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="147" spans="16:16">
       <c r="P147" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="148" spans="16:16">
       <c r="P148" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="149" spans="16:16">
       <c r="P149" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="150" spans="16:16">
       <c r="P150" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="151" spans="16:16">
       <c r="P151" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="152" spans="16:16">
       <c r="P152" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="153" spans="16:16">
       <c r="P153" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="154" spans="16:16">
       <c r="P154" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="155" spans="16:16">
       <c r="P155" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="156" spans="16:16">
       <c r="P156" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="157" spans="16:16">
       <c r="P157" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="158" spans="16:16">
       <c r="P158" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="159" spans="16:16">
       <c r="P159" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="160" spans="16:16">
       <c r="P160" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="161" spans="16:16">
       <c r="P161" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="162" spans="16:16">
       <c r="P162" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="163" spans="16:16">
       <c r="P163" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="164" spans="16:16">
       <c r="P164" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="165" spans="16:16">
       <c r="P165" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="166" spans="16:16">
       <c r="P166" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="167" spans="16:16">
       <c r="P167" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="168" spans="16:16">
       <c r="P168" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="169" spans="16:16">
       <c r="P169" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="170" spans="16:16">
       <c r="P170" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="171" spans="16:16">
       <c r="P171" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="172" spans="16:16">
       <c r="P172" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="173" spans="16:16">
       <c r="P173" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="174" spans="16:16">
       <c r="P174" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="175" spans="16:16">
       <c r="P175" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="176" spans="16:16">
       <c r="P176" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="177" spans="16:16">
       <c r="P177" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="178" spans="16:16">
       <c r="P178" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="179" spans="16:16">
       <c r="P179" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="180" spans="16:16">
       <c r="P180" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="181" spans="16:16">
       <c r="P181" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="182" spans="16:16">
       <c r="P182" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="183" spans="16:16">
       <c r="P183" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="184" spans="16:16">
       <c r="P184" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="185" spans="16:16">
       <c r="P185" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="186" spans="16:16">
       <c r="P186" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="187" spans="16:16">
       <c r="P187" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="188" spans="16:16">
       <c r="P188" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="189" spans="16:16">
       <c r="P189" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="190" spans="16:16">
       <c r="P190" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="191" spans="16:16">
       <c r="P191" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="192" spans="16:16">
       <c r="P192" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="193" spans="16:16">
       <c r="P193" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="194" spans="16:16">
       <c r="P194" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="195" spans="16:16">
       <c r="P195" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="196" spans="16:16">
       <c r="P196" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="197" spans="16:16">
       <c r="P197" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="198" spans="16:16">
       <c r="P198" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="199" spans="16:16">
       <c r="P199" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="200" spans="16:16">
       <c r="P200" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="201" spans="16:16">
       <c r="P201" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="202" spans="16:16">
       <c r="P202" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="203" spans="16:16">
       <c r="P203" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="204" spans="16:16">
       <c r="P204" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="205" spans="16:16">
       <c r="P205" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="206" spans="16:16">
       <c r="P206" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="207" spans="16:16">
       <c r="P207" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="208" spans="16:16">
       <c r="P208" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="209" spans="16:16">
       <c r="P209" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="210" spans="16:16">
       <c r="P210" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="211" spans="16:16">
       <c r="P211" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="212" spans="16:16">
       <c r="P212" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="213" spans="16:16">
       <c r="P213" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="214" spans="16:16">
       <c r="P214" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="215" spans="16:16">
       <c r="P215" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="216" spans="16:16">
       <c r="P216" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="217" spans="16:16">
       <c r="P217" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="218" spans="16:16">
       <c r="P218" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="219" spans="16:16">
       <c r="P219" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="220" spans="16:16">
       <c r="P220" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="221" spans="16:16">
       <c r="P221" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="222" spans="16:16">
       <c r="P222" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="223" spans="16:16">
       <c r="P223" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="224" spans="16:16">
       <c r="P224" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="225" spans="16:16">
       <c r="P225" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="226" spans="16:16">
       <c r="P226" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="227" spans="16:16">
       <c r="P227" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="228" spans="16:16">
       <c r="P228" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="229" spans="16:16">
       <c r="P229" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="230" spans="16:16">
       <c r="P230" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="231" spans="16:16">
       <c r="P231" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="232" spans="16:16">
       <c r="P232" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="233" spans="16:16">
       <c r="P233" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="234" spans="16:16">
       <c r="P234" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="235" spans="16:16">
       <c r="P235" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="236" spans="16:16">
       <c r="P236" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="237" spans="16:16">
       <c r="P237" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="238" spans="16:16">
       <c r="P238" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="239" spans="16:16">
       <c r="P239" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="240" spans="16:16">
       <c r="P240" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="241" spans="16:16">
       <c r="P241" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="242" spans="16:16">
       <c r="P242" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="243" spans="16:16">
       <c r="P243" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="244" spans="16:16">
       <c r="P244" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="245" spans="16:16">
       <c r="P245" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="246" spans="16:16">
       <c r="P246" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="247" spans="16:16">
       <c r="P247" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="248" spans="16:16">
       <c r="P248" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="249" spans="16:16">
       <c r="P249" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="250" spans="16:16">
       <c r="P250" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="251" spans="16:16">
       <c r="P251" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="252" spans="16:16">
       <c r="P252" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="253" spans="16:16">
       <c r="P253" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="254" spans="16:16">
       <c r="P254" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="255" spans="16:16">
       <c r="P255" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="256" spans="16:16">
       <c r="P256" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="257" spans="16:16">
       <c r="P257" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="258" spans="16:16">
       <c r="P258" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -4011,15 +4002,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now ignores empty sheets when creating meta data
</commit_message>
<xml_diff>
--- a/data/MetaMaster.xlsx
+++ b/data/MetaMaster.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="19155" windowHeight="5790" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="19155" windowHeight="5790"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,15 +17,16 @@
   </externalReferences>
   <definedNames>
     <definedName name="Assay">Lists!$A$2:$A$8</definedName>
+    <definedName name="Automatic">Lists!$M$2</definedName>
     <definedName name="Category">Lists!$A$1:$H$1</definedName>
-    <definedName name="Column">Lists!$P$2:$P$258</definedName>
+    <definedName name="Column">Lists!$Q$2:$Q$258</definedName>
     <definedName name="DerivationFactor">Lists!$K$2:$K$6</definedName>
     <definedName name="Designation">Lists!$B$2:$B$6</definedName>
     <definedName name="Factor">Lists!$J$2:$J$52</definedName>
     <definedName name="FeildsThatNeedUnit" localSheetId="2">[1]Lists!$P$2:$P$4</definedName>
-    <definedName name="FeildsThatNeedUnit">Lists!$O$2:$O$4</definedName>
+    <definedName name="FeildsThatNeedUnit">Lists!$P$2:$P$4</definedName>
     <definedName name="Location">Lists!$C$2:$C$14</definedName>
-    <definedName name="NotApplicable">Lists!$M$2</definedName>
+    <definedName name="NotApplicable">Lists!$N$2</definedName>
     <definedName name="Observation">Lists!$D$2:$D$10</definedName>
     <definedName name="OnlyTrue">Lists!#REF!</definedName>
     <definedName name="Person">Lists!$E$2:$E$11</definedName>
@@ -35,14 +36,14 @@
     <definedName name="Survey">Lists!$H$2:$H$10</definedName>
     <definedName name="TrueFalse">Lists!#REF!</definedName>
     <definedName name="UNDEFINED">Lists!$L$2</definedName>
-    <definedName name="Unit">Lists!$N$2:$N$9</definedName>
+    <definedName name="Unit">Lists!$O$2:$O$9</definedName>
   </definedNames>
   <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="424">
   <si>
     <t>Easting</t>
   </si>
@@ -464,9 +465,6 @@
     <t>id/Value Column</t>
   </si>
   <si>
-    <t>The column that contains the ID/value of the Category this columns applies to. Enter "row" if the Category has no Id column. Not required for "Id" or Observation's "value" fields.</t>
-  </si>
-  <si>
     <t>Factor for Observation's Value</t>
   </si>
   <si>
@@ -494,9 +492,6 @@
     <t>Unexpected Value</t>
   </si>
   <si>
-    <t>Please select a value from the list or contact an Admin to explain why a different value is required.</t>
-  </si>
-  <si>
     <t>Unexpected Factor</t>
   </si>
   <si>
@@ -1277,9 +1272,6 @@
     <t>SKIDDAW_S</t>
   </si>
   <si>
-    <t>INDIRECT(IF(OR($B$2="Id",$B$2="Value"),"NotApplicable","Column"))</t>
-  </si>
-  <si>
     <t>INDIRECT(SUBSTITUTE($B$1," ","_"))</t>
   </si>
   <si>
@@ -1305,6 +1297,24 @@
   </si>
   <si>
     <t>all</t>
+  </si>
+  <si>
+    <t>Automatic</t>
+  </si>
+  <si>
+    <t>INDIRECT(IF(AND($B$1="Observation",$B$2="Value"),"Column","Automatic"))</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>INDIRECT(IF(AND($B$1="Observation",$B$2&lt;&gt;"Value"),"Column","Automatic"))</t>
+  </si>
+  <si>
+    <t>The column that contains the ID/value of the Observation this columns applies to. Enter "all" to apply it to all Observations. Only required Observation's none "value" fields.</t>
+  </si>
+  <si>
+    <t>Please select a value from the list.</t>
   </si>
 </sst>
 </file>
@@ -1778,18 +1788,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z119"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="13" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="13" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" customWidth="1"/>
     <col min="6" max="7" width="13.28515625" customWidth="1"/>
@@ -1812,13 +1822,13 @@
         <v>137</v>
       </c>
       <c r="F1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" t="s">
         <v>144</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>145</v>
-      </c>
-      <c r="H1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:26">
@@ -1826,10 +1836,10 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
@@ -1838,13 +1848,13 @@
         <v>138</v>
       </c>
       <c r="F2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H2" t="s">
         <v>147</v>
-      </c>
-      <c r="H2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -1852,57 +1862,57 @@
         <v>77</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="D3" t="s">
         <v>139</v>
       </c>
       <c r="E3" t="s">
-        <v>140</v>
+        <v>422</v>
       </c>
       <c r="F3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H3" t="s">
-        <v>150</v>
+        <v>423</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D5" t="s">
+        <v>387</v>
+      </c>
+      <c r="E5" t="s">
+        <v>388</v>
+      </c>
+      <c r="F5" t="s">
+        <v>143</v>
+      </c>
+      <c r="G5" t="s">
         <v>389</v>
-      </c>
-      <c r="E5" t="s">
-        <v>390</v>
-      </c>
-      <c r="F5" t="s">
-        <v>144</v>
-      </c>
-      <c r="G5" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -1910,16 +1920,16 @@
         <v>128</v>
       </c>
       <c r="C6" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="F6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G6" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="H6" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -1927,22 +1937,22 @@
         <v>14</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E7" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="G7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -1950,22 +1960,22 @@
         <v>34</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E8" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F8" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="G8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -1973,22 +1983,22 @@
         <v>12</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E9" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F9" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="G9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -2008,7 +2018,7 @@
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="16" spans="1:26">
@@ -2029,12 +2039,20 @@
     <row r="23" spans="1:3">
       <c r="C23" s="4"/>
     </row>
+    <row r="26" spans="1:3">
+      <c r="B26" t="s">
+        <v>420</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>419</v>
+      </c>
+    </row>
     <row r="119" spans="14:14">
       <c r="N119" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations xWindow="284" yWindow="481" count="9">
+  <dataValidations xWindow="284" yWindow="481" count="10">
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Unit." error="The Unit provided was not in the list. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." promptTitle="Unit for Observation's Value" prompt="Please describe the Unit the values are in. Whenever possible pick a value from the list." sqref="B8">
       <formula1>"INDIRECT(IF(ISNA(VLOOKUP($B$2,FeildsThatNeedUnit,1,FALSE)),""NotApplicable"",""UNIT""))"</formula1>
     </dataValidation>
@@ -2061,7 +2079,10 @@
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="id/Value Column" prompt="The column that contains the ID/value of the Category this columns applies to. Enter &quot;row&quot; if the Category has no Id column. Not required for &quot;Id&quot; or Observation's &quot;value&quot; fields." sqref="B3">
-      <formula1>INDIRECT(IF(OR($B$2="Id",$B$2="Value"),"NotApplicable","Column"))</formula1>
+      <formula1>INDIRECT(IF(AND($B$1="Observation",$B$2&lt;&gt;"Value"),"Column","Automatic"))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+      <formula1>"if($B$1=""Observatio"",{""Yes,""NO""},{""true"",""false""})"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2072,10 +2093,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P258"/>
+  <dimension ref="A1:Q258"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -2086,11 +2107,11 @@
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="6" width="13.140625" customWidth="1"/>
     <col min="11" max="11" width="19.5703125" customWidth="1"/>
-    <col min="16" max="16" width="9.42578125" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" customWidth="1"/>
+    <col min="18" max="18" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15">
+    <row r="1" spans="1:17" ht="15">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -2125,20 +2146,23 @@
       <c r="L1" t="s">
         <v>29</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="N1" t="s">
         <v>43</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>34</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>49</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15">
+    <row r="2" spans="1:17" ht="15">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2174,19 +2198,22 @@
         <v>30</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P2" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15">
+      <c r="Q2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -2218,17 +2245,17 @@
       <c r="K3" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>46</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15">
+    <row r="4" spans="1:17" ht="15">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -2260,17 +2287,17 @@
       <c r="K4" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>47</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15">
+    <row r="5" spans="1:17" ht="15">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -2301,14 +2328,14 @@
       <c r="K5" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15">
+    <row r="6" spans="1:17" ht="15">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
@@ -2340,14 +2367,14 @@
       <c r="K6" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15">
+    <row r="7" spans="1:17" ht="15">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -2371,17 +2398,17 @@
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="6" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="K7" s="2"/>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>45</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15">
+    <row r="8" spans="1:17" ht="15">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -2408,14 +2435,14 @@
         <v>83</v>
       </c>
       <c r="K8" s="2"/>
-      <c r="N8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15">
+    <row r="9" spans="1:17" ht="15">
       <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
@@ -2439,14 +2466,14 @@
         <v>84</v>
       </c>
       <c r="K9" s="2"/>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>48</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15">
+    <row r="10" spans="1:17" ht="15">
       <c r="C10" s="2" t="s">
         <v>28</v>
       </c>
@@ -2470,11 +2497,11 @@
         <v>85</v>
       </c>
       <c r="K10" s="2"/>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15">
+    <row r="11" spans="1:17" ht="15">
       <c r="C11" s="2" t="s">
         <v>0</v>
       </c>
@@ -2485,7 +2512,7 @@
         <v>39</v>
       </c>
       <c r="F11" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>18</v>
@@ -2495,35 +2522,35 @@
         <v>86</v>
       </c>
       <c r="K11" s="2"/>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15">
+    <row r="12" spans="1:17" ht="15">
       <c r="C12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F12" t="s">
+        <v>395</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>397</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>399</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K12" s="2"/>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15">
+    <row r="13" spans="1:17" ht="15">
       <c r="C13" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F13" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>40</v>
@@ -2534,71 +2561,71 @@
         <v>89</v>
       </c>
       <c r="K13" s="2"/>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15">
+    <row r="14" spans="1:17" ht="15">
       <c r="C14" s="2" t="s">
         <v>33</v>
       </c>
       <c r="J14" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="K14" s="2"/>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15">
+    <row r="15" spans="1:17" ht="15">
       <c r="J15" s="2" t="s">
         <v>90</v>
       </c>
       <c r="K15" s="2"/>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15">
+    <row r="16" spans="1:17" ht="15">
       <c r="J16" s="2" t="s">
         <v>91</v>
       </c>
       <c r="K16" s="2"/>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="15">
+    <row r="17" spans="1:17" ht="15">
       <c r="J17" s="2" t="s">
         <v>92</v>
       </c>
       <c r="K17" s="2"/>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15">
+    <row r="18" spans="1:17" ht="15">
       <c r="J18" s="2" t="s">
         <v>87</v>
       </c>
       <c r="K18" s="2"/>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15">
+    <row r="19" spans="1:17" ht="15">
       <c r="D19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="K19" s="2"/>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15">
+    <row r="20" spans="1:17" ht="15">
       <c r="D20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -2607,11 +2634,11 @@
         <v>4</v>
       </c>
       <c r="K20" s="2"/>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15">
+    <row r="21" spans="1:17" ht="15">
       <c r="D21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -2620,11 +2647,11 @@
         <v>93</v>
       </c>
       <c r="K21" s="2"/>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15">
+    <row r="22" spans="1:17" ht="15">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="D22" s="2"/>
@@ -2636,24 +2663,24 @@
         <v>94</v>
       </c>
       <c r="K22" s="2"/>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15">
+    <row r="23" spans="1:17" ht="15">
       <c r="D23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="K23" s="2"/>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15">
+    <row r="24" spans="1:17" ht="15">
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -2661,24 +2688,24 @@
         <v>95</v>
       </c>
       <c r="K24" s="2"/>
-      <c r="P24" t="s">
+      <c r="Q24" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15">
+    <row r="25" spans="1:17" ht="15">
       <c r="D25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="5" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="K25" s="2"/>
-      <c r="P25" t="s">
+      <c r="Q25" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="15">
+    <row r="26" spans="1:17" ht="15">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="D26" s="2"/>
@@ -2690,31 +2717,31 @@
         <v>2</v>
       </c>
       <c r="K26" s="2"/>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15">
+    <row r="27" spans="1:17" ht="15">
       <c r="E27" s="2"/>
       <c r="J27" s="2" t="s">
         <v>96</v>
       </c>
       <c r="K27" s="2"/>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15">
+    <row r="28" spans="1:17" ht="15">
       <c r="E28" s="2"/>
       <c r="J28" s="2" t="s">
         <v>97</v>
       </c>
       <c r="K28" s="2"/>
-      <c r="P28" t="s">
+      <c r="Q28" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15">
+    <row r="29" spans="1:17" ht="15">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="E29" s="2"/>
@@ -2722,1265 +2749,1265 @@
         <v>103</v>
       </c>
       <c r="K29" s="2"/>
-      <c r="P29" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="15">
+      <c r="Q29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="15">
       <c r="E30" s="2"/>
       <c r="J30" s="2" t="s">
         <v>98</v>
       </c>
       <c r="K30" s="2"/>
-      <c r="P30" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="15">
+      <c r="Q30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="15">
       <c r="E31" s="2"/>
       <c r="J31" s="2" t="s">
         <v>99</v>
       </c>
       <c r="K31" s="2"/>
-      <c r="P31" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" ht="15">
+      <c r="Q31" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="15">
       <c r="E32" s="2"/>
       <c r="J32" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K32" s="2"/>
-      <c r="P32" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="33" spans="5:16" ht="15">
+      <c r="Q32" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="5:17" ht="15">
       <c r="E33" s="2"/>
       <c r="J33" s="2" t="s">
         <v>101</v>
       </c>
       <c r="K33" s="2"/>
-      <c r="P33" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="34" spans="5:16" ht="15">
+      <c r="Q33" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="5:17" ht="15">
       <c r="E34" s="2"/>
       <c r="J34" s="2" t="s">
         <v>3</v>
       </c>
       <c r="K34" s="2"/>
-      <c r="P34" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="35" spans="5:16" ht="15">
+      <c r="Q34" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="5:17" ht="15">
       <c r="E35" s="2"/>
       <c r="J35" s="2" t="s">
         <v>45</v>
       </c>
       <c r="K35" s="2"/>
-      <c r="P35" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="36" spans="5:16" ht="15">
+      <c r="Q35" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="5:17" ht="15">
       <c r="E36" s="2"/>
       <c r="J36" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="K36" s="2"/>
-      <c r="P36" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="37" spans="5:16" ht="15">
+      <c r="Q36" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="5:17" ht="15">
       <c r="E37" s="2"/>
       <c r="J37" s="2" t="s">
         <v>102</v>
       </c>
       <c r="K37" s="2"/>
-      <c r="P37" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="38" spans="5:16" ht="15">
+      <c r="Q37" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" spans="5:17" ht="15">
       <c r="E38" s="2"/>
       <c r="J38" s="2" t="s">
         <v>104</v>
       </c>
       <c r="K38" s="2"/>
-      <c r="P38" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="39" spans="5:16" ht="15">
+      <c r="Q38" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" spans="5:17" ht="15">
       <c r="E39" s="2"/>
       <c r="J39" s="2" t="s">
         <v>106</v>
       </c>
       <c r="K39" s="2"/>
-      <c r="P39" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="40" spans="5:16" ht="15">
+      <c r="Q39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" spans="5:17" ht="15">
       <c r="J40" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K40" s="2"/>
-      <c r="P40" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="41" spans="5:16" ht="15">
+      <c r="Q40" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="5:17" ht="15">
       <c r="J41" s="2" t="s">
         <v>110</v>
       </c>
       <c r="K41" s="2"/>
-      <c r="P41" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="42" spans="5:16" ht="15">
+      <c r="Q41" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="5:17" ht="15">
       <c r="J42" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="K42" s="2"/>
-      <c r="P42" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="43" spans="5:16" ht="15">
+      <c r="Q42" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" spans="5:17" ht="15">
       <c r="J43" s="2" t="s">
         <v>107</v>
       </c>
       <c r="K43" s="2"/>
-      <c r="P43" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="44" spans="5:16" ht="15">
+      <c r="Q43" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="5:17" ht="15">
       <c r="J44" s="2" t="s">
         <v>108</v>
       </c>
       <c r="K44" s="2"/>
-      <c r="P44" t="s">
+      <c r="Q44" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="5:17" ht="15">
+      <c r="J45" t="s">
+        <v>404</v>
+      </c>
+      <c r="K45" s="2"/>
+      <c r="Q45" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="5:17" ht="15">
+      <c r="J46" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="K46" s="2"/>
+      <c r="Q46" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="45" spans="5:16" ht="15">
-      <c r="J45" t="s">
-        <v>406</v>
-      </c>
-      <c r="K45" s="2"/>
-      <c r="P45" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="46" spans="5:16" ht="15">
-      <c r="J46" s="6" t="s">
-        <v>410</v>
-      </c>
-      <c r="K46" s="2"/>
-      <c r="P46" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="47" spans="5:16" ht="15">
+    <row r="47" spans="5:17" ht="15">
       <c r="J47" s="2" t="s">
         <v>111</v>
       </c>
       <c r="K47" s="2"/>
-      <c r="P47" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="48" spans="5:16" ht="15">
+      <c r="Q47" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="48" spans="5:17" ht="15">
       <c r="J48" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="P48" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="49" spans="10:16">
+      <c r="Q48" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="49" spans="10:17">
       <c r="J49" t="s">
         <v>22</v>
       </c>
-      <c r="P49" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="50" spans="10:16" ht="15">
+      <c r="Q49" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="50" spans="10:17" ht="15">
       <c r="J50" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="P50" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="51" spans="10:16" ht="15">
+      <c r="Q50" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="51" spans="10:17" ht="15">
       <c r="J51" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="P51" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="52" spans="10:16" ht="15">
+      <c r="Q51" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="52" spans="10:17" ht="15">
       <c r="J52" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="P52" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="53" spans="10:16" ht="15">
+      <c r="Q52" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="53" spans="10:17" ht="15">
       <c r="J53" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="P53" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="54" spans="10:16" ht="15">
+      <c r="Q53" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="54" spans="10:17" ht="15">
       <c r="J54" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="P54" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="55" spans="10:16" ht="15">
+      <c r="Q54" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="55" spans="10:17" ht="15">
       <c r="J55" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="P55" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="56" spans="10:16" ht="15">
+      <c r="Q55" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="10:17" ht="15">
       <c r="J56" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="P56" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="57" spans="10:16" ht="15">
+      <c r="Q56" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="57" spans="10:17" ht="15">
       <c r="J57" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="P57" t="s">
+      <c r="Q57" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="58" spans="10:17">
+      <c r="Q58" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="59" spans="10:17">
+      <c r="Q59" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="58" spans="10:16">
-      <c r="P58" t="s">
+    <row r="60" spans="10:17">
+      <c r="Q60" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="59" spans="10:16">
-      <c r="P59" t="s">
+    <row r="61" spans="10:17">
+      <c r="Q61" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="60" spans="10:16">
-      <c r="P60" t="s">
+    <row r="62" spans="10:17">
+      <c r="Q62" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="61" spans="10:16">
-      <c r="P61" t="s">
+    <row r="63" spans="10:17">
+      <c r="Q63" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="62" spans="10:16">
-      <c r="P62" t="s">
+    <row r="64" spans="10:17">
+      <c r="Q64" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="63" spans="10:16">
-      <c r="P63" t="s">
+    <row r="65" spans="17:17">
+      <c r="Q65" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="64" spans="10:16">
-      <c r="P64" t="s">
+    <row r="66" spans="17:17">
+      <c r="Q66" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="65" spans="16:16">
-      <c r="P65" t="s">
+    <row r="67" spans="17:17">
+      <c r="Q67" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="66" spans="16:16">
-      <c r="P66" t="s">
+    <row r="68" spans="17:17">
+      <c r="Q68" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="67" spans="16:16">
-      <c r="P67" t="s">
+    <row r="69" spans="17:17">
+      <c r="Q69" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="68" spans="16:16">
-      <c r="P68" t="s">
+    <row r="70" spans="17:17">
+      <c r="Q70" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="69" spans="16:16">
-      <c r="P69" t="s">
+    <row r="71" spans="17:17">
+      <c r="Q71" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="70" spans="16:16">
-      <c r="P70" t="s">
+    <row r="72" spans="17:17">
+      <c r="Q72" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="71" spans="16:16">
-      <c r="P71" t="s">
+    <row r="73" spans="17:17">
+      <c r="Q73" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="72" spans="16:16">
-      <c r="P72" t="s">
+    <row r="74" spans="17:17">
+      <c r="Q74" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="73" spans="16:16">
-      <c r="P73" t="s">
+    <row r="75" spans="17:17">
+      <c r="Q75" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="74" spans="16:16">
-      <c r="P74" t="s">
+    <row r="76" spans="17:17">
+      <c r="Q76" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="75" spans="16:16">
-      <c r="P75" t="s">
+    <row r="77" spans="17:17">
+      <c r="Q77" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="76" spans="16:16">
-      <c r="P76" t="s">
+    <row r="78" spans="17:17">
+      <c r="Q78" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="77" spans="16:16">
-      <c r="P77" t="s">
+    <row r="79" spans="17:17">
+      <c r="Q79" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="78" spans="16:16">
-      <c r="P78" t="s">
+    <row r="80" spans="17:17">
+      <c r="Q80" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="79" spans="16:16">
-      <c r="P79" t="s">
+    <row r="81" spans="17:17">
+      <c r="Q81" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="80" spans="16:16">
-      <c r="P80" t="s">
+    <row r="82" spans="17:17">
+      <c r="Q82" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="81" spans="16:16">
-      <c r="P81" t="s">
+    <row r="83" spans="17:17">
+      <c r="Q83" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="82" spans="16:16">
-      <c r="P82" t="s">
+    <row r="84" spans="17:17">
+      <c r="Q84" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="83" spans="16:16">
-      <c r="P83" t="s">
+    <row r="85" spans="17:17">
+      <c r="Q85" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="84" spans="16:16">
-      <c r="P84" t="s">
+    <row r="86" spans="17:17">
+      <c r="Q86" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="85" spans="16:16">
-      <c r="P85" t="s">
+    <row r="87" spans="17:17">
+      <c r="Q87" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="86" spans="16:16">
-      <c r="P86" t="s">
+    <row r="88" spans="17:17">
+      <c r="Q88" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="87" spans="16:16">
-      <c r="P87" t="s">
+    <row r="89" spans="17:17">
+      <c r="Q89" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="88" spans="16:16">
-      <c r="P88" t="s">
+    <row r="90" spans="17:17">
+      <c r="Q90" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="89" spans="16:16">
-      <c r="P89" t="s">
+    <row r="91" spans="17:17">
+      <c r="Q91" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="90" spans="16:16">
-      <c r="P90" t="s">
+    <row r="92" spans="17:17">
+      <c r="Q92" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="91" spans="16:16">
-      <c r="P91" t="s">
+    <row r="93" spans="17:17">
+      <c r="Q93" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="92" spans="16:16">
-      <c r="P92" t="s">
+    <row r="94" spans="17:17">
+      <c r="Q94" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="93" spans="16:16">
-      <c r="P93" t="s">
+    <row r="95" spans="17:17">
+      <c r="Q95" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="94" spans="16:16">
-      <c r="P94" t="s">
+    <row r="96" spans="17:17">
+      <c r="Q96" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="95" spans="16:16">
-      <c r="P95" t="s">
+    <row r="97" spans="17:17">
+      <c r="Q97" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="96" spans="16:16">
-      <c r="P96" t="s">
+    <row r="98" spans="17:17">
+      <c r="Q98" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="97" spans="16:16">
-      <c r="P97" t="s">
+    <row r="99" spans="17:17">
+      <c r="Q99" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="98" spans="16:16">
-      <c r="P98" t="s">
+    <row r="100" spans="17:17">
+      <c r="Q100" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="99" spans="16:16">
-      <c r="P99" t="s">
+    <row r="101" spans="17:17">
+      <c r="Q101" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="100" spans="16:16">
-      <c r="P100" t="s">
+    <row r="102" spans="17:17">
+      <c r="Q102" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="101" spans="16:16">
-      <c r="P101" t="s">
+    <row r="103" spans="17:17">
+      <c r="Q103" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="102" spans="16:16">
-      <c r="P102" t="s">
+    <row r="104" spans="17:17">
+      <c r="Q104" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="103" spans="16:16">
-      <c r="P103" t="s">
+    <row r="105" spans="17:17">
+      <c r="Q105" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="104" spans="16:16">
-      <c r="P104" t="s">
+    <row r="106" spans="17:17">
+      <c r="Q106" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="105" spans="16:16">
-      <c r="P105" t="s">
+    <row r="107" spans="17:17">
+      <c r="Q107" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="106" spans="16:16">
-      <c r="P106" t="s">
+    <row r="108" spans="17:17">
+      <c r="Q108" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="107" spans="16:16">
-      <c r="P107" t="s">
+    <row r="109" spans="17:17">
+      <c r="Q109" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="108" spans="16:16">
-      <c r="P108" t="s">
+    <row r="110" spans="17:17">
+      <c r="Q110" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="109" spans="16:16">
-      <c r="P109" t="s">
+    <row r="111" spans="17:17">
+      <c r="Q111" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="110" spans="16:16">
-      <c r="P110" t="s">
+    <row r="112" spans="17:17">
+      <c r="Q112" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="111" spans="16:16">
-      <c r="P111" t="s">
+    <row r="113" spans="17:17">
+      <c r="Q113" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="112" spans="16:16">
-      <c r="P112" t="s">
+    <row r="114" spans="17:17">
+      <c r="Q114" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="113" spans="16:16">
-      <c r="P113" t="s">
+    <row r="115" spans="17:17">
+      <c r="Q115" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="114" spans="16:16">
-      <c r="P114" t="s">
+    <row r="116" spans="17:17">
+      <c r="Q116" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="115" spans="16:16">
-      <c r="P115" t="s">
+    <row r="117" spans="17:17">
+      <c r="Q117" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="116" spans="16:16">
-      <c r="P116" t="s">
+    <row r="118" spans="17:17">
+      <c r="Q118" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="117" spans="16:16">
-      <c r="P117" t="s">
+    <row r="119" spans="17:17">
+      <c r="Q119" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="118" spans="16:16">
-      <c r="P118" t="s">
+    <row r="120" spans="17:17">
+      <c r="Q120" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="119" spans="16:16">
-      <c r="P119" t="s">
+    <row r="121" spans="17:17">
+      <c r="Q121" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="120" spans="16:16">
-      <c r="P120" t="s">
+    <row r="122" spans="17:17">
+      <c r="Q122" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="121" spans="16:16">
-      <c r="P121" t="s">
+    <row r="123" spans="17:17">
+      <c r="Q123" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="122" spans="16:16">
-      <c r="P122" t="s">
+    <row r="124" spans="17:17">
+      <c r="Q124" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="123" spans="16:16">
-      <c r="P123" t="s">
+    <row r="125" spans="17:17">
+      <c r="Q125" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="124" spans="16:16">
-      <c r="P124" t="s">
+    <row r="126" spans="17:17">
+      <c r="Q126" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="125" spans="16:16">
-      <c r="P125" t="s">
+    <row r="127" spans="17:17">
+      <c r="Q127" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="126" spans="16:16">
-      <c r="P126" t="s">
+    <row r="128" spans="17:17">
+      <c r="Q128" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="127" spans="16:16">
-      <c r="P127" t="s">
+    <row r="129" spans="17:17">
+      <c r="Q129" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="128" spans="16:16">
-      <c r="P128" t="s">
+    <row r="130" spans="17:17">
+      <c r="Q130" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="129" spans="16:16">
-      <c r="P129" t="s">
+    <row r="131" spans="17:17">
+      <c r="Q131" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="130" spans="16:16">
-      <c r="P130" t="s">
+    <row r="132" spans="17:17">
+      <c r="Q132" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="131" spans="16:16">
-      <c r="P131" t="s">
+    <row r="133" spans="17:17">
+      <c r="Q133" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="132" spans="16:16">
-      <c r="P132" t="s">
+    <row r="134" spans="17:17">
+      <c r="Q134" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="133" spans="16:16">
-      <c r="P133" t="s">
+    <row r="135" spans="17:17">
+      <c r="Q135" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="134" spans="16:16">
-      <c r="P134" t="s">
+    <row r="136" spans="17:17">
+      <c r="Q136" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="135" spans="16:16">
-      <c r="P135" t="s">
+    <row r="137" spans="17:17">
+      <c r="Q137" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="136" spans="16:16">
-      <c r="P136" t="s">
+    <row r="138" spans="17:17">
+      <c r="Q138" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="137" spans="16:16">
-      <c r="P137" t="s">
+    <row r="139" spans="17:17">
+      <c r="Q139" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="138" spans="16:16">
-      <c r="P138" t="s">
+    <row r="140" spans="17:17">
+      <c r="Q140" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="139" spans="16:16">
-      <c r="P139" t="s">
+    <row r="141" spans="17:17">
+      <c r="Q141" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="140" spans="16:16">
-      <c r="P140" t="s">
+    <row r="142" spans="17:17">
+      <c r="Q142" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="141" spans="16:16">
-      <c r="P141" t="s">
+    <row r="143" spans="17:17">
+      <c r="Q143" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="142" spans="16:16">
-      <c r="P142" t="s">
+    <row r="144" spans="17:17">
+      <c r="Q144" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="143" spans="16:16">
-      <c r="P143" t="s">
+    <row r="145" spans="17:17">
+      <c r="Q145" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="144" spans="16:16">
-      <c r="P144" t="s">
+    <row r="146" spans="17:17">
+      <c r="Q146" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="145" spans="16:16">
-      <c r="P145" t="s">
+    <row r="147" spans="17:17">
+      <c r="Q147" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="146" spans="16:16">
-      <c r="P146" t="s">
+    <row r="148" spans="17:17">
+      <c r="Q148" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="147" spans="16:16">
-      <c r="P147" t="s">
+    <row r="149" spans="17:17">
+      <c r="Q149" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="148" spans="16:16">
-      <c r="P148" t="s">
+    <row r="150" spans="17:17">
+      <c r="Q150" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="149" spans="16:16">
-      <c r="P149" t="s">
+    <row r="151" spans="17:17">
+      <c r="Q151" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="150" spans="16:16">
-      <c r="P150" t="s">
+    <row r="152" spans="17:17">
+      <c r="Q152" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="151" spans="16:16">
-      <c r="P151" t="s">
+    <row r="153" spans="17:17">
+      <c r="Q153" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="152" spans="16:16">
-      <c r="P152" t="s">
+    <row r="154" spans="17:17">
+      <c r="Q154" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="153" spans="16:16">
-      <c r="P153" t="s">
+    <row r="155" spans="17:17">
+      <c r="Q155" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="154" spans="16:16">
-      <c r="P154" t="s">
+    <row r="156" spans="17:17">
+      <c r="Q156" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="155" spans="16:16">
-      <c r="P155" t="s">
+    <row r="157" spans="17:17">
+      <c r="Q157" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="156" spans="16:16">
-      <c r="P156" t="s">
+    <row r="158" spans="17:17">
+      <c r="Q158" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="157" spans="16:16">
-      <c r="P157" t="s">
+    <row r="159" spans="17:17">
+      <c r="Q159" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="158" spans="16:16">
-      <c r="P158" t="s">
+    <row r="160" spans="17:17">
+      <c r="Q160" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="159" spans="16:16">
-      <c r="P159" t="s">
+    <row r="161" spans="17:17">
+      <c r="Q161" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="160" spans="16:16">
-      <c r="P160" t="s">
+    <row r="162" spans="17:17">
+      <c r="Q162" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="161" spans="16:16">
-      <c r="P161" t="s">
+    <row r="163" spans="17:17">
+      <c r="Q163" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="162" spans="16:16">
-      <c r="P162" t="s">
+    <row r="164" spans="17:17">
+      <c r="Q164" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="163" spans="16:16">
-      <c r="P163" t="s">
+    <row r="165" spans="17:17">
+      <c r="Q165" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="164" spans="16:16">
-      <c r="P164" t="s">
+    <row r="166" spans="17:17">
+      <c r="Q166" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="165" spans="16:16">
-      <c r="P165" t="s">
+    <row r="167" spans="17:17">
+      <c r="Q167" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="166" spans="16:16">
-      <c r="P166" t="s">
+    <row r="168" spans="17:17">
+      <c r="Q168" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="167" spans="16:16">
-      <c r="P167" t="s">
+    <row r="169" spans="17:17">
+      <c r="Q169" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="168" spans="16:16">
-      <c r="P168" t="s">
+    <row r="170" spans="17:17">
+      <c r="Q170" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="169" spans="16:16">
-      <c r="P169" t="s">
+    <row r="171" spans="17:17">
+      <c r="Q171" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="170" spans="16:16">
-      <c r="P170" t="s">
+    <row r="172" spans="17:17">
+      <c r="Q172" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="171" spans="16:16">
-      <c r="P171" t="s">
+    <row r="173" spans="17:17">
+      <c r="Q173" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="172" spans="16:16">
-      <c r="P172" t="s">
+    <row r="174" spans="17:17">
+      <c r="Q174" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="173" spans="16:16">
-      <c r="P173" t="s">
+    <row r="175" spans="17:17">
+      <c r="Q175" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="174" spans="16:16">
-      <c r="P174" t="s">
+    <row r="176" spans="17:17">
+      <c r="Q176" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="175" spans="16:16">
-      <c r="P175" t="s">
+    <row r="177" spans="17:17">
+      <c r="Q177" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="176" spans="16:16">
-      <c r="P176" t="s">
+    <row r="178" spans="17:17">
+      <c r="Q178" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="177" spans="16:16">
-      <c r="P177" t="s">
+    <row r="179" spans="17:17">
+      <c r="Q179" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="178" spans="16:16">
-      <c r="P178" t="s">
+    <row r="180" spans="17:17">
+      <c r="Q180" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="179" spans="16:16">
-      <c r="P179" t="s">
+    <row r="181" spans="17:17">
+      <c r="Q181" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="180" spans="16:16">
-      <c r="P180" t="s">
+    <row r="182" spans="17:17">
+      <c r="Q182" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="181" spans="16:16">
-      <c r="P181" t="s">
+    <row r="183" spans="17:17">
+      <c r="Q183" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="182" spans="16:16">
-      <c r="P182" t="s">
+    <row r="184" spans="17:17">
+      <c r="Q184" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="183" spans="16:16">
-      <c r="P183" t="s">
+    <row r="185" spans="17:17">
+      <c r="Q185" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="184" spans="16:16">
-      <c r="P184" t="s">
+    <row r="186" spans="17:17">
+      <c r="Q186" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="185" spans="16:16">
-      <c r="P185" t="s">
+    <row r="187" spans="17:17">
+      <c r="Q187" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="186" spans="16:16">
-      <c r="P186" t="s">
+    <row r="188" spans="17:17">
+      <c r="Q188" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="187" spans="16:16">
-      <c r="P187" t="s">
+    <row r="189" spans="17:17">
+      <c r="Q189" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="188" spans="16:16">
-      <c r="P188" t="s">
+    <row r="190" spans="17:17">
+      <c r="Q190" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="189" spans="16:16">
-      <c r="P189" t="s">
+    <row r="191" spans="17:17">
+      <c r="Q191" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="190" spans="16:16">
-      <c r="P190" t="s">
+    <row r="192" spans="17:17">
+      <c r="Q192" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="191" spans="16:16">
-      <c r="P191" t="s">
+    <row r="193" spans="17:17">
+      <c r="Q193" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="192" spans="16:16">
-      <c r="P192" t="s">
+    <row r="194" spans="17:17">
+      <c r="Q194" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="193" spans="16:16">
-      <c r="P193" t="s">
+    <row r="195" spans="17:17">
+      <c r="Q195" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="194" spans="16:16">
-      <c r="P194" t="s">
+    <row r="196" spans="17:17">
+      <c r="Q196" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="195" spans="16:16">
-      <c r="P195" t="s">
+    <row r="197" spans="17:17">
+      <c r="Q197" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="196" spans="16:16">
-      <c r="P196" t="s">
+    <row r="198" spans="17:17">
+      <c r="Q198" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="197" spans="16:16">
-      <c r="P197" t="s">
+    <row r="199" spans="17:17">
+      <c r="Q199" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="198" spans="16:16">
-      <c r="P198" t="s">
+    <row r="200" spans="17:17">
+      <c r="Q200" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="199" spans="16:16">
-      <c r="P199" t="s">
+    <row r="201" spans="17:17">
+      <c r="Q201" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="200" spans="16:16">
-      <c r="P200" t="s">
+    <row r="202" spans="17:17">
+      <c r="Q202" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="201" spans="16:16">
-      <c r="P201" t="s">
+    <row r="203" spans="17:17">
+      <c r="Q203" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="202" spans="16:16">
-      <c r="P202" t="s">
+    <row r="204" spans="17:17">
+      <c r="Q204" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="203" spans="16:16">
-      <c r="P203" t="s">
+    <row r="205" spans="17:17">
+      <c r="Q205" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="204" spans="16:16">
-      <c r="P204" t="s">
+    <row r="206" spans="17:17">
+      <c r="Q206" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="205" spans="16:16">
-      <c r="P205" t="s">
+    <row r="207" spans="17:17">
+      <c r="Q207" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="206" spans="16:16">
-      <c r="P206" t="s">
+    <row r="208" spans="17:17">
+      <c r="Q208" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="207" spans="16:16">
-      <c r="P207" t="s">
+    <row r="209" spans="17:17">
+      <c r="Q209" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="208" spans="16:16">
-      <c r="P208" t="s">
+    <row r="210" spans="17:17">
+      <c r="Q210" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="209" spans="16:16">
-      <c r="P209" t="s">
+    <row r="211" spans="17:17">
+      <c r="Q211" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="210" spans="16:16">
-      <c r="P210" t="s">
+    <row r="212" spans="17:17">
+      <c r="Q212" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="211" spans="16:16">
-      <c r="P211" t="s">
+    <row r="213" spans="17:17">
+      <c r="Q213" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="212" spans="16:16">
-      <c r="P212" t="s">
+    <row r="214" spans="17:17">
+      <c r="Q214" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="213" spans="16:16">
-      <c r="P213" t="s">
+    <row r="215" spans="17:17">
+      <c r="Q215" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="214" spans="16:16">
-      <c r="P214" t="s">
+    <row r="216" spans="17:17">
+      <c r="Q216" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="215" spans="16:16">
-      <c r="P215" t="s">
+    <row r="217" spans="17:17">
+      <c r="Q217" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="216" spans="16:16">
-      <c r="P216" t="s">
+    <row r="218" spans="17:17">
+      <c r="Q218" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="217" spans="16:16">
-      <c r="P217" t="s">
+    <row r="219" spans="17:17">
+      <c r="Q219" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="218" spans="16:16">
-      <c r="P218" t="s">
+    <row r="220" spans="17:17">
+      <c r="Q220" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="219" spans="16:16">
-      <c r="P219" t="s">
+    <row r="221" spans="17:17">
+      <c r="Q221" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="220" spans="16:16">
-      <c r="P220" t="s">
+    <row r="222" spans="17:17">
+      <c r="Q222" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="221" spans="16:16">
-      <c r="P221" t="s">
+    <row r="223" spans="17:17">
+      <c r="Q223" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="222" spans="16:16">
-      <c r="P222" t="s">
+    <row r="224" spans="17:17">
+      <c r="Q224" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="223" spans="16:16">
-      <c r="P223" t="s">
+    <row r="225" spans="17:17">
+      <c r="Q225" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="224" spans="16:16">
-      <c r="P224" t="s">
+    <row r="226" spans="17:17">
+      <c r="Q226" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="225" spans="16:16">
-      <c r="P225" t="s">
+    <row r="227" spans="17:17">
+      <c r="Q227" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="226" spans="16:16">
-      <c r="P226" t="s">
+    <row r="228" spans="17:17">
+      <c r="Q228" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="227" spans="16:16">
-      <c r="P227" t="s">
+    <row r="229" spans="17:17">
+      <c r="Q229" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="228" spans="16:16">
-      <c r="P228" t="s">
+    <row r="230" spans="17:17">
+      <c r="Q230" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="229" spans="16:16">
-      <c r="P229" t="s">
+    <row r="231" spans="17:17">
+      <c r="Q231" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="230" spans="16:16">
-      <c r="P230" t="s">
+    <row r="232" spans="17:17">
+      <c r="Q232" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="231" spans="16:16">
-      <c r="P231" t="s">
+    <row r="233" spans="17:17">
+      <c r="Q233" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="232" spans="16:16">
-      <c r="P232" t="s">
+    <row r="234" spans="17:17">
+      <c r="Q234" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="233" spans="16:16">
-      <c r="P233" t="s">
+    <row r="235" spans="17:17">
+      <c r="Q235" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="234" spans="16:16">
-      <c r="P234" t="s">
+    <row r="236" spans="17:17">
+      <c r="Q236" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="235" spans="16:16">
-      <c r="P235" t="s">
+    <row r="237" spans="17:17">
+      <c r="Q237" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="236" spans="16:16">
-      <c r="P236" t="s">
+    <row r="238" spans="17:17">
+      <c r="Q238" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="237" spans="16:16">
-      <c r="P237" t="s">
+    <row r="239" spans="17:17">
+      <c r="Q239" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="238" spans="16:16">
-      <c r="P238" t="s">
+    <row r="240" spans="17:17">
+      <c r="Q240" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="239" spans="16:16">
-      <c r="P239" t="s">
+    <row r="241" spans="17:17">
+      <c r="Q241" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="240" spans="16:16">
-      <c r="P240" t="s">
+    <row r="242" spans="17:17">
+      <c r="Q242" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="241" spans="16:16">
-      <c r="P241" t="s">
+    <row r="243" spans="17:17">
+      <c r="Q243" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="242" spans="16:16">
-      <c r="P242" t="s">
+    <row r="244" spans="17:17">
+      <c r="Q244" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="243" spans="16:16">
-      <c r="P243" t="s">
+    <row r="245" spans="17:17">
+      <c r="Q245" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="244" spans="16:16">
-      <c r="P244" t="s">
+    <row r="246" spans="17:17">
+      <c r="Q246" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="245" spans="16:16">
-      <c r="P245" t="s">
+    <row r="247" spans="17:17">
+      <c r="Q247" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="246" spans="16:16">
-      <c r="P246" t="s">
+    <row r="248" spans="17:17">
+      <c r="Q248" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="247" spans="16:16">
-      <c r="P247" t="s">
+    <row r="249" spans="17:17">
+      <c r="Q249" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="248" spans="16:16">
-      <c r="P248" t="s">
+    <row r="250" spans="17:17">
+      <c r="Q250" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="249" spans="16:16">
-      <c r="P249" t="s">
+    <row r="251" spans="17:17">
+      <c r="Q251" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="250" spans="16:16">
-      <c r="P250" t="s">
+    <row r="252" spans="17:17">
+      <c r="Q252" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="251" spans="16:16">
-      <c r="P251" t="s">
+    <row r="253" spans="17:17">
+      <c r="Q253" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="252" spans="16:16">
-      <c r="P252" t="s">
+    <row r="254" spans="17:17">
+      <c r="Q254" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="253" spans="16:16">
-      <c r="P253" t="s">
+    <row r="255" spans="17:17">
+      <c r="Q255" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="254" spans="16:16">
-      <c r="P254" t="s">
+    <row r="256" spans="17:17">
+      <c r="Q256" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="255" spans="16:16">
-      <c r="P255" t="s">
+    <row r="257" spans="17:17">
+      <c r="Q257" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="256" spans="16:16">
-      <c r="P256" t="s">
+    <row r="258" spans="17:17">
+      <c r="Q258" t="s">
         <v>383</v>
-      </c>
-    </row>
-    <row r="257" spans="16:16">
-      <c r="P257" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="258" spans="16:16">
-      <c r="P258" t="s">
-        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First attempt at spit and style
>
</commit_message>
<xml_diff>
--- a/data/MetaMaster.xlsx
+++ b/data/MetaMaster.xlsx
@@ -1344,12 +1344,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1366,7 +1372,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1376,6 +1382,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1792,7 +1799,7 @@
       <pane xSplit="1" ySplit="13" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12"/>
@@ -2016,8 +2023,11 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
     </row>
+    <row r="13" spans="1:26">
+      <c r="D13" s="1"/>
+    </row>
     <row r="15" spans="1:26">
-      <c r="A15" t="s">
+      <c r="A15" s="7" t="s">
         <v>390</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More checking fo datavalidation
</commit_message>
<xml_diff>
--- a/data/MetaMaster.xlsx
+++ b/data/MetaMaster.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="19155" windowHeight="5790" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="19155" windowHeight="5790"/>
   </bookViews>
   <sheets>
     <sheet name="DropDowns" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="470">
   <si>
     <t>Easting</t>
   </si>
@@ -454,9 +454,6 @@
     <t>Unit for Observation's Value</t>
   </si>
   <si>
-    <t>Derivation Factor for Observation</t>
-  </si>
-  <si>
     <t>STOP</t>
   </si>
   <si>
@@ -1174,9 +1171,6 @@
     <t>External Sheet</t>
   </si>
   <si>
-    <t>Extrenal Sheet to be used as uri base</t>
-  </si>
-  <si>
     <t>Overrides the normal pattern of using the local DOI and sheet as the base URI. Format is [doi]sheetName</t>
   </si>
   <si>
@@ -1448,6 +1442,15 @@
   </si>
   <si>
     <t>WillbyAttributeGroup</t>
+  </si>
+  <si>
+    <t>Unexpected Ignore Zero</t>
+  </si>
+  <si>
+    <t>Extrenal Sheet for uri base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Derivation Factor </t>
   </si>
 </sst>
 </file>
@@ -1814,11 +1817,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z117"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="11" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12"/>
@@ -1848,13 +1851,13 @@
         <v>132</v>
       </c>
       <c r="F1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" t="s">
         <v>138</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>139</v>
-      </c>
-      <c r="H1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:26">
@@ -1862,7 +1865,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
@@ -1871,68 +1874,71 @@
         <v>133</v>
       </c>
       <c r="F2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="G2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D3" t="s">
         <v>134</v>
       </c>
       <c r="E3" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H3" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" t="s">
-        <v>377</v>
+        <v>468</v>
       </c>
       <c r="E4" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
+        <v>377</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="D5" t="s">
+        <v>377</v>
+      </c>
+      <c r="E5" t="s">
+        <v>378</v>
+      </c>
+      <c r="F5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G5" t="s">
+        <v>467</v>
+      </c>
+      <c r="H5" t="s">
         <v>379</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>388</v>
-      </c>
-      <c r="D5" t="s">
-        <v>379</v>
-      </c>
-      <c r="E5" t="s">
-        <v>380</v>
-      </c>
-      <c r="F5" t="s">
-        <v>138</v>
-      </c>
-      <c r="G5" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -1940,16 +1946,16 @@
         <v>123</v>
       </c>
       <c r="C6" t="s">
+        <v>402</v>
+      </c>
+      <c r="F6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G6" t="s">
+        <v>403</v>
+      </c>
+      <c r="H6" t="s">
         <v>404</v>
-      </c>
-      <c r="F6" t="s">
-        <v>138</v>
-      </c>
-      <c r="G6" t="s">
-        <v>405</v>
-      </c>
-      <c r="H6" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -1957,22 +1963,22 @@
         <v>11</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D7" t="s">
         <v>135</v>
       </c>
       <c r="E7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="G7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -1980,22 +1986,22 @@
         <v>30</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D8" t="s">
         <v>136</v>
       </c>
       <c r="E8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F8" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="G8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H8" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -2003,36 +2009,36 @@
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D9" t="s">
-        <v>137</v>
+        <v>469</v>
       </c>
       <c r="E9" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F9" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="G9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H9" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
+        <v>458</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="D10" t="s">
+        <v>459</v>
+      </c>
+      <c r="E10" t="s">
         <v>460</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>466</v>
-      </c>
-      <c r="D10" t="s">
-        <v>461</v>
-      </c>
-      <c r="E10" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -2052,10 +2058,10 @@
     </row>
     <row r="12" spans="1:26">
       <c r="B12" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C12" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D12">
         <v>32</v>
@@ -2072,7 +2078,7 @@
     </row>
     <row r="13" spans="1:26">
       <c r="A13" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C13">
         <f t="shared" ref="C13:H22" si="0">LEN(C1)</f>
@@ -2155,7 +2161,7 @@
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
@@ -2188,11 +2194,11 @@
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="H17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2280,7 +2286,7 @@
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
@@ -2322,7 +2328,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="B24" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C24" s="4"/>
     </row>
@@ -2374,7 +2380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X258"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -2407,7 +2413,7 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -2420,25 +2426,25 @@
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>430</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>432</v>
       </c>
       <c r="P1" s="2"/>
       <c r="Q1" s="2" t="s">
@@ -2454,7 +2460,7 @@
         <v>25</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="V1" t="s">
         <v>39</v>
@@ -2502,10 +2508,10 @@
         <v>16</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>38</v>
@@ -2524,7 +2530,7 @@
         <v>26</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>38</v>
@@ -2533,7 +2539,7 @@
         <v>31</v>
       </c>
       <c r="X2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="15">
@@ -2561,17 +2567,17 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
@@ -2608,7 +2614,7 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -2619,13 +2625,13 @@
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="N4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
@@ -2656,25 +2662,25 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="G5" t="s">
         <v>37</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="N5" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>76</v>
@@ -2706,7 +2712,7 @@
         <v>124</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>22</v>
@@ -2715,13 +2721,13 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="N6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
@@ -2749,10 +2755,10 @@
         <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>126</v>
@@ -2764,7 +2770,7 @@
         <v>38</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="N7" t="s">
         <v>12</v>
@@ -2772,7 +2778,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="R7" t="s">
         <v>41</v>
@@ -2793,10 +2799,10 @@
         <v>128</v>
       </c>
       <c r="E8" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F8" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>23</v>
@@ -2806,10 +2812,10 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="N8" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
@@ -2835,10 +2841,10 @@
         <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>10</v>
@@ -2868,7 +2874,7 @@
     </row>
     <row r="10" spans="1:24" ht="15">
       <c r="B10" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>125</v>
@@ -2880,7 +2886,7 @@
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>7</v>
@@ -2905,7 +2911,7 @@
     </row>
     <row r="11" spans="1:24" ht="15">
       <c r="C11" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>22</v>
@@ -2914,10 +2920,10 @@
         <v>21</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="H11" s="2"/>
       <c r="J11" s="2"/>
@@ -2943,7 +2949,7 @@
         <v>127</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -2963,13 +2969,13 @@
     </row>
     <row r="13" spans="1:24" ht="15">
       <c r="D13" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -2990,13 +2996,13 @@
     </row>
     <row r="14" spans="1:24" ht="15">
       <c r="E14" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F14" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="Q14" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="S14" s="2"/>
       <c r="X14" t="s">
@@ -3005,7 +3011,7 @@
     </row>
     <row r="15" spans="1:24" ht="15">
       <c r="F15" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="Q15" s="2" t="s">
         <v>85</v>
@@ -3017,7 +3023,7 @@
     </row>
     <row r="16" spans="1:24" ht="15">
       <c r="F16" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="Q16" s="2" t="s">
         <v>86</v>
@@ -3029,7 +3035,7 @@
     </row>
     <row r="17" spans="1:24" ht="15">
       <c r="F17" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="Q17" s="2" t="s">
         <v>87</v>
@@ -3054,7 +3060,7 @@
     <row r="19" spans="1:24" ht="15">
       <c r="C19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -3066,7 +3072,7 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="S19" s="2"/>
       <c r="X19" t="s">
@@ -3076,7 +3082,7 @@
     <row r="20" spans="1:24" ht="15">
       <c r="C20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -3099,7 +3105,7 @@
     <row r="21" spans="1:24" ht="15">
       <c r="C21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -3124,7 +3130,7 @@
       <c r="C22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -3158,7 +3164,7 @@
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="S23" s="2"/>
       <c r="X23" t="s">
@@ -3199,7 +3205,7 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="S25" s="2"/>
       <c r="X25" t="s">
@@ -3257,7 +3263,7 @@
       </c>
       <c r="S29" s="2"/>
       <c r="X29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:24" ht="15">
@@ -3267,7 +3273,7 @@
       </c>
       <c r="S30" s="2"/>
       <c r="X30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:24" ht="15">
@@ -3277,7 +3283,7 @@
       </c>
       <c r="S31" s="2"/>
       <c r="X31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:24" ht="15">
@@ -3287,7 +3293,7 @@
       </c>
       <c r="S32" s="2"/>
       <c r="X32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="4:24" ht="15">
@@ -3297,7 +3303,7 @@
       </c>
       <c r="S33" s="2"/>
       <c r="X33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="4:24" ht="15">
@@ -3307,7 +3313,7 @@
       </c>
       <c r="S34" s="2"/>
       <c r="X34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="4:24" ht="15">
@@ -3317,17 +3323,17 @@
       </c>
       <c r="S35" s="2"/>
       <c r="X35" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="4:24" ht="15">
       <c r="D36" s="2"/>
       <c r="Q36" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="S36" s="2"/>
       <c r="X36" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="4:24" ht="15">
@@ -3337,7 +3343,7 @@
       </c>
       <c r="S37" s="2"/>
       <c r="X37" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="4:24" ht="15">
@@ -3347,7 +3353,7 @@
       </c>
       <c r="S38" s="2"/>
       <c r="X38" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="4:24" ht="15">
@@ -3357,7 +3363,7 @@
       </c>
       <c r="S39" s="2"/>
       <c r="X39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="4:24" ht="15">
@@ -3366,7 +3372,7 @@
       </c>
       <c r="S40" s="2"/>
       <c r="X40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="4:24" ht="15">
@@ -3375,16 +3381,16 @@
       </c>
       <c r="S41" s="2"/>
       <c r="X41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="4:24" ht="15">
       <c r="Q42" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="S42" s="2"/>
       <c r="X42" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="4:24" ht="15">
@@ -3393,7 +3399,7 @@
       </c>
       <c r="S43" s="2"/>
       <c r="X43" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="4:24" ht="15">
@@ -3402,25 +3408,25 @@
       </c>
       <c r="S44" s="2"/>
       <c r="X44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="4:24" ht="15">
       <c r="Q45" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="S45" s="2"/>
       <c r="X45" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="46" spans="4:24" ht="15">
       <c r="Q46" s="6" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="S46" s="2"/>
       <c r="X46" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="4:24" ht="15">
@@ -3429,7 +3435,7 @@
       </c>
       <c r="S47" s="2"/>
       <c r="X47" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="48" spans="4:24" ht="15">
@@ -3437,7 +3443,7 @@
         <v>107</v>
       </c>
       <c r="X48" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="17:24">
@@ -3445,7 +3451,7 @@
         <v>18</v>
       </c>
       <c r="X49" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="50" spans="17:24" ht="15">
@@ -3453,7 +3459,7 @@
         <v>104</v>
       </c>
       <c r="X50" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="17:24" ht="15">
@@ -3461,7 +3467,7 @@
         <v>108</v>
       </c>
       <c r="X51" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="52" spans="17:24" ht="15">
@@ -3469,7 +3475,7 @@
         <v>109</v>
       </c>
       <c r="X52" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="53" spans="17:24" ht="15">
@@ -3477,7 +3483,7 @@
         <v>110</v>
       </c>
       <c r="X53" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="54" spans="17:24" ht="15">
@@ -3485,7 +3491,7 @@
         <v>111</v>
       </c>
       <c r="X54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="17:24" ht="15">
@@ -3493,7 +3499,7 @@
         <v>113</v>
       </c>
       <c r="X55" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="56" spans="17:24" ht="15">
@@ -3501,7 +3507,7 @@
         <v>112</v>
       </c>
       <c r="X56" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="57" spans="17:24" ht="15">
@@ -3509,1012 +3515,1012 @@
         <v>114</v>
       </c>
       <c r="X57" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="58" spans="17:24">
       <c r="X58" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="59" spans="17:24">
       <c r="X59" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="60" spans="17:24">
       <c r="X60" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="61" spans="17:24">
       <c r="X61" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" spans="17:24">
       <c r="X62" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="63" spans="17:24">
       <c r="X63" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" spans="17:24">
       <c r="X64" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" spans="24:24">
       <c r="X65" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="66" spans="24:24">
       <c r="X66" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="67" spans="24:24">
       <c r="X67" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="68" spans="24:24">
       <c r="X68" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="69" spans="24:24">
       <c r="X69" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70" spans="24:24">
       <c r="X70" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="71" spans="24:24">
       <c r="X71" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="72" spans="24:24">
       <c r="X72" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="73" spans="24:24">
       <c r="X73" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74" spans="24:24">
       <c r="X74" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="75" spans="24:24">
       <c r="X75" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="76" spans="24:24">
       <c r="X76" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="77" spans="24:24">
       <c r="X77" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="78" spans="24:24">
       <c r="X78" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="79" spans="24:24">
       <c r="X79" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="80" spans="24:24">
       <c r="X80" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="81" spans="24:24">
       <c r="X81" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="82" spans="24:24">
       <c r="X82" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="83" spans="24:24">
       <c r="X83" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="84" spans="24:24">
       <c r="X84" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="85" spans="24:24">
       <c r="X85" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="86" spans="24:24">
       <c r="X86" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="87" spans="24:24">
       <c r="X87" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="88" spans="24:24">
       <c r="X88" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="89" spans="24:24">
       <c r="X89" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="90" spans="24:24">
       <c r="X90" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="91" spans="24:24">
       <c r="X91" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="92" spans="24:24">
       <c r="X92" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="93" spans="24:24">
       <c r="X93" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="94" spans="24:24">
       <c r="X94" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="95" spans="24:24">
       <c r="X95" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="96" spans="24:24">
       <c r="X96" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="97" spans="24:24">
       <c r="X97" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="98" spans="24:24">
       <c r="X98" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="99" spans="24:24">
       <c r="X99" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="100" spans="24:24">
       <c r="X100" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="101" spans="24:24">
       <c r="X101" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="102" spans="24:24">
       <c r="X102" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="103" spans="24:24">
       <c r="X103" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="104" spans="24:24">
       <c r="X104" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="105" spans="24:24">
       <c r="X105" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="106" spans="24:24">
       <c r="X106" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="107" spans="24:24">
       <c r="X107" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="108" spans="24:24">
       <c r="X108" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="109" spans="24:24">
       <c r="X109" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="110" spans="24:24">
       <c r="X110" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="111" spans="24:24">
       <c r="X111" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="112" spans="24:24">
       <c r="X112" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="113" spans="24:24">
       <c r="X113" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="114" spans="24:24">
       <c r="X114" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="115" spans="24:24">
       <c r="X115" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="116" spans="24:24">
       <c r="X116" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="117" spans="24:24">
       <c r="X117" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="118" spans="24:24">
       <c r="X118" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="119" spans="24:24">
       <c r="X119" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="120" spans="24:24">
       <c r="X120" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="121" spans="24:24">
       <c r="X121" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="122" spans="24:24">
       <c r="X122" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="123" spans="24:24">
       <c r="X123" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="124" spans="24:24">
       <c r="X124" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="125" spans="24:24">
       <c r="X125" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="126" spans="24:24">
       <c r="X126" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="127" spans="24:24">
       <c r="X127" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="128" spans="24:24">
       <c r="X128" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="129" spans="24:24">
       <c r="X129" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="130" spans="24:24">
       <c r="X130" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="131" spans="24:24">
       <c r="X131" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="132" spans="24:24">
       <c r="X132" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="133" spans="24:24">
       <c r="X133" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="134" spans="24:24">
       <c r="X134" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="135" spans="24:24">
       <c r="X135" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="136" spans="24:24">
       <c r="X136" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="137" spans="24:24">
       <c r="X137" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="138" spans="24:24">
       <c r="X138" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="139" spans="24:24">
       <c r="X139" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="140" spans="24:24">
       <c r="X140" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="141" spans="24:24">
       <c r="X141" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="142" spans="24:24">
       <c r="X142" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="143" spans="24:24">
       <c r="X143" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="144" spans="24:24">
       <c r="X144" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="145" spans="24:24">
       <c r="X145" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="146" spans="24:24">
       <c r="X146" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="147" spans="24:24">
       <c r="X147" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="148" spans="24:24">
       <c r="X148" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="149" spans="24:24">
       <c r="X149" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="150" spans="24:24">
       <c r="X150" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="151" spans="24:24">
       <c r="X151" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="152" spans="24:24">
       <c r="X152" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="153" spans="24:24">
       <c r="X153" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="154" spans="24:24">
       <c r="X154" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="155" spans="24:24">
       <c r="X155" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="156" spans="24:24">
       <c r="X156" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="157" spans="24:24">
       <c r="X157" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="158" spans="24:24">
       <c r="X158" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="159" spans="24:24">
       <c r="X159" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="160" spans="24:24">
       <c r="X160" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="161" spans="24:24">
       <c r="X161" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="162" spans="24:24">
       <c r="X162" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="163" spans="24:24">
       <c r="X163" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="164" spans="24:24">
       <c r="X164" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="165" spans="24:24">
       <c r="X165" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="166" spans="24:24">
       <c r="X166" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="167" spans="24:24">
       <c r="X167" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="168" spans="24:24">
       <c r="X168" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="169" spans="24:24">
       <c r="X169" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="170" spans="24:24">
       <c r="X170" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="171" spans="24:24">
       <c r="X171" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="172" spans="24:24">
       <c r="X172" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="173" spans="24:24">
       <c r="X173" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="174" spans="24:24">
       <c r="X174" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="175" spans="24:24">
       <c r="X175" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="176" spans="24:24">
       <c r="X176" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="177" spans="24:24">
       <c r="X177" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="178" spans="24:24">
       <c r="X178" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="179" spans="24:24">
       <c r="X179" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="180" spans="24:24">
       <c r="X180" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="181" spans="24:24">
       <c r="X181" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="182" spans="24:24">
       <c r="X182" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="183" spans="24:24">
       <c r="X183" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="184" spans="24:24">
       <c r="X184" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="185" spans="24:24">
       <c r="X185" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="186" spans="24:24">
       <c r="X186" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="187" spans="24:24">
       <c r="X187" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="188" spans="24:24">
       <c r="X188" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="189" spans="24:24">
       <c r="X189" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="190" spans="24:24">
       <c r="X190" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="191" spans="24:24">
       <c r="X191" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="192" spans="24:24">
       <c r="X192" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="193" spans="24:24">
       <c r="X193" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="194" spans="24:24">
       <c r="X194" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="195" spans="24:24">
       <c r="X195" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="196" spans="24:24">
       <c r="X196" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="197" spans="24:24">
       <c r="X197" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="198" spans="24:24">
       <c r="X198" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="199" spans="24:24">
       <c r="X199" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="200" spans="24:24">
       <c r="X200" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="201" spans="24:24">
       <c r="X201" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="202" spans="24:24">
       <c r="X202" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="203" spans="24:24">
       <c r="X203" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="204" spans="24:24">
       <c r="X204" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="205" spans="24:24">
       <c r="X205" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="206" spans="24:24">
       <c r="X206" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="207" spans="24:24">
       <c r="X207" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="208" spans="24:24">
       <c r="X208" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="209" spans="24:24">
       <c r="X209" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="210" spans="24:24">
       <c r="X210" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="211" spans="24:24">
       <c r="X211" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="212" spans="24:24">
       <c r="X212" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="213" spans="24:24">
       <c r="X213" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="214" spans="24:24">
       <c r="X214" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="215" spans="24:24">
       <c r="X215" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="216" spans="24:24">
       <c r="X216" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="217" spans="24:24">
       <c r="X217" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="218" spans="24:24">
       <c r="X218" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="219" spans="24:24">
       <c r="X219" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="220" spans="24:24">
       <c r="X220" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="221" spans="24:24">
       <c r="X221" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="222" spans="24:24">
       <c r="X222" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="223" spans="24:24">
       <c r="X223" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="224" spans="24:24">
       <c r="X224" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="225" spans="24:24">
       <c r="X225" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="226" spans="24:24">
       <c r="X226" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="227" spans="24:24">
       <c r="X227" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="228" spans="24:24">
       <c r="X228" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="229" spans="24:24">
       <c r="X229" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="230" spans="24:24">
       <c r="X230" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="231" spans="24:24">
       <c r="X231" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="232" spans="24:24">
       <c r="X232" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="233" spans="24:24">
       <c r="X233" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="234" spans="24:24">
       <c r="X234" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="235" spans="24:24">
       <c r="X235" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="236" spans="24:24">
       <c r="X236" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="237" spans="24:24">
       <c r="X237" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="238" spans="24:24">
       <c r="X238" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="239" spans="24:24">
       <c r="X239" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="240" spans="24:24">
       <c r="X240" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="241" spans="24:24">
       <c r="X241" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="242" spans="24:24">
       <c r="X242" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="243" spans="24:24">
       <c r="X243" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="244" spans="24:24">
       <c r="X244" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="245" spans="24:24">
       <c r="X245" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="246" spans="24:24">
       <c r="X246" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="247" spans="24:24">
       <c r="X247" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="248" spans="24:24">
       <c r="X248" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="249" spans="24:24">
       <c r="X249" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="250" spans="24:24">
       <c r="X250" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="251" spans="24:24">
       <c r="X251" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="252" spans="24:24">
       <c r="X252" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="253" spans="24:24">
       <c r="X253" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="254" spans="24:24">
       <c r="X254" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="255" spans="24:24">
       <c r="X255" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="256" spans="24:24">
       <c r="X256" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="257" spans="24:24">
       <c r="X257" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="258" spans="24:24">
       <c r="X258" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now checks constanst are in list. Added onse that where missing BUG fix observation given wrong uri
</commit_message>
<xml_diff>
--- a/data/MetaMaster.xlsx
+++ b/data/MetaMaster.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="19155" windowHeight="5790" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="19155" windowHeight="5730" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DropDowns" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="DesignationSubType">Lists!$I$2</definedName>
     <definedName name="Entity">Lists!$D$2:$D$13</definedName>
     <definedName name="EntitySubType">Lists!$L$2:$L$7</definedName>
-    <definedName name="Factor">Lists!$Q$2:$Q$52</definedName>
+    <definedName name="Factor">Lists!$Q$2:$Q$53</definedName>
     <definedName name="FeildsThatNeedUnit">Lists!$V$2:$V$4</definedName>
     <definedName name="Location">Lists!$B$2:$B$10</definedName>
     <definedName name="LocationSubType">Lists!$J$2:$J$4</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="469">
   <si>
     <t>Easting</t>
   </si>
@@ -1445,6 +1445,9 @@
   </si>
   <si>
     <t xml:space="preserve">Derivation Factor </t>
+  </si>
+  <si>
+    <t>Abundance</t>
   </si>
 </sst>
 </file>
@@ -2375,7 +2378,7 @@
   <dimension ref="A1:W258"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:T1048576"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -2508,8 +2511,8 @@
         <v>36</v>
       </c>
       <c r="P2" s="2"/>
-      <c r="Q2" s="2" t="s">
-        <v>72</v>
+      <c r="Q2" t="s">
+        <v>468</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>113</v>
@@ -2570,7 +2573,7 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="R3" t="s">
         <v>40</v>
@@ -2624,7 +2627,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="R4" t="s">
         <v>41</v>
@@ -2671,7 +2674,7 @@
         <v>450</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R5" s="2" t="s">
         <v>114</v>
@@ -2720,7 +2723,7 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R6" s="2" t="s">
         <v>38</v>
@@ -2765,8 +2768,8 @@
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
-      <c r="Q7" s="6" t="s">
-        <v>394</v>
+      <c r="Q7" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="R7" t="s">
         <v>39</v>
@@ -2807,8 +2810,8 @@
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
-      <c r="Q8" s="2" t="s">
-        <v>76</v>
+      <c r="Q8" s="6" t="s">
+        <v>394</v>
       </c>
       <c r="R8" s="2" t="s">
         <v>115</v>
@@ -2850,7 +2853,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R9" t="s">
         <v>42</v>
@@ -2890,7 +2893,7 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="S10" s="2"/>
       <c r="W10" t="s">
@@ -2921,7 +2924,7 @@
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="S11" s="2"/>
       <c r="W11" t="s">
@@ -2948,7 +2951,7 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="S12" s="2"/>
       <c r="W12" t="s">
@@ -2975,7 +2978,7 @@
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="S13" s="2"/>
       <c r="W13" t="s">
@@ -2989,8 +2992,8 @@
       <c r="F14" t="s">
         <v>443</v>
       </c>
-      <c r="Q14" t="s">
-        <v>390</v>
+      <c r="Q14" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="S14" s="2"/>
       <c r="W14" t="s">
@@ -3001,8 +3004,8 @@
       <c r="F15" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="Q15" s="2" t="s">
-        <v>83</v>
+      <c r="Q15" t="s">
+        <v>390</v>
       </c>
       <c r="S15" s="2"/>
       <c r="W15" t="s">
@@ -3014,7 +3017,7 @@
         <v>442</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="S16" s="2"/>
       <c r="W16" t="s">
@@ -3026,7 +3029,7 @@
         <v>434</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S17" s="2"/>
       <c r="W17" t="s">
@@ -3038,7 +3041,7 @@
         <v>22</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="S18" s="2"/>
       <c r="W18" t="s">
@@ -3059,8 +3062,8 @@
       <c r="M19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
-      <c r="Q19" s="5" t="s">
-        <v>392</v>
+      <c r="Q19" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="S19" s="2"/>
       <c r="W19" t="s">
@@ -3082,8 +3085,8 @@
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
-      <c r="Q20" s="2" t="s">
-        <v>4</v>
+      <c r="Q20" s="5" t="s">
+        <v>392</v>
       </c>
       <c r="S20" s="2"/>
       <c r="W20" t="s">
@@ -3106,7 +3109,7 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2" t="s">
-        <v>86</v>
+        <v>4</v>
       </c>
       <c r="S21" s="2"/>
       <c r="W21" t="s">
@@ -3131,7 +3134,7 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S22" s="2"/>
       <c r="W22" t="s">
@@ -3152,7 +3155,7 @@
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2" t="s">
-        <v>388</v>
+        <v>87</v>
       </c>
       <c r="S23" s="2"/>
       <c r="W23" t="s">
@@ -3172,7 +3175,7 @@
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2" t="s">
-        <v>88</v>
+        <v>388</v>
       </c>
       <c r="S24" s="2"/>
       <c r="W24" t="s">
@@ -3192,8 +3195,8 @@
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
-      <c r="Q25" s="5" t="s">
-        <v>393</v>
+      <c r="Q25" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="S25" s="2"/>
       <c r="W25" t="s">
@@ -3215,8 +3218,8 @@
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
-      <c r="Q26" s="2" t="s">
-        <v>2</v>
+      <c r="Q26" s="5" t="s">
+        <v>393</v>
       </c>
       <c r="S26" s="2"/>
       <c r="W26" t="s">
@@ -3226,7 +3229,7 @@
     <row r="27" spans="1:23" ht="15">
       <c r="D27" s="2"/>
       <c r="Q27" s="2" t="s">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="S27" s="2"/>
       <c r="W27" t="s">
@@ -3236,7 +3239,7 @@
     <row r="28" spans="1:23" ht="15">
       <c r="D28" s="2"/>
       <c r="Q28" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="S28" s="2"/>
       <c r="W28" t="s">
@@ -3247,7 +3250,7 @@
       <c r="A29" s="2"/>
       <c r="D29" s="2"/>
       <c r="Q29" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="S29" s="2"/>
       <c r="W29" t="s">
@@ -3257,7 +3260,7 @@
     <row r="30" spans="1:23" ht="15">
       <c r="D30" s="2"/>
       <c r="Q30" s="2" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="S30" s="2"/>
       <c r="W30" t="s">
@@ -3267,7 +3270,7 @@
     <row r="31" spans="1:23" ht="15">
       <c r="D31" s="2"/>
       <c r="Q31" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S31" s="2"/>
       <c r="W31" t="s">
@@ -3277,7 +3280,7 @@
     <row r="32" spans="1:23" ht="15">
       <c r="D32" s="2"/>
       <c r="Q32" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S32" s="2"/>
       <c r="W32" t="s">
@@ -3287,7 +3290,7 @@
     <row r="33" spans="4:23" ht="15">
       <c r="D33" s="2"/>
       <c r="Q33" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S33" s="2"/>
       <c r="W33" t="s">
@@ -3297,7 +3300,7 @@
     <row r="34" spans="4:23" ht="15">
       <c r="D34" s="2"/>
       <c r="Q34" s="2" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="S34" s="2"/>
       <c r="W34" t="s">
@@ -3307,7 +3310,7 @@
     <row r="35" spans="4:23" ht="15">
       <c r="D35" s="2"/>
       <c r="Q35" s="2" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="S35" s="2"/>
       <c r="W35" t="s">
@@ -3316,8 +3319,8 @@
     </row>
     <row r="36" spans="4:23" ht="15">
       <c r="D36" s="2"/>
-      <c r="Q36" t="s">
-        <v>387</v>
+      <c r="Q36" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="S36" s="2"/>
       <c r="W36" t="s">
@@ -3326,8 +3329,8 @@
     </row>
     <row r="37" spans="4:23" ht="15">
       <c r="D37" s="2"/>
-      <c r="Q37" s="2" t="s">
-        <v>95</v>
+      <c r="Q37" t="s">
+        <v>387</v>
       </c>
       <c r="S37" s="2"/>
       <c r="W37" t="s">
@@ -3337,7 +3340,7 @@
     <row r="38" spans="4:23" ht="15">
       <c r="D38" s="2"/>
       <c r="Q38" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="S38" s="2"/>
       <c r="W38" t="s">
@@ -3347,7 +3350,7 @@
     <row r="39" spans="4:23" ht="15">
       <c r="D39" s="2"/>
       <c r="Q39" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="S39" s="2"/>
       <c r="W39" t="s">
@@ -3356,7 +3359,7 @@
     </row>
     <row r="40" spans="4:23" ht="15">
       <c r="Q40" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="S40" s="2"/>
       <c r="W40" t="s">
@@ -3365,7 +3368,7 @@
     </row>
     <row r="41" spans="4:23" ht="15">
       <c r="Q41" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="S41" s="2"/>
       <c r="W41" t="s">
@@ -3374,7 +3377,7 @@
     </row>
     <row r="42" spans="4:23" ht="15">
       <c r="Q42" s="2" t="s">
-        <v>389</v>
+        <v>103</v>
       </c>
       <c r="S42" s="2"/>
       <c r="W42" t="s">
@@ -3383,7 +3386,7 @@
     </row>
     <row r="43" spans="4:23" ht="15">
       <c r="Q43" s="2" t="s">
-        <v>100</v>
+        <v>389</v>
       </c>
       <c r="S43" s="2"/>
       <c r="W43" t="s">
@@ -3392,7 +3395,7 @@
     </row>
     <row r="44" spans="4:23" ht="15">
       <c r="Q44" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S44" s="2"/>
       <c r="W44" t="s">
@@ -3400,8 +3403,8 @@
       </c>
     </row>
     <row r="45" spans="4:23" ht="15">
-      <c r="Q45" t="s">
-        <v>391</v>
+      <c r="Q45" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="S45" s="2"/>
       <c r="W45" t="s">
@@ -3409,8 +3412,8 @@
       </c>
     </row>
     <row r="46" spans="4:23" ht="15">
-      <c r="Q46" s="6" t="s">
-        <v>395</v>
+      <c r="Q46" t="s">
+        <v>391</v>
       </c>
       <c r="S46" s="2"/>
       <c r="W46" t="s">
@@ -3418,8 +3421,8 @@
       </c>
     </row>
     <row r="47" spans="4:23" ht="15">
-      <c r="Q47" s="2" t="s">
-        <v>104</v>
+      <c r="Q47" s="6" t="s">
+        <v>395</v>
       </c>
       <c r="S47" s="2"/>
       <c r="W47" t="s">
@@ -3428,23 +3431,23 @@
     </row>
     <row r="48" spans="4:23" ht="15">
       <c r="Q48" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="W48" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="49" spans="17:23">
-      <c r="Q49" t="s">
-        <v>18</v>
+    <row r="49" spans="17:23" ht="15">
+      <c r="Q49" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="W49" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="50" spans="17:23" ht="15">
-      <c r="Q50" s="2" t="s">
-        <v>102</v>
+    <row r="50" spans="17:23">
+      <c r="Q50" t="s">
+        <v>18</v>
       </c>
       <c r="W50" t="s">
         <v>164</v>
@@ -3452,7 +3455,7 @@
     </row>
     <row r="51" spans="17:23" ht="15">
       <c r="Q51" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="W51" t="s">
         <v>165</v>
@@ -3460,7 +3463,7 @@
     </row>
     <row r="52" spans="17:23" ht="15">
       <c r="Q52" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="W52" t="s">
         <v>166</v>
@@ -3468,7 +3471,7 @@
     </row>
     <row r="53" spans="17:23" ht="15">
       <c r="Q53" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="W53" t="s">
         <v>167</v>
@@ -3476,7 +3479,7 @@
     </row>
     <row r="54" spans="17:23" ht="15">
       <c r="Q54" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="W54" t="s">
         <v>168</v>
@@ -3484,7 +3487,7 @@
     </row>
     <row r="55" spans="17:23" ht="15">
       <c r="Q55" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="W55" t="s">
         <v>169</v>
@@ -3492,7 +3495,7 @@
     </row>
     <row r="56" spans="17:23" ht="15">
       <c r="Q56" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="W56" t="s">
         <v>170</v>
@@ -3500,13 +3503,16 @@
     </row>
     <row r="57" spans="17:23" ht="15">
       <c r="Q57" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="W57" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="58" spans="17:23">
+    <row r="58" spans="17:23" ht="15">
+      <c r="Q58" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="W58" t="s">
         <v>172</v>
       </c>
@@ -4516,6 +4522,11 @@
     <sortCondition ref="F3:F20"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Factor" error="Entered value not found in list of expected Factors. Any other value will need to be added to the global accepted list." promptTitle="Factor for Observation's Value" prompt="Select the Factor or thing that the values in this column describe.  To use the value of another column enter !column" sqref="Q2">
+      <formula1>INDIRECT(IF($H$2="Value","Factor","NotApplicable"))</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added option to convert Nulls to zero or Zeros to Nulls. Works for URI's not for values yet.
</commit_message>
<xml_diff>
--- a/data/MetaMaster.xlsx
+++ b/data/MetaMaster.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="472">
   <si>
     <t>Easting</t>
   </si>
@@ -1168,15 +1168,6 @@
     <t>Overrides the normal pattern of using the local DOI and sheet as the base URI. Format is [doi]sheetName</t>
   </si>
   <si>
-    <t>Ignore Zeros</t>
-  </si>
-  <si>
-    <t>If set to true any zeros in this column will be treated as nulls.</t>
-  </si>
-  <si>
-    <t>Only legal values are "TRUE", "FALSE". Where a null/Blank is treated as "FALSE".</t>
-  </si>
-  <si>
     <t>Header</t>
   </si>
   <si>
@@ -1195,9 +1186,6 @@
     <t>hasSubsite</t>
   </si>
   <si>
-    <t>{TRUE,FALSE}</t>
-  </si>
-  <si>
     <t>Entered value not found in list of expected Factors. Any other value will need to be added to the global accepted list.</t>
   </si>
   <si>
@@ -1454,6 +1442,21 @@
   </si>
   <si>
     <t>isSubTaxonOf</t>
+  </si>
+  <si>
+    <t>Zeros vs Nulls</t>
+  </si>
+  <si>
+    <t>How to treat Zeros and Nulls</t>
+  </si>
+  <si>
+    <t>{Keep as is,Zeros as Nulls,Nulls as Zeros}</t>
+  </si>
+  <si>
+    <t>"Keep as is", leaves Nulls and Nulls and Zeros ans Zeros, "Zeros as Nulls" assumes any Zero found is in fact a Null or don't know. While "Nulls as Zeros" assumes any Nulls and Blanks are in fact a known zero or known Absence.</t>
+  </si>
+  <si>
+    <t>Only legal values are "Keep as is", "Zeros as Nulls","Nulls as Zeros". Where a null/Blank is treated as "Keep as is".</t>
   </si>
 </sst>
 </file>
@@ -1821,10 +1824,10 @@
   <dimension ref="A1:Z117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="11" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="11" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12"/>
@@ -1868,7 +1871,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
@@ -1877,27 +1880,27 @@
         <v>131</v>
       </c>
       <c r="F2" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="G2" t="s">
         <v>138</v>
       </c>
       <c r="H2" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D3" t="s">
         <v>132</v>
       </c>
       <c r="E3" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="F3" t="s">
         <v>135</v>
@@ -1906,7 +1909,7 @@
         <v>139</v>
       </c>
       <c r="H3" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -1915,7 +1918,7 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="E4" t="s">
         <v>374</v>
@@ -1923,25 +1926,25 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
-        <v>375</v>
+        <v>467</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>384</v>
+        <v>469</v>
       </c>
       <c r="D5" t="s">
-        <v>375</v>
-      </c>
-      <c r="E5" t="s">
-        <v>376</v>
+        <v>468</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>470</v>
       </c>
       <c r="F5" t="s">
         <v>135</v>
       </c>
       <c r="G5" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="H5" t="s">
-        <v>377</v>
+        <v>471</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -1949,16 +1952,16 @@
         <v>121</v>
       </c>
       <c r="C6" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="F6" t="s">
         <v>135</v>
       </c>
       <c r="G6" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="H6" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -1966,22 +1969,22 @@
         <v>11</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D7" t="s">
         <v>133</v>
       </c>
       <c r="E7" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="F7" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="G7" t="s">
         <v>140</v>
       </c>
       <c r="H7" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -1989,22 +1992,22 @@
         <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D8" t="s">
         <v>134</v>
       </c>
       <c r="E8" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F8" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="G8" t="s">
         <v>141</v>
       </c>
       <c r="H8" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -2012,36 +2015,36 @@
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D9" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="E9" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="F9" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="G9" t="s">
         <v>142</v>
       </c>
       <c r="H9" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D10" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="E10" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -2061,10 +2064,10 @@
     </row>
     <row r="12" spans="1:26">
       <c r="B12" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="C12" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="D12">
         <v>32</v>
@@ -2081,7 +2084,7 @@
     </row>
     <row r="13" spans="1:26">
       <c r="A13" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C13">
         <f t="shared" ref="C13:H22" si="0">LEN(C1)</f>
@@ -2185,15 +2188,15 @@
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>225</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
@@ -2201,7 +2204,7 @@
       </c>
       <c r="H17">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2331,7 +2334,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="B24" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C24" s="4"/>
     </row>
@@ -2340,7 +2343,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations xWindow="281" yWindow="244" count="10">
+  <dataValidations disablePrompts="1" xWindow="281" yWindow="244" count="10">
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unexpected Unit." error="The Unit provided was not in the list. Only use values not in the list if you are absolutely sure none of the values in the list are applicable." promptTitle="Unit for Observation's Value" prompt="Please describe the Unit the values are in. Whenever possible pick a value from the list." sqref="B8">
       <formula1>"INDIRECT(IF(ISNA(VLOOKUP($B$2,FeildsThatNeedUnit,1,FALSE)),""NotApplicable"",""UNIT""))"</formula1>
     </dataValidation>
@@ -2383,8 +2386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W258"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -2416,7 +2419,7 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -2429,25 +2432,25 @@
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>423</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>427</v>
       </c>
       <c r="P1" s="2"/>
       <c r="Q1" s="2" t="s">
@@ -2460,7 +2463,7 @@
         <v>9</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="U1" t="s">
         <v>37</v>
@@ -2508,17 +2511,17 @@
         <v>16</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>36</v>
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>113</v>
@@ -2527,7 +2530,7 @@
         <v>120</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>36</v>
@@ -2536,7 +2539,7 @@
         <v>29</v>
       </c>
       <c r="W2" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="15">
@@ -2564,17 +2567,17 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
@@ -2611,7 +2614,7 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -2622,13 +2625,13 @@
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="N4" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
@@ -2665,19 +2668,19 @@
         <v>122</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="N5" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>73</v>
@@ -2718,13 +2721,13 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="N6" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
@@ -2755,7 +2758,7 @@
         <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>8</v>
@@ -2770,7 +2773,7 @@
         <v>36</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="N7" t="s">
         <v>12</v>
@@ -2793,34 +2796,34 @@
         <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>126</v>
       </c>
       <c r="E8" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="F8" t="s">
         <v>124</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="H8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="N8" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="6" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="R8" s="2" t="s">
         <v>115</v>
@@ -2841,10 +2844,10 @@
         <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>10</v>
@@ -2874,7 +2877,7 @@
     </row>
     <row r="10" spans="1:23" ht="15">
       <c r="B10" s="2" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
@@ -2886,7 +2889,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>11</v>
@@ -2920,10 +2923,10 @@
         <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="G11" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="H11" s="2"/>
       <c r="J11" s="2"/>
@@ -2942,7 +2945,7 @@
     </row>
     <row r="12" spans="1:23" ht="15">
       <c r="C12" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>32</v>
@@ -2951,7 +2954,7 @@
         <v>125</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>21</v>
@@ -2977,13 +2980,13 @@
         <v>123</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>22</v>
@@ -3009,10 +3012,10 @@
         <v>28</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>5</v>
@@ -3027,16 +3030,16 @@
     </row>
     <row r="15" spans="1:23" ht="15">
       <c r="C15" s="2" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="F15" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="Q15" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="S15" s="2"/>
       <c r="W15" t="s">
@@ -3045,7 +3048,7 @@
     </row>
     <row r="16" spans="1:23" ht="15">
       <c r="F16" s="2" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>34</v>
@@ -3060,7 +3063,7 @@
     </row>
     <row r="17" spans="1:23" ht="15">
       <c r="F17" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="G17" t="s">
         <v>28</v>
@@ -3075,10 +3078,10 @@
     </row>
     <row r="18" spans="1:23" ht="15">
       <c r="F18" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="Q18" s="2" t="s">
         <v>85</v>
@@ -3091,7 +3094,7 @@
     <row r="19" spans="1:23" ht="15">
       <c r="C19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -3112,7 +3115,7 @@
     </row>
     <row r="20" spans="1:23" ht="15">
       <c r="F20" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -3125,7 +3128,7 @@
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="5" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="S20" s="2"/>
       <c r="W20" t="s">
@@ -3135,7 +3138,7 @@
     <row r="21" spans="1:23" ht="15">
       <c r="C21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -3183,7 +3186,7 @@
     <row r="23" spans="1:23" ht="15">
       <c r="C23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -3205,7 +3208,7 @@
     </row>
     <row r="24" spans="1:23" ht="15">
       <c r="F24" s="2" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -3218,7 +3221,7 @@
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="S24" s="2"/>
       <c r="W24" t="s">
@@ -3228,7 +3231,7 @@
     <row r="25" spans="1:23" ht="15">
       <c r="C25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -3253,7 +3256,7 @@
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -3266,7 +3269,7 @@
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="5" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="S26" s="2"/>
       <c r="W26" t="s">
@@ -3377,7 +3380,7 @@
     <row r="37" spans="4:23" ht="15">
       <c r="D37" s="2"/>
       <c r="Q37" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="S37" s="2"/>
       <c r="W37" t="s">
@@ -3433,7 +3436,7 @@
     </row>
     <row r="43" spans="4:23" ht="15">
       <c r="Q43" s="2" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="S43" s="2"/>
       <c r="W43" t="s">
@@ -3460,7 +3463,7 @@
     </row>
     <row r="46" spans="4:23" ht="15">
       <c r="Q46" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="S46" s="2"/>
       <c r="W46" t="s">
@@ -3469,7 +3472,7 @@
     </row>
     <row r="47" spans="4:23" ht="15">
       <c r="Q47" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="S47" s="2"/>
       <c r="W47" t="s">

</xml_diff>

<commit_message>
Cointributor split into Survey, Owner and uploader
</commit_message>
<xml_diff>
--- a/data/MetaMaster.xlsx
+++ b/data/MetaMaster.xlsx
@@ -24,13 +24,13 @@
     <definedName name="Location">Lists!$B$2:$B$10</definedName>
     <definedName name="LocationSubType">Lists!$J$2:$J$4</definedName>
     <definedName name="NotApplicable">Lists!$U$2</definedName>
-    <definedName name="Observation">Lists!$C$2:$C$15</definedName>
+    <definedName name="Observation">Lists!$C$2:$C$17</definedName>
     <definedName name="ObservationSubType">Lists!$K$2</definedName>
     <definedName name="Site">Lists!$E$2:$E$14</definedName>
     <definedName name="SiteSubType">Lists!$M$2:$M$9</definedName>
-    <definedName name="Survey">Lists!$G$2:$G$14</definedName>
+    <definedName name="Survey">Lists!$G$2:$G$16</definedName>
     <definedName name="SurveySubType">Lists!$O$2</definedName>
-    <definedName name="Taxon">Lists!$F$2:$F$25</definedName>
+    <definedName name="Taxon">Lists!$F$2:$F$27</definedName>
     <definedName name="TaxonSubType">Lists!$N$2:$N$10</definedName>
     <definedName name="UNDEFINED">Lists!#REF!</definedName>
     <definedName name="Unit">Lists!$R$2:$R$9</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="471">
   <si>
     <t>Easting</t>
   </si>
@@ -1422,9 +1422,6 @@
     <t>DevriationFactor</t>
   </si>
   <si>
-    <t>isSubTaxonOf</t>
-  </si>
-  <si>
     <t>Zeros vs Nulls</t>
   </si>
   <si>
@@ -1444,6 +1441,18 @@
   </si>
   <si>
     <t>Meqvl/l</t>
+  </si>
+  <si>
+    <t>hasSubtaxon</t>
+  </si>
+  <si>
+    <t>isSubtaxonOf</t>
+  </si>
+  <si>
+    <t>Surveyor</t>
+  </si>
+  <si>
+    <t>Uploader</t>
   </si>
 </sst>
 </file>
@@ -1810,11 +1819,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z117"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="11" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="11" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12"/>
@@ -1916,16 +1925,16 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
+        <v>460</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="D5" t="s">
         <v>461</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>463</v>
-      </c>
-      <c r="D5" t="s">
-        <v>462</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>464</v>
       </c>
       <c r="F5" t="s">
         <v>130</v>
@@ -1934,7 +1943,7 @@
         <v>454</v>
       </c>
       <c r="H5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -1982,7 +1991,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D8" t="s">
         <v>129</v>
@@ -2376,8 +2385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -2586,7 +2595,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>469</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -2637,7 +2646,7 @@
         <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>123</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>33</v>
@@ -2649,7 +2658,7 @@
         <v>424</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>7</v>
+        <v>469</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>444</v>
@@ -2664,7 +2673,7 @@
         <v>72</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>115</v>
@@ -2681,7 +2690,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>470</v>
       </c>
       <c r="D6" t="s">
         <v>122</v>
@@ -2693,7 +2702,7 @@
         <v>7</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>8</v>
+        <v>123</v>
       </c>
       <c r="H6" s="2"/>
       <c r="J6" s="2"/>
@@ -2730,7 +2739,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>30</v>
@@ -2741,8 +2750,8 @@
       <c r="F7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G7" t="s">
-        <v>122</v>
+      <c r="G7" s="2" t="s">
+        <v>470</v>
       </c>
       <c r="H7" s="2"/>
       <c r="J7" s="2"/>
@@ -2774,7 +2783,7 @@
         <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>459</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>124</v>
@@ -2786,7 +2795,7 @@
         <v>122</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>459</v>
+        <v>8</v>
       </c>
       <c r="H8" s="2"/>
       <c r="J8" s="2"/>
@@ -2816,7 +2825,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>31</v>
@@ -2827,8 +2836,8 @@
       <c r="F9" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>10</v>
+      <c r="G9" t="s">
+        <v>122</v>
       </c>
       <c r="H9" s="2"/>
       <c r="J9" s="2"/>
@@ -2858,7 +2867,7 @@
         <v>445</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>5</v>
+        <v>459</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>21</v>
@@ -2870,7 +2879,7 @@
         <v>422</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>11</v>
+        <v>459</v>
       </c>
       <c r="H10" s="2"/>
       <c r="J10" s="2"/>
@@ -2892,7 +2901,7 @@
     </row>
     <row r="11" spans="1:22" ht="15">
       <c r="C11" s="2" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>22</v>
@@ -2903,8 +2912,8 @@
       <c r="F11" t="s">
         <v>433</v>
       </c>
-      <c r="G11" t="s">
-        <v>458</v>
+      <c r="G11" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="H11" s="2"/>
       <c r="J11" s="2"/>
@@ -2922,8 +2931,8 @@
       </c>
     </row>
     <row r="12" spans="1:22" ht="15">
-      <c r="C12" t="s">
-        <v>458</v>
+      <c r="C12" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>32</v>
@@ -2935,7 +2944,7 @@
         <v>426</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -2955,7 +2964,7 @@
     </row>
     <row r="13" spans="1:22" ht="15">
       <c r="C13" s="2" t="s">
-        <v>121</v>
+        <v>34</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>445</v>
@@ -2966,8 +2975,8 @@
       <c r="F13" t="s">
         <v>434</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>22</v>
+      <c r="G13" t="s">
+        <v>458</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -2987,7 +2996,7 @@
     </row>
     <row r="14" spans="1:22" ht="15">
       <c r="C14" t="s">
-        <v>28</v>
+        <v>458</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>445</v>
@@ -2996,7 +3005,7 @@
         <v>427</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="Q14" s="2" t="s">
         <v>81</v>
@@ -3008,13 +3017,13 @@
     </row>
     <row r="15" spans="1:22" ht="15">
       <c r="C15" s="2" t="s">
-        <v>402</v>
+        <v>121</v>
       </c>
       <c r="F15" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q15" t="s">
         <v>381</v>
@@ -3025,11 +3034,14 @@
       </c>
     </row>
     <row r="16" spans="1:22" ht="15">
-      <c r="F16" s="2" t="s">
-        <v>430</v>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" t="s">
+        <v>468</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="Q16" s="2" t="s">
         <v>82</v>
@@ -3040,11 +3052,14 @@
       </c>
     </row>
     <row r="17" spans="1:22" ht="15">
+      <c r="C17" s="2" t="s">
+        <v>402</v>
+      </c>
       <c r="F17" t="s">
-        <v>421</v>
-      </c>
-      <c r="G17" t="s">
-        <v>28</v>
+        <v>393</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="Q17" s="2" t="s">
         <v>83</v>
@@ -3055,11 +3070,11 @@
       </c>
     </row>
     <row r="18" spans="1:22" ht="15">
-      <c r="F18" t="s">
-        <v>432</v>
+      <c r="F18" s="2" t="s">
+        <v>430</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>402</v>
+        <v>34</v>
       </c>
       <c r="Q18" s="2" t="s">
         <v>84</v>
@@ -3071,10 +3086,12 @@
     </row>
     <row r="19" spans="1:22" ht="15">
       <c r="C19" s="2"/>
-      <c r="F19" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="G19" s="2"/>
+      <c r="F19" t="s">
+        <v>421</v>
+      </c>
+      <c r="G19" t="s">
+        <v>28</v>
+      </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -3093,9 +3110,11 @@
     </row>
     <row r="20" spans="1:22" ht="15">
       <c r="F20" t="s">
-        <v>431</v>
-      </c>
-      <c r="G20" s="2"/>
+        <v>432</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>402</v>
+      </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -3116,7 +3135,7 @@
     <row r="21" spans="1:22" ht="15">
       <c r="C21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -3140,8 +3159,8 @@
       <c r="A22" s="2"/>
       <c r="C22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="2" t="s">
-        <v>22</v>
+      <c r="F22" t="s">
+        <v>431</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -3164,7 +3183,7 @@
     <row r="23" spans="1:22" ht="15">
       <c r="C23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -3186,7 +3205,7 @@
     </row>
     <row r="24" spans="1:22" ht="15">
       <c r="F24" s="2" t="s">
-        <v>428</v>
+        <v>22</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -3209,7 +3228,7 @@
     <row r="25" spans="1:22" ht="15">
       <c r="C25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -3234,7 +3253,7 @@
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>453</v>
+        <v>428</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -3256,6 +3275,9 @@
     </row>
     <row r="27" spans="1:22" ht="15">
       <c r="D27" s="2"/>
+      <c r="F27" s="2" t="s">
+        <v>445</v>
+      </c>
       <c r="Q27" s="2" t="s">
         <v>2</v>
       </c>
@@ -3266,6 +3288,9 @@
     </row>
     <row r="28" spans="1:22" ht="15">
       <c r="D28" s="2"/>
+      <c r="F28" s="2" t="s">
+        <v>453</v>
+      </c>
       <c r="Q28" s="2" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
metaMaster before final Ontology check.
</commit_message>
<xml_diff>
--- a/data/MetaMaster.xlsx
+++ b/data/MetaMaster.xlsx
@@ -63,9 +63,6 @@
     <t>AlternativeName</t>
   </si>
   <si>
-    <t>Contributor</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -1453,6 +1450,9 @@
   </si>
   <si>
     <t>Uploader</t>
+  </si>
+  <si>
+    <t>Authority</t>
   </si>
 </sst>
 </file>
@@ -1838,212 +1838,212 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" t="s">
         <v>130</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>131</v>
-      </c>
-      <c r="H1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="D3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" t="s">
         <v>397</v>
       </c>
-      <c r="D3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H3" t="s">
         <v>398</v>
-      </c>
-      <c r="F3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G3" t="s">
-        <v>134</v>
-      </c>
-      <c r="H3" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
+        <v>459</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="D5" t="s">
         <v>460</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>462</v>
       </c>
-      <c r="D5" t="s">
-        <v>461</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" t="s">
+        <v>453</v>
+      </c>
+      <c r="H5" t="s">
         <v>463</v>
-      </c>
-      <c r="F5" t="s">
-        <v>130</v>
-      </c>
-      <c r="G5" t="s">
-        <v>454</v>
-      </c>
-      <c r="H5" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C6" t="s">
+        <v>389</v>
+      </c>
+      <c r="F6" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" t="s">
         <v>390</v>
       </c>
-      <c r="F6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>391</v>
-      </c>
-      <c r="H6" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E7" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E9" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F9" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H9" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
+        <v>444</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="D10" t="s">
         <v>445</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>451</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>446</v>
-      </c>
-      <c r="E10" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -2063,10 +2063,10 @@
     </row>
     <row r="12" spans="1:26">
       <c r="B12" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C12" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D12">
         <v>32</v>
@@ -2083,7 +2083,7 @@
     </row>
     <row r="13" spans="1:26">
       <c r="A13" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C13">
         <f t="shared" ref="C13:H22" si="0">LEN(C1)</f>
@@ -2333,7 +2333,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="B24" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C24" s="4"/>
     </row>
@@ -2386,7 +2386,7 @@
   <dimension ref="A1:V258"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -2409,182 +2409,182 @@
   <sheetData>
     <row r="1" spans="1:22" ht="15">
       <c r="A1" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>417</v>
       </c>
       <c r="P1" s="2"/>
       <c r="Q1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="U1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="15">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="V2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="15">
       <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="15">
@@ -2592,10 +2592,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -2603,283 +2603,283 @@
       <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F4" t="s">
-        <v>436</v>
+      <c r="F4" s="2" t="s">
+        <v>470</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H4" s="2"/>
       <c r="J4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="N4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="V4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="15">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>424</v>
+        <v>119</v>
+      </c>
+      <c r="F5" t="s">
+        <v>435</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="N5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="V5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="15">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="E6" t="s">
-        <v>122</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="H6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="N6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="V6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="15">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="N7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S7" s="2"/>
       <c r="V7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="15">
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="N8" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S8" s="2"/>
       <c r="V8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="15">
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S9" s="2"/>
       <c r="V9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="15">
       <c r="B10" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H10" s="2"/>
       <c r="J10" s="2"/>
@@ -2887,33 +2887,33 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S10" s="2"/>
       <c r="V10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="15">
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H11" s="2"/>
       <c r="J11" s="2"/>
@@ -2923,11 +2923,11 @@
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S11" s="2"/>
       <c r="V11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="15">
@@ -2935,16 +2935,16 @@
         <v>5</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -2955,28 +2955,28 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="S12" s="2"/>
       <c r="V12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15">
       <c r="C13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G13" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -2987,110 +2987,110 @@
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S13" s="2"/>
       <c r="V13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="15">
       <c r="C14" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S14" s="2"/>
       <c r="V14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="15">
       <c r="C15" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q15" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="S15" s="2"/>
       <c r="V15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="15">
       <c r="C16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="S16" s="2"/>
       <c r="V16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="15">
       <c r="C17" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="S17" s="2"/>
       <c r="V17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="15">
       <c r="F18" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="S18" s="2"/>
       <c r="V18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="15">
       <c r="C19" s="2"/>
       <c r="F19" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -3101,19 +3101,19 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="S19" s="2"/>
       <c r="V19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="15">
       <c r="F20" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -3125,17 +3125,17 @@
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="S20" s="2"/>
       <c r="V20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="15">
       <c r="C21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -3152,7 +3152,7 @@
       </c>
       <c r="S21" s="2"/>
       <c r="V21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="15">
@@ -3160,7 +3160,7 @@
       <c r="C22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -3173,17 +3173,17 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S22" s="2"/>
       <c r="V22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="15">
       <c r="C23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -3196,16 +3196,16 @@
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S23" s="2"/>
       <c r="V23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:22" ht="15">
       <c r="F24" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -3218,17 +3218,17 @@
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="S24" s="2"/>
       <c r="V24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="15">
       <c r="C25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -3241,11 +3241,11 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S25" s="2"/>
       <c r="V25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="15">
@@ -3253,7 +3253,7 @@
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -3266,98 +3266,98 @@
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="S26" s="2"/>
       <c r="V26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:22" ht="15">
       <c r="D27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="Q27" s="2" t="s">
         <v>2</v>
       </c>
       <c r="S27" s="2"/>
       <c r="V27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="15">
       <c r="D28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S28" s="2"/>
       <c r="V28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="15">
       <c r="A29" s="2"/>
       <c r="D29" s="2"/>
       <c r="Q29" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="S29" s="2"/>
       <c r="V29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="15">
       <c r="D30" s="2"/>
       <c r="Q30" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S30" s="2"/>
       <c r="V30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="15">
       <c r="D31" s="2"/>
       <c r="Q31" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="S31" s="2"/>
       <c r="V31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="15">
       <c r="D32" s="2"/>
       <c r="Q32" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S32" s="2"/>
       <c r="V32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="4:22" ht="15">
       <c r="D33" s="2"/>
       <c r="Q33" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S33" s="2"/>
       <c r="V33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="4:22" ht="15">
       <c r="D34" s="2"/>
       <c r="Q34" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S34" s="2"/>
       <c r="V34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="4:22" ht="15">
@@ -3367,1212 +3367,1212 @@
       </c>
       <c r="S35" s="2"/>
       <c r="V35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="4:22" ht="15">
       <c r="D36" s="2"/>
       <c r="Q36" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S36" s="2"/>
       <c r="V36" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="4:22" ht="15">
       <c r="D37" s="2"/>
       <c r="Q37" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="S37" s="2"/>
       <c r="V37" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="4:22" ht="15">
       <c r="D38" s="2"/>
       <c r="Q38" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S38" s="2"/>
       <c r="V38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="4:22" ht="15">
       <c r="D39" s="2"/>
       <c r="Q39" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S39" s="2"/>
       <c r="V39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="4:22" ht="15">
       <c r="Q40" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="S40" s="2"/>
       <c r="V40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="4:22" ht="15">
       <c r="Q41" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S41" s="2"/>
       <c r="V41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" spans="4:22" ht="15">
       <c r="Q42" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="S42" s="2"/>
       <c r="V42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="4:22" ht="15">
       <c r="Q43" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="S43" s="2"/>
       <c r="V43" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="4:22" ht="15">
       <c r="Q44" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S44" s="2"/>
       <c r="V44" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="4:22" ht="15">
       <c r="Q45" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S45" s="2"/>
       <c r="V45" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="4:22" ht="15">
       <c r="Q46" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="S46" s="2"/>
       <c r="V46" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="4:22" ht="15">
       <c r="Q47" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="S47" s="2"/>
       <c r="V47" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="48" spans="4:22" ht="15">
       <c r="Q48" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="V48" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="49" spans="17:22" ht="15">
       <c r="Q49" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="V49" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="17:22">
       <c r="Q50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="V50" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51" spans="17:22" ht="15">
       <c r="Q51" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="V51" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="17:22" ht="15">
       <c r="Q52" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="V52" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="17:22" ht="15">
       <c r="Q53" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="V53" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="17:22" ht="15">
       <c r="Q54" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V54" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="17:22" ht="15">
       <c r="Q55" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="V55" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="56" spans="17:22" ht="15">
       <c r="Q56" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="V56" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="57" spans="17:22" ht="15">
       <c r="Q57" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="V57" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="58" spans="17:22" ht="15">
       <c r="Q58" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="V58" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="59" spans="17:22">
       <c r="V59" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="60" spans="17:22">
       <c r="V60" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="61" spans="17:22">
       <c r="V61" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="62" spans="17:22">
       <c r="V62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="63" spans="17:22">
       <c r="V63" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="64" spans="17:22">
       <c r="V64" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="65" spans="22:22">
       <c r="V65" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="66" spans="22:22">
       <c r="V66" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="67" spans="22:22">
       <c r="V67" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="68" spans="22:22">
       <c r="V68" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="69" spans="22:22">
       <c r="V69" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="70" spans="22:22">
       <c r="V70" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="71" spans="22:22">
       <c r="V71" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="72" spans="22:22">
       <c r="V72" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="73" spans="22:22">
       <c r="V73" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="74" spans="22:22">
       <c r="V74" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="75" spans="22:22">
       <c r="V75" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="76" spans="22:22">
       <c r="V76" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="77" spans="22:22">
       <c r="V77" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="78" spans="22:22">
       <c r="V78" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="79" spans="22:22">
       <c r="V79" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="80" spans="22:22">
       <c r="V80" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="81" spans="22:22">
       <c r="V81" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="82" spans="22:22">
       <c r="V82" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="83" spans="22:22">
       <c r="V83" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="84" spans="22:22">
       <c r="V84" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="85" spans="22:22">
       <c r="V85" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="86" spans="22:22">
       <c r="V86" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="87" spans="22:22">
       <c r="V87" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="88" spans="22:22">
       <c r="V88" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="89" spans="22:22">
       <c r="V89" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="90" spans="22:22">
       <c r="V90" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="91" spans="22:22">
       <c r="V91" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="92" spans="22:22">
       <c r="V92" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="93" spans="22:22">
       <c r="V93" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="94" spans="22:22">
       <c r="V94" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="95" spans="22:22">
       <c r="V95" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="96" spans="22:22">
       <c r="V96" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="97" spans="22:22">
       <c r="V97" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="98" spans="22:22">
       <c r="V98" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="99" spans="22:22">
       <c r="V99" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="100" spans="22:22">
       <c r="V100" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="101" spans="22:22">
       <c r="V101" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="102" spans="22:22">
       <c r="V102" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="103" spans="22:22">
       <c r="V103" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="104" spans="22:22">
       <c r="V104" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="105" spans="22:22">
       <c r="V105" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="106" spans="22:22">
       <c r="V106" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="107" spans="22:22">
       <c r="V107" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="108" spans="22:22">
       <c r="V108" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="109" spans="22:22">
       <c r="V109" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="110" spans="22:22">
       <c r="V110" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="111" spans="22:22">
       <c r="V111" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="112" spans="22:22">
       <c r="V112" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="113" spans="22:22">
       <c r="V113" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="114" spans="22:22">
       <c r="V114" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="115" spans="22:22">
       <c r="V115" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="116" spans="22:22">
       <c r="V116" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="117" spans="22:22">
       <c r="V117" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="118" spans="22:22">
       <c r="V118" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="119" spans="22:22">
       <c r="V119" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="120" spans="22:22">
       <c r="V120" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="121" spans="22:22">
       <c r="V121" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="122" spans="22:22">
       <c r="V122" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="123" spans="22:22">
       <c r="V123" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="124" spans="22:22">
       <c r="V124" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="125" spans="22:22">
       <c r="V125" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="126" spans="22:22">
       <c r="V126" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="127" spans="22:22">
       <c r="V127" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="128" spans="22:22">
       <c r="V128" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="129" spans="22:22">
       <c r="V129" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="130" spans="22:22">
       <c r="V130" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="131" spans="22:22">
       <c r="V131" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="132" spans="22:22">
       <c r="V132" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="133" spans="22:22">
       <c r="V133" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="134" spans="22:22">
       <c r="V134" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="135" spans="22:22">
       <c r="V135" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="136" spans="22:22">
       <c r="V136" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="137" spans="22:22">
       <c r="V137" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="138" spans="22:22">
       <c r="V138" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="139" spans="22:22">
       <c r="V139" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="140" spans="22:22">
       <c r="V140" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="141" spans="22:22">
       <c r="V141" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="142" spans="22:22">
       <c r="V142" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="143" spans="22:22">
       <c r="V143" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="144" spans="22:22">
       <c r="V144" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="145" spans="22:22">
       <c r="V145" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="146" spans="22:22">
       <c r="V146" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="147" spans="22:22">
       <c r="V147" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="148" spans="22:22">
       <c r="V148" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="149" spans="22:22">
       <c r="V149" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="150" spans="22:22">
       <c r="V150" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="151" spans="22:22">
       <c r="V151" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="152" spans="22:22">
       <c r="V152" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="153" spans="22:22">
       <c r="V153" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="154" spans="22:22">
       <c r="V154" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="155" spans="22:22">
       <c r="V155" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="156" spans="22:22">
       <c r="V156" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="157" spans="22:22">
       <c r="V157" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="158" spans="22:22">
       <c r="V158" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="159" spans="22:22">
       <c r="V159" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="160" spans="22:22">
       <c r="V160" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="161" spans="22:22">
       <c r="V161" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="162" spans="22:22">
       <c r="V162" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="163" spans="22:22">
       <c r="V163" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="164" spans="22:22">
       <c r="V164" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="165" spans="22:22">
       <c r="V165" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="166" spans="22:22">
       <c r="V166" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="167" spans="22:22">
       <c r="V167" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="168" spans="22:22">
       <c r="V168" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="169" spans="22:22">
       <c r="V169" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="170" spans="22:22">
       <c r="V170" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="171" spans="22:22">
       <c r="V171" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="172" spans="22:22">
       <c r="V172" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="173" spans="22:22">
       <c r="V173" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="174" spans="22:22">
       <c r="V174" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="175" spans="22:22">
       <c r="V175" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="176" spans="22:22">
       <c r="V176" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="177" spans="22:22">
       <c r="V177" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="178" spans="22:22">
       <c r="V178" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="179" spans="22:22">
       <c r="V179" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="180" spans="22:22">
       <c r="V180" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="181" spans="22:22">
       <c r="V181" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="182" spans="22:22">
       <c r="V182" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="183" spans="22:22">
       <c r="V183" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="184" spans="22:22">
       <c r="V184" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="185" spans="22:22">
       <c r="V185" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="186" spans="22:22">
       <c r="V186" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="187" spans="22:22">
       <c r="V187" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="188" spans="22:22">
       <c r="V188" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="189" spans="22:22">
       <c r="V189" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="190" spans="22:22">
       <c r="V190" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="191" spans="22:22">
       <c r="V191" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="192" spans="22:22">
       <c r="V192" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="193" spans="22:22">
       <c r="V193" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="194" spans="22:22">
       <c r="V194" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="195" spans="22:22">
       <c r="V195" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="196" spans="22:22">
       <c r="V196" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="197" spans="22:22">
       <c r="V197" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="198" spans="22:22">
       <c r="V198" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="199" spans="22:22">
       <c r="V199" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="200" spans="22:22">
       <c r="V200" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="201" spans="22:22">
       <c r="V201" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="202" spans="22:22">
       <c r="V202" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="203" spans="22:22">
       <c r="V203" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="204" spans="22:22">
       <c r="V204" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="205" spans="22:22">
       <c r="V205" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="206" spans="22:22">
       <c r="V206" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="207" spans="22:22">
       <c r="V207" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="208" spans="22:22">
       <c r="V208" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="209" spans="22:22">
       <c r="V209" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="210" spans="22:22">
       <c r="V210" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="211" spans="22:22">
       <c r="V211" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="212" spans="22:22">
       <c r="V212" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="213" spans="22:22">
       <c r="V213" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="214" spans="22:22">
       <c r="V214" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="215" spans="22:22">
       <c r="V215" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="216" spans="22:22">
       <c r="V216" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="217" spans="22:22">
       <c r="V217" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="218" spans="22:22">
       <c r="V218" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="219" spans="22:22">
       <c r="V219" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="220" spans="22:22">
       <c r="V220" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="221" spans="22:22">
       <c r="V221" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="222" spans="22:22">
       <c r="V222" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="223" spans="22:22">
       <c r="V223" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="224" spans="22:22">
       <c r="V224" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="225" spans="22:22">
       <c r="V225" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="226" spans="22:22">
       <c r="V226" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="227" spans="22:22">
       <c r="V227" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="228" spans="22:22">
       <c r="V228" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="229" spans="22:22">
       <c r="V229" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="230" spans="22:22">
       <c r="V230" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="231" spans="22:22">
       <c r="V231" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="232" spans="22:22">
       <c r="V232" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="233" spans="22:22">
       <c r="V233" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="234" spans="22:22">
       <c r="V234" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="235" spans="22:22">
       <c r="V235" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="236" spans="22:22">
       <c r="V236" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="237" spans="22:22">
       <c r="V237" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="238" spans="22:22">
       <c r="V238" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="239" spans="22:22">
       <c r="V239" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="240" spans="22:22">
       <c r="V240" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="241" spans="22:22">
       <c r="V241" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="242" spans="22:22">
       <c r="V242" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="243" spans="22:22">
       <c r="V243" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="244" spans="22:22">
       <c r="V244" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="245" spans="22:22">
       <c r="V245" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="246" spans="22:22">
       <c r="V246" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="247" spans="22:22">
       <c r="V247" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="248" spans="22:22">
       <c r="V248" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="249" spans="22:22">
       <c r="V249" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="250" spans="22:22">
       <c r="V250" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="251" spans="22:22">
       <c r="V251" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="252" spans="22:22">
       <c r="V252" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="253" spans="22:22">
       <c r="V253" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="254" spans="22:22">
       <c r="V254" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="255" spans="22:22">
       <c r="V255" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="256" spans="22:22">
       <c r="V256" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="257" spans="22:22">
       <c r="V257" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="258" spans="22:22">
       <c r="V258" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="G3:G17">
-    <sortCondition ref="G17"/>
+  <sortState ref="F3:F7">
+    <sortCondition ref="F3"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>